<commit_message>
Completed items for database updated
</commit_message>
<xml_diff>
--- a/PayBack - CEN3031 Scrum.xlsx
+++ b/PayBack - CEN3031 Scrum.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HJeon\Documents\GitHub\PayBack\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="390" yWindow="615" windowWidth="16935" windowHeight="7620" activeTab="2"/>
   </bookViews>
@@ -17,7 +12,7 @@
     <sheet name="Sprint 1" sheetId="4" r:id="rId3"/>
     <sheet name="Sprint 1 Burndown" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -27,7 +22,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="V1" authorId="0" shapeId="0">
+    <comment ref="V1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -50,7 +45,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -73,7 +68,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="B2" authorId="0" shapeId="0">
+    <comment ref="B2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -89,7 +84,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C2" authorId="0" shapeId="0">
+    <comment ref="C2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -102,7 +97,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D2" authorId="0" shapeId="0">
+    <comment ref="D2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -115,7 +110,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E2" authorId="0" shapeId="0">
+    <comment ref="E2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -133,7 +128,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="213">
   <si>
     <t>User Stories</t>
   </si>
@@ -769,17 +764,27 @@
   </si>
   <si>
     <t>Total Hrs:</t>
+  </si>
+  <si>
+    <t>Figure out how to connect database to app.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="54" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="55">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1669,80 +1674,80 @@
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="13" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="21" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="22" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="16" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="16" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="33" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="20" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="20" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1751,224 +1756,230 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="25" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="25" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="45" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="46" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="50" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="50" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="51" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="40" borderId="0" xfId="4" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="40" borderId="0" xfId="4" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="38" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="38" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="37" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="37" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="40" borderId="0" xfId="4" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="38" borderId="0" xfId="2" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="37" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="40" borderId="0" xfId="4" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="40" borderId="0" xfId="4" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="38" borderId="0" xfId="2" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="37" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="40" borderId="0" xfId="4" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="38" borderId="0" xfId="2" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="38" borderId="0" xfId="2" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="38" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="38" borderId="0" xfId="2" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="38" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="38" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="41" borderId="0" xfId="5" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="41" borderId="0" xfId="5" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="41" borderId="0" xfId="5" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="41" borderId="0" xfId="5" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="41" borderId="0" xfId="5" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="41" borderId="0" xfId="5" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="41" borderId="0" xfId="5" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="41" borderId="0" xfId="5" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="37" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="37" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="37" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="37" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="37" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="37" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="37" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="37" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="37" borderId="19" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="37" borderId="19" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="37" borderId="25" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="37" borderId="25" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="37" borderId="12" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="37" borderId="12" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="37" borderId="10" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="37" borderId="10" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="41" borderId="0" xfId="5" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="41" borderId="0" xfId="5" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="41" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="41" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="41" borderId="19" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="41" borderId="19" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="41" borderId="25" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="41" borderId="25" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="41" borderId="12" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="41" borderId="12" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="41" borderId="10" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="41" borderId="10" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="38" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="38" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" xfId="5" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" xfId="5" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="38" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="38" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="38" borderId="12" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="38" borderId="12" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="38" borderId="10" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="38" borderId="10" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="39" borderId="0" xfId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="39" borderId="0" xfId="3" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="39" borderId="12" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="39" borderId="12" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="39" borderId="10" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="39" borderId="10" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="42" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="42" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="39" borderId="0" xfId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="39" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="37" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="38" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="37" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="38" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="39" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="39" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="41" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="41" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="41" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="41" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="41" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="32" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="36" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="24" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="21" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="27" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="19" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="15" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="17" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="42" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="37" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="32" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="36" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="24" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="21" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="27" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="19" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="15" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="17" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1999,17 +2010,8 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -2027,10 +2029,7 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:areaChart>
@@ -2120,16 +2119,16 @@
                   <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>49</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>49</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>49</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>49</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2234,19 +2233,12 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="188679192"/>
-        <c:axId val="188678016"/>
+        <c:dLbls/>
+        <c:axId val="237650304"/>
+        <c:axId val="237652224"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="188679192"/>
+        <c:axId val="237650304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2268,14 +2260,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="cross"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="188678016"/>
+        <c:crossAx val="237652224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2283,11 +2273,10 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="188678016"/>
+        <c:axId val="237652224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -2306,8 +2295,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="cross"/>
@@ -2328,15 +2315,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="188679192"/>
+        <c:crossAx val="237650304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="zero"/>
@@ -2344,7 +2329,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2567,7 +2552,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2599,10 +2584,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2634,7 +2618,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2810,7 +2793,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:V54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2818,7 +2801,7 @@
       <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="11.7109375" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
@@ -2827,7 +2810,7 @@
     <col min="5" max="5" width="60.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" ht="26.25" customHeight="1">
       <c r="A1" s="84" t="s">
         <v>0</v>
       </c>
@@ -2836,7 +2819,7 @@
       <c r="D1" s="84"/>
       <c r="E1" s="84"/>
     </row>
-    <row r="2" spans="1:22" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" ht="22.5" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -2854,7 +2837,7 @@
       </c>
       <c r="F2" s="43"/>
     </row>
-    <row r="3" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" ht="18.75" customHeight="1">
       <c r="A3" s="38" t="s">
         <v>34</v>
       </c>
@@ -2872,7 +2855,7 @@
       </c>
       <c r="F3" s="43"/>
     </row>
-    <row r="4" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" ht="18.75" customHeight="1">
       <c r="A4" s="35" t="s">
         <v>34</v>
       </c>
@@ -2890,7 +2873,7 @@
       </c>
       <c r="F4" s="43"/>
     </row>
-    <row r="5" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" ht="18.75" customHeight="1">
       <c r="A5" s="35" t="s">
         <v>34</v>
       </c>
@@ -2908,7 +2891,7 @@
       </c>
       <c r="F5" s="43"/>
     </row>
-    <row r="6" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" ht="18.75" customHeight="1">
       <c r="A6" s="38" t="s">
         <v>34</v>
       </c>
@@ -2926,7 +2909,7 @@
       </c>
       <c r="F6" s="79"/>
     </row>
-    <row r="7" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" ht="18.75" customHeight="1">
       <c r="A7" s="38" t="s">
         <v>34</v>
       </c>
@@ -2944,7 +2927,7 @@
       </c>
       <c r="F7" s="43"/>
     </row>
-    <row r="8" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" ht="18.75" customHeight="1">
       <c r="A8" s="38" t="s">
         <v>34</v>
       </c>
@@ -2962,7 +2945,7 @@
       </c>
       <c r="F8" s="43"/>
     </row>
-    <row r="9" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" ht="18.75" customHeight="1">
       <c r="A9" s="38" t="s">
         <v>34</v>
       </c>
@@ -2980,7 +2963,7 @@
       </c>
       <c r="F9" s="43"/>
     </row>
-    <row r="10" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" ht="18.75" customHeight="1">
       <c r="A10" s="38" t="s">
         <v>34</v>
       </c>
@@ -2998,7 +2981,7 @@
       </c>
       <c r="F10" s="43"/>
     </row>
-    <row r="11" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" ht="18.75" customHeight="1">
       <c r="A11" s="38" t="s">
         <v>34</v>
       </c>
@@ -3016,7 +2999,7 @@
       </c>
       <c r="F11" s="43"/>
     </row>
-    <row r="12" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" ht="18.75" customHeight="1">
       <c r="A12" s="35" t="s">
         <v>34</v>
       </c>
@@ -3034,7 +3017,7 @@
       </c>
       <c r="F12" s="43"/>
     </row>
-    <row r="13" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" ht="18.75" customHeight="1">
       <c r="A13" s="39" t="s">
         <v>53</v>
       </c>
@@ -3052,7 +3035,7 @@
       </c>
       <c r="F13" s="43"/>
     </row>
-    <row r="14" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" ht="18.75" customHeight="1">
       <c r="A14" s="39" t="s">
         <v>53</v>
       </c>
@@ -3070,7 +3053,7 @@
       </c>
       <c r="F14" s="43"/>
     </row>
-    <row r="15" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" ht="18.75" customHeight="1">
       <c r="A15" s="36" t="s">
         <v>53</v>
       </c>
@@ -3088,7 +3071,7 @@
       </c>
       <c r="F15" s="43"/>
     </row>
-    <row r="16" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" ht="18.75" customHeight="1">
       <c r="A16" s="36" t="s">
         <v>53</v>
       </c>
@@ -3106,7 +3089,7 @@
       </c>
       <c r="F16" s="43"/>
     </row>
-    <row r="17" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="18.75" customHeight="1">
       <c r="A17" s="39" t="s">
         <v>53</v>
       </c>
@@ -3124,7 +3107,7 @@
       </c>
       <c r="F17" s="43"/>
     </row>
-    <row r="18" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="18.75" customHeight="1">
       <c r="A18" s="39" t="s">
         <v>53</v>
       </c>
@@ -3142,7 +3125,7 @@
       </c>
       <c r="F18" s="43"/>
     </row>
-    <row r="19" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="18.75" customHeight="1">
       <c r="A19" s="39" t="s">
         <v>53</v>
       </c>
@@ -3160,7 +3143,7 @@
       </c>
       <c r="F19" s="43"/>
     </row>
-    <row r="20" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="18.75" customHeight="1">
       <c r="A20" s="39" t="s">
         <v>53</v>
       </c>
@@ -3178,7 +3161,7 @@
       </c>
       <c r="F20" s="43"/>
     </row>
-    <row r="21" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="18.75" customHeight="1">
       <c r="A21" s="39" t="s">
         <v>53</v>
       </c>
@@ -3196,7 +3179,7 @@
       </c>
       <c r="F21" s="43"/>
     </row>
-    <row r="22" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="18.75" customHeight="1">
       <c r="A22" s="39" t="s">
         <v>53</v>
       </c>
@@ -3214,7 +3197,7 @@
       </c>
       <c r="F22" s="43"/>
     </row>
-    <row r="23" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="18.75" customHeight="1">
       <c r="A23" s="39" t="s">
         <v>53</v>
       </c>
@@ -3232,7 +3215,7 @@
       </c>
       <c r="F23" s="43"/>
     </row>
-    <row r="24" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="18.75" customHeight="1">
       <c r="A24" s="39" t="s">
         <v>53</v>
       </c>
@@ -3250,7 +3233,7 @@
       </c>
       <c r="F24" s="43"/>
     </row>
-    <row r="25" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="18.75" customHeight="1">
       <c r="A25" s="39" t="s">
         <v>53</v>
       </c>
@@ -3268,7 +3251,7 @@
       </c>
       <c r="F25" s="43"/>
     </row>
-    <row r="26" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="18.75" customHeight="1">
       <c r="A26" s="39" t="s">
         <v>53</v>
       </c>
@@ -3286,7 +3269,7 @@
       </c>
       <c r="F26" s="43"/>
     </row>
-    <row r="27" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="18.75" customHeight="1">
       <c r="A27" s="39" t="s">
         <v>53</v>
       </c>
@@ -3304,7 +3287,7 @@
       </c>
       <c r="F27" s="43"/>
     </row>
-    <row r="28" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="18.75" customHeight="1">
       <c r="A28" s="39" t="s">
         <v>53</v>
       </c>
@@ -3322,7 +3305,7 @@
       </c>
       <c r="F28" s="43"/>
     </row>
-    <row r="29" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="18.75" customHeight="1">
       <c r="A29" s="36" t="s">
         <v>53</v>
       </c>
@@ -3340,7 +3323,7 @@
       </c>
       <c r="F29" s="43"/>
     </row>
-    <row r="30" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="18.75" customHeight="1">
       <c r="A30" s="39" t="s">
         <v>53</v>
       </c>
@@ -3358,7 +3341,7 @@
       </c>
       <c r="F30" s="43"/>
     </row>
-    <row r="31" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="18.75" customHeight="1">
       <c r="A31" s="39" t="s">
         <v>53</v>
       </c>
@@ -3376,7 +3359,7 @@
       </c>
       <c r="F31" s="43"/>
     </row>
-    <row r="32" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="18.75" customHeight="1">
       <c r="A32" s="39" t="s">
         <v>53</v>
       </c>
@@ -3394,7 +3377,7 @@
       </c>
       <c r="F32" s="43"/>
     </row>
-    <row r="33" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="18.75" customHeight="1">
       <c r="A33" s="36" t="s">
         <v>53</v>
       </c>
@@ -3412,7 +3395,7 @@
       </c>
       <c r="F33" s="43"/>
     </row>
-    <row r="34" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="18.75" customHeight="1">
       <c r="A34" s="40" t="s">
         <v>96</v>
       </c>
@@ -3429,7 +3412,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="18.75" customHeight="1">
       <c r="A35" s="40" t="s">
         <v>96</v>
       </c>
@@ -3446,7 +3429,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="18.75" customHeight="1">
       <c r="A36" s="40" t="s">
         <v>96</v>
       </c>
@@ -3463,7 +3446,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="18.75" customHeight="1">
       <c r="A37" s="37" t="s">
         <v>96</v>
       </c>
@@ -3480,7 +3463,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="18.75" customHeight="1">
       <c r="A38" s="40" t="s">
         <v>96</v>
       </c>
@@ -3497,7 +3480,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="18.75" customHeight="1">
       <c r="A39" s="40" t="s">
         <v>96</v>
       </c>
@@ -3514,7 +3497,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="18.75" customHeight="1">
       <c r="A40" s="40" t="s">
         <v>96</v>
       </c>
@@ -3531,7 +3514,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" ht="18.75" customHeight="1">
       <c r="A41" s="40" t="s">
         <v>96</v>
       </c>
@@ -3548,7 +3531,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="18.75" customHeight="1">
       <c r="A42" s="40" t="s">
         <v>96</v>
       </c>
@@ -3565,7 +3548,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" ht="18.75" customHeight="1">
       <c r="A43" s="40" t="s">
         <v>96</v>
       </c>
@@ -3582,7 +3565,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" ht="18.75" customHeight="1">
       <c r="A44" s="37" t="s">
         <v>96</v>
       </c>
@@ -3599,7 +3582,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" ht="18.75" customHeight="1">
       <c r="A45" s="37" t="s">
         <v>96</v>
       </c>
@@ -3616,7 +3599,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" ht="18.75" customHeight="1">
       <c r="A46" s="40" t="s">
         <v>96</v>
       </c>
@@ -3633,7 +3616,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" ht="18.75" customHeight="1">
       <c r="A47" s="40" t="s">
         <v>96</v>
       </c>
@@ -3650,7 +3633,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" ht="18.75" customHeight="1">
       <c r="A48" s="40" t="s">
         <v>96</v>
       </c>
@@ -3667,7 +3650,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" ht="18.75" customHeight="1">
       <c r="A49" s="40" t="s">
         <v>96</v>
       </c>
@@ -3684,7 +3667,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" ht="18.75" customHeight="1">
       <c r="A50" s="40" t="s">
         <v>96</v>
       </c>
@@ -3701,7 +3684,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" ht="18.75" customHeight="1">
       <c r="A51" s="40" t="s">
         <v>96</v>
       </c>
@@ -3718,7 +3701,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" ht="18.75" customHeight="1">
       <c r="A52" s="40" t="s">
         <v>96</v>
       </c>
@@ -3735,7 +3718,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" ht="18.75" customHeight="1">
       <c r="A53" s="40" t="s">
         <v>96</v>
       </c>
@@ -3752,7 +3735,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" ht="18.75" customHeight="1">
       <c r="A54" s="40" t="s">
         <v>96</v>
       </c>
@@ -3780,7 +3763,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3788,14 +3771,14 @@
       <selection pane="bottomLeft" activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16.7109375" customWidth="1"/>
     <col min="2" max="2" width="78.140625" customWidth="1"/>
     <col min="3" max="3" width="6.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="24" customHeight="1">
       <c r="A1" s="86" t="s">
         <v>11</v>
       </c>
@@ -3803,7 +3786,7 @@
       <c r="C1" s="16"/>
       <c r="D1" s="16"/>
     </row>
-    <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="18.75" customHeight="1">
       <c r="A2" s="29" t="s">
         <v>1</v>
       </c>
@@ -3817,7 +3800,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="18.75" customHeight="1">
       <c r="A3" s="46" t="s">
         <v>34</v>
       </c>
@@ -3831,7 +3814,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="18.75" customHeight="1">
       <c r="A4" s="46" t="s">
         <v>34</v>
       </c>
@@ -3845,7 +3828,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="18.75" customHeight="1">
       <c r="A5" s="46" t="s">
         <v>34</v>
       </c>
@@ -3859,7 +3842,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="18.75" customHeight="1">
       <c r="A6" s="46" t="s">
         <v>34</v>
       </c>
@@ -3873,7 +3856,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="18.75" customHeight="1">
       <c r="A7" s="46" t="s">
         <v>34</v>
       </c>
@@ -3887,7 +3870,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="18.75" customHeight="1">
       <c r="A8" s="46" t="s">
         <v>34</v>
       </c>
@@ -3901,7 +3884,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="18.75" customHeight="1">
       <c r="A9" s="46" t="s">
         <v>34</v>
       </c>
@@ -3915,7 +3898,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="18.75" customHeight="1">
       <c r="A10" s="46" t="s">
         <v>34</v>
       </c>
@@ -3929,7 +3912,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="18.75" customHeight="1">
       <c r="A11" s="46" t="s">
         <v>34</v>
       </c>
@@ -3943,7 +3926,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="18.75" customHeight="1">
       <c r="A12" s="46" t="s">
         <v>34</v>
       </c>
@@ -3957,7 +3940,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="18.75" customHeight="1">
       <c r="A13" s="46" t="s">
         <v>34</v>
       </c>
@@ -3971,7 +3954,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="18.75" customHeight="1">
       <c r="A14" s="46" t="s">
         <v>34</v>
       </c>
@@ -3985,7 +3968,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="18.75" customHeight="1">
       <c r="A15" s="46" t="s">
         <v>34</v>
       </c>
@@ -3999,7 +3982,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="18.75" customHeight="1">
       <c r="A16" s="46" t="s">
         <v>34</v>
       </c>
@@ -4013,7 +3996,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="18.75" customHeight="1">
       <c r="A17" s="49" t="s">
         <v>34</v>
       </c>
@@ -4027,7 +4010,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="18.75" customHeight="1">
       <c r="A18" s="49" t="s">
         <v>34</v>
       </c>
@@ -4041,7 +4024,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="18.75" customHeight="1">
       <c r="A19" s="49" t="s">
         <v>34</v>
       </c>
@@ -4055,7 +4038,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="18.75" customHeight="1">
       <c r="A20" s="49" t="s">
         <v>34</v>
       </c>
@@ -4069,7 +4052,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="18.75" customHeight="1">
       <c r="A21" s="49" t="s">
         <v>34</v>
       </c>
@@ -4083,7 +4066,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="18.75" customHeight="1">
       <c r="A22" s="49" t="s">
         <v>34</v>
       </c>
@@ -4097,7 +4080,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="18.75" customHeight="1">
       <c r="A23" s="49" t="s">
         <v>34</v>
       </c>
@@ -4111,7 +4094,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="18.75" customHeight="1">
       <c r="A24" s="49" t="s">
         <v>34</v>
       </c>
@@ -4125,7 +4108,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="18.75" customHeight="1">
       <c r="A25" s="49" t="s">
         <v>34</v>
       </c>
@@ -4139,7 +4122,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="18.75" customHeight="1">
       <c r="A26" s="46" t="s">
         <v>34</v>
       </c>
@@ -4153,7 +4136,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="18.75" customHeight="1">
       <c r="A27" s="46" t="s">
         <v>34</v>
       </c>
@@ -4167,7 +4150,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="18.75" customHeight="1">
       <c r="A28" s="44" t="s">
         <v>53</v>
       </c>
@@ -4181,7 +4164,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="18.75" customHeight="1">
       <c r="A29" s="44" t="s">
         <v>53</v>
       </c>
@@ -4195,7 +4178,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="18.75" customHeight="1">
       <c r="A30" s="44" t="s">
         <v>53</v>
       </c>
@@ -4209,7 +4192,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="18.75" customHeight="1">
       <c r="A31" s="44" t="s">
         <v>53</v>
       </c>
@@ -4223,7 +4206,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="18.75" customHeight="1">
       <c r="A32" s="44" t="s">
         <v>53</v>
       </c>
@@ -4237,7 +4220,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="18.75" customHeight="1">
       <c r="A33" s="44" t="s">
         <v>53</v>
       </c>
@@ -4251,7 +4234,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="18.75" customHeight="1">
       <c r="A34" s="44" t="s">
         <v>53</v>
       </c>
@@ -4265,7 +4248,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="18.75" customHeight="1">
       <c r="A35" s="44" t="s">
         <v>53</v>
       </c>
@@ -4279,7 +4262,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="18.75" customHeight="1">
       <c r="A36" s="44" t="s">
         <v>53</v>
       </c>
@@ -4293,7 +4276,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="18.75" customHeight="1">
       <c r="A37" s="44" t="s">
         <v>53</v>
       </c>
@@ -4307,7 +4290,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="18.75" customHeight="1">
       <c r="A38" s="44" t="s">
         <v>53</v>
       </c>
@@ -4321,7 +4304,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="18.75" customHeight="1">
       <c r="A39" s="44" t="s">
         <v>53</v>
       </c>
@@ -4335,7 +4318,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="18.75" customHeight="1">
       <c r="A40" s="44" t="s">
         <v>53</v>
       </c>
@@ -4349,7 +4332,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="18.75" customHeight="1">
       <c r="A41" s="44" t="s">
         <v>53</v>
       </c>
@@ -4363,7 +4346,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="18.75" customHeight="1">
       <c r="A42" s="44" t="s">
         <v>53</v>
       </c>
@@ -4377,7 +4360,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" ht="18.75" customHeight="1">
       <c r="A43" s="44" t="s">
         <v>53</v>
       </c>
@@ -4391,7 +4374,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" ht="18.75" customHeight="1">
       <c r="A44" s="44" t="s">
         <v>53</v>
       </c>
@@ -4405,7 +4388,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="18.75" customHeight="1">
       <c r="A45" s="44" t="s">
         <v>53</v>
       </c>
@@ -4419,7 +4402,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" ht="18.75" customHeight="1">
       <c r="A46" s="44" t="s">
         <v>53</v>
       </c>
@@ -4433,7 +4416,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" ht="18.75" customHeight="1">
       <c r="A47" s="44" t="s">
         <v>53</v>
       </c>
@@ -4447,7 +4430,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" ht="18.75" customHeight="1">
       <c r="A48" s="50" t="s">
         <v>96</v>
       </c>
@@ -4461,7 +4444,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" ht="18.75" customHeight="1">
       <c r="A49" s="50" t="s">
         <v>96</v>
       </c>
@@ -4475,7 +4458,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" ht="18.75" customHeight="1">
       <c r="A50" s="50" t="s">
         <v>96</v>
       </c>
@@ -4489,7 +4472,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" ht="18.75" customHeight="1">
       <c r="A51" s="50" t="s">
         <v>96</v>
       </c>
@@ -4503,7 +4486,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" ht="18.75" customHeight="1">
       <c r="A52" s="50" t="s">
         <v>96</v>
       </c>
@@ -4517,7 +4500,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" ht="18.75" customHeight="1">
       <c r="A53" s="50" t="s">
         <v>96</v>
       </c>
@@ -4531,7 +4514,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" ht="18.75" customHeight="1">
       <c r="A54" s="50" t="s">
         <v>96</v>
       </c>
@@ -4545,7 +4528,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" ht="18.75" customHeight="1">
       <c r="A55" s="50" t="s">
         <v>96</v>
       </c>
@@ -4559,7 +4542,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" ht="18.75" customHeight="1">
       <c r="A56" s="50" t="s">
         <v>96</v>
       </c>
@@ -4573,7 +4556,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" ht="18.75" customHeight="1">
       <c r="A57" s="50" t="s">
         <v>96</v>
       </c>
@@ -4587,7 +4570,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" ht="18.75" customHeight="1">
       <c r="A58" s="50" t="s">
         <v>96</v>
       </c>
@@ -4601,7 +4584,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" ht="18.75" customHeight="1">
       <c r="A59" s="50" t="s">
         <v>96</v>
       </c>
@@ -4615,7 +4598,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" ht="18.75" customHeight="1">
       <c r="A60" s="50" t="s">
         <v>96</v>
       </c>
@@ -4629,7 +4612,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" ht="18.75" customHeight="1">
       <c r="A61" s="50" t="s">
         <v>96</v>
       </c>
@@ -4643,7 +4626,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" ht="18.75" customHeight="1">
       <c r="A62" s="50" t="s">
         <v>96</v>
       </c>
@@ -4657,7 +4640,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" ht="18.75" customHeight="1">
       <c r="A63" s="50" t="s">
         <v>96</v>
       </c>
@@ -4671,7 +4654,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" ht="18.75" customHeight="1">
       <c r="A64" s="50" t="s">
         <v>96</v>
       </c>
@@ -4685,7 +4668,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="3:3" ht="12.75" customHeight="1">
       <c r="C65">
         <f>SUM(C3:C64)</f>
         <v>248</v>
@@ -4699,8 +4682,8 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+  <extLst xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
+    <ext uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="81" yWindow="476" count="1">
         <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="validationFailedClick and enter a value from range 'User Stories'!A3:A15">
           <x14:formula1>
@@ -4715,15 +4698,15 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O17" sqref="O17"/>
+      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="80.85546875" customWidth="1"/>
     <col min="2" max="2" width="4.140625" customWidth="1"/>
@@ -4736,7 +4719,7 @@
     <col min="9" max="16" width="3.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" ht="29.25" customHeight="1">
       <c r="A1" s="32" t="s">
         <v>15</v>
       </c>
@@ -4764,7 +4747,7 @@
       <c r="O1" s="91"/>
       <c r="P1" s="92"/>
     </row>
-    <row r="2" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" ht="25.5">
       <c r="A2" s="32" t="s">
         <v>20</v>
       </c>
@@ -4814,7 +4797,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="24" customHeight="1">
       <c r="A3" s="81" t="s">
         <v>201</v>
       </c>
@@ -4860,7 +4843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" ht="24" customHeight="1">
       <c r="A4" s="46" t="s">
         <v>133</v>
       </c>
@@ -4906,7 +4889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" ht="24" customHeight="1">
       <c r="A5" s="46" t="s">
         <v>134</v>
       </c>
@@ -4952,7 +4935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="24" customHeight="1">
       <c r="A6" s="46" t="s">
         <v>141</v>
       </c>
@@ -4998,7 +4981,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="24" customHeight="1">
       <c r="A7" s="46" t="s">
         <v>135</v>
       </c>
@@ -5044,7 +5027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" ht="24" customHeight="1">
       <c r="A8" s="46" t="s">
         <v>137</v>
       </c>
@@ -5090,7 +5073,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" ht="24" customHeight="1">
       <c r="A9" s="46" t="s">
         <v>139</v>
       </c>
@@ -5136,7 +5119,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" ht="24" customHeight="1">
       <c r="A10" s="46" t="s">
         <v>138</v>
       </c>
@@ -5182,7 +5165,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" ht="24" customHeight="1">
       <c r="A11" s="47" t="s">
         <v>140</v>
       </c>
@@ -5228,7 +5211,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" ht="24" customHeight="1">
       <c r="A12" s="47" t="s">
         <v>136</v>
       </c>
@@ -5274,7 +5257,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" ht="24" customHeight="1">
       <c r="A13" s="44" t="s">
         <v>150</v>
       </c>
@@ -5320,9 +5303,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="50" t="s">
-        <v>172</v>
+    <row r="14" spans="1:16" ht="24" customHeight="1">
+      <c r="A14" s="102" t="s">
+        <v>212</v>
       </c>
       <c r="B14" s="50">
         <v>4</v>
@@ -5333,8 +5316,8 @@
       <c r="D14" s="50" t="s">
         <v>193</v>
       </c>
-      <c r="E14" s="67" t="s">
-        <v>28</v>
+      <c r="E14" s="75" t="s">
+        <v>194</v>
       </c>
       <c r="F14" s="50"/>
       <c r="G14" s="56"/>
@@ -5366,7 +5349,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" ht="24" customHeight="1">
       <c r="A15" s="50" t="s">
         <v>173</v>
       </c>
@@ -5379,8 +5362,8 @@
       <c r="D15" s="50" t="s">
         <v>191</v>
       </c>
-      <c r="E15" s="67" t="s">
-        <v>28</v>
+      <c r="E15" s="75" t="s">
+        <v>194</v>
       </c>
       <c r="F15" s="50"/>
       <c r="G15" s="56"/>
@@ -5400,19 +5383,19 @@
         <v>2</v>
       </c>
       <c r="M15" s="56">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N15" s="57">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O15" s="53">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P15" s="53">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="24" customHeight="1">
       <c r="A16" s="50" t="s">
         <v>174</v>
       </c>
@@ -5425,8 +5408,8 @@
       <c r="D16" s="50" t="s">
         <v>191</v>
       </c>
-      <c r="E16" s="67" t="s">
-        <v>28</v>
+      <c r="E16" s="101" t="s">
+        <v>194</v>
       </c>
       <c r="F16" s="50"/>
       <c r="G16" s="56"/>
@@ -5458,7 +5441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" ht="24" customHeight="1">
       <c r="A17" s="50" t="s">
         <v>176</v>
       </c>
@@ -5504,7 +5487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" ht="24" customHeight="1">
       <c r="A18" s="50" t="s">
         <v>180</v>
       </c>
@@ -5550,7 +5533,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" ht="24" customHeight="1">
       <c r="A19" s="50" t="s">
         <v>181</v>
       </c>
@@ -5596,7 +5579,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" ht="24" customHeight="1">
       <c r="A20" s="80" t="s">
         <v>197</v>
       </c>
@@ -5642,7 +5625,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" ht="24" customHeight="1">
       <c r="A21" s="80" t="s">
         <v>199</v>
       </c>
@@ -5688,7 +5671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" ht="24" customHeight="1">
       <c r="A22" s="80" t="s">
         <v>200</v>
       </c>
@@ -5734,7 +5717,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" ht="24" customHeight="1">
       <c r="A23" s="71" t="s">
         <v>195</v>
       </c>
@@ -5780,8 +5763,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" ht="24" customHeight="1"/>
+    <row r="25" spans="1:16" ht="24" customHeight="1">
       <c r="F25" s="43" t="s">
         <v>211</v>
       </c>
@@ -5790,13 +5773,13 @@
         <v>80</v>
       </c>
     </row>
-    <row r="26" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" ht="24" customHeight="1"/>
+    <row r="27" spans="1:16" ht="24" customHeight="1"/>
+    <row r="28" spans="1:16" ht="24" customHeight="1"/>
+    <row r="29" spans="1:16" ht="24" customHeight="1"/>
+    <row r="30" spans="1:16" ht="24" customHeight="1"/>
+    <row r="31" spans="1:16" ht="24" customHeight="1"/>
+    <row r="32" spans="1:16" ht="24" customHeight="1">
       <c r="E32" s="24"/>
       <c r="L32" s="23"/>
       <c r="M32" s="5"/>
@@ -5804,7 +5787,7 @@
       <c r="O32" s="22"/>
       <c r="P32" s="22"/>
     </row>
-    <row r="33" spans="5:16" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="5:16" ht="24" customHeight="1">
       <c r="E33" s="24"/>
       <c r="L33" s="23"/>
       <c r="M33" s="5"/>
@@ -5812,7 +5795,7 @@
       <c r="O33" s="22"/>
       <c r="P33" s="22"/>
     </row>
-    <row r="34" spans="5:16" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="5:16" ht="24" customHeight="1">
       <c r="E34" s="24"/>
       <c r="L34" s="23"/>
       <c r="M34" s="5"/>
@@ -5820,7 +5803,7 @@
       <c r="O34" s="22"/>
       <c r="P34" s="22"/>
     </row>
-    <row r="35" spans="5:16" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="5:16" ht="24" customHeight="1">
       <c r="E35" s="24"/>
       <c r="L35" s="23"/>
       <c r="M35" s="5"/>
@@ -5828,7 +5811,7 @@
       <c r="O35" s="22"/>
       <c r="P35" s="22"/>
     </row>
-    <row r="36" spans="5:16" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="5:16" ht="24" customHeight="1">
       <c r="E36" s="24"/>
       <c r="L36" s="23"/>
       <c r="M36" s="5"/>
@@ -5858,7 +5841,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5866,12 +5849,12 @@
       <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1"/>
   <cols>
     <col min="2" max="10" width="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="25.5" customHeight="1">
       <c r="A1" s="93" t="s">
         <v>29</v>
       </c>
@@ -5885,7 +5868,7 @@
       <c r="I1" s="94"/>
       <c r="J1" s="94"/>
     </row>
-    <row r="2" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="14.25">
       <c r="A2" s="10"/>
       <c r="B2" s="95"/>
       <c r="C2" s="96"/>
@@ -5897,7 +5880,7 @@
       <c r="I2" s="99"/>
       <c r="J2" s="100"/>
     </row>
-    <row r="3" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="14.25">
       <c r="A3" s="1" t="s">
         <v>30</v>
       </c>
@@ -5929,7 +5912,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="27" customHeight="1">
       <c r="A4" s="31"/>
       <c r="B4" s="26">
         <v>1</v>
@@ -5967,7 +5950,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="26.25" customHeight="1">
       <c r="A5" s="25" t="s">
         <v>31</v>
       </c>
@@ -5993,22 +5976,22 @@
       </c>
       <c r="G5" s="34">
         <f>SUM('Sprint 1'!M3:M31)</f>
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H5" s="12">
         <f>SUM('Sprint 1'!N3:N31)</f>
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="I5" s="17">
         <f>SUM('Sprint 1'!O3:O31)</f>
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="J5" s="34">
         <f>SUM('Sprint 1'!P3:P31)</f>
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="26.25" customHeight="1">
       <c r="A6" s="25" t="s">
         <v>32</v>
       </c>
@@ -6049,7 +6032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="24" customHeight="1">
       <c r="B7" s="17" t="s">
         <v>33</v>
       </c>
@@ -6059,7 +6042,7 @@
       <c r="F7" s="17"/>
       <c r="G7" s="17"/>
     </row>
-    <row r="8" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="26.25" customHeight="1">
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
       <c r="D8" s="17"/>
@@ -6067,7 +6050,7 @@
       <c r="F8" s="17"/>
       <c r="G8" s="17"/>
     </row>
-    <row r="9" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="26.25" customHeight="1">
       <c r="B9" s="17"/>
       <c r="C9" s="17"/>
       <c r="D9" s="17"/>
@@ -6075,7 +6058,7 @@
       <c r="F9" s="17"/>
       <c r="G9" s="17"/>
     </row>
-    <row r="10" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="26.25" customHeight="1">
       <c r="B10" s="17"/>
       <c r="C10" s="17"/>
       <c r="D10" s="17"/>
@@ -6083,7 +6066,7 @@
       <c r="F10" s="17"/>
       <c r="G10" s="17"/>
     </row>
-    <row r="11" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="26.25" customHeight="1">
       <c r="B11" s="17"/>
       <c r="C11" s="17"/>
       <c r="D11" s="17"/>
@@ -6091,7 +6074,7 @@
       <c r="F11" s="17"/>
       <c r="G11" s="17"/>
     </row>
-    <row r="12" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="26.25" customHeight="1">
       <c r="B12" s="17"/>
       <c r="C12" s="17"/>
       <c r="D12" s="17"/>
@@ -6099,7 +6082,7 @@
       <c r="F12" s="17"/>
       <c r="G12" s="17"/>
     </row>
-    <row r="13" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="26.25" customHeight="1">
       <c r="B13" s="17"/>
       <c r="C13" s="17"/>
       <c r="D13" s="17"/>
@@ -6107,7 +6090,7 @@
       <c r="F13" s="17"/>
       <c r="G13" s="17"/>
     </row>
-    <row r="14" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="26.25" customHeight="1">
       <c r="B14" s="17"/>
       <c r="C14" s="17"/>
       <c r="D14" s="17"/>
@@ -6115,7 +6098,7 @@
       <c r="F14" s="17"/>
       <c r="G14" s="17"/>
     </row>
-    <row r="15" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="26.25" customHeight="1">
       <c r="B15" s="17"/>
       <c r="C15" s="17"/>
       <c r="D15" s="17"/>
@@ -6123,7 +6106,7 @@
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
     </row>
-    <row r="16" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="26.25" customHeight="1">
       <c r="B16" s="17"/>
       <c r="C16" s="17"/>
       <c r="D16" s="17"/>
@@ -6131,7 +6114,7 @@
       <c r="F16" s="17"/>
       <c r="G16" s="17"/>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:7">
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
       <c r="D17" s="17"/>
@@ -6139,7 +6122,7 @@
       <c r="F17" s="17"/>
       <c r="G17" s="17"/>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:7">
       <c r="B18" s="17"/>
       <c r="C18" s="17"/>
       <c r="D18" s="17"/>
@@ -6147,7 +6130,7 @@
       <c r="F18" s="17"/>
       <c r="G18" s="17"/>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:7">
       <c r="B19" s="17"/>
       <c r="C19" s="17"/>
       <c r="D19" s="17"/>
@@ -6155,7 +6138,7 @@
       <c r="F19" s="17"/>
       <c r="G19" s="17"/>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:7">
       <c r="B20" s="17"/>
       <c r="C20" s="17"/>
       <c r="D20" s="17"/>
@@ -6163,7 +6146,7 @@
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:7">
       <c r="B21" s="17"/>
       <c r="C21" s="17"/>
       <c r="D21" s="17"/>
@@ -6171,7 +6154,7 @@
       <c r="F21" s="17"/>
       <c r="G21" s="17"/>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:7">
       <c r="B22" s="17"/>
       <c r="C22" s="17"/>
       <c r="D22" s="17"/>
@@ -6179,7 +6162,7 @@
       <c r="F22" s="17"/>
       <c r="G22" s="17"/>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:7">
       <c r="B23" s="17"/>
       <c r="C23" s="17"/>
       <c r="D23" s="17"/>
@@ -6187,7 +6170,7 @@
       <c r="F23" s="17"/>
       <c r="G23" s="17"/>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:7">
       <c r="B24" s="17"/>
       <c r="C24" s="17"/>
       <c r="D24" s="17"/>
@@ -6195,7 +6178,7 @@
       <c r="F24" s="17"/>
       <c r="G24" s="17"/>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:7">
       <c r="B25" s="17"/>
       <c r="C25" s="17"/>
       <c r="D25" s="17"/>

</xml_diff>

<commit_message>
Ryan Updated Scrum 1
</commit_message>
<xml_diff>
--- a/PayBack - CEN3031 Scrum.xlsx
+++ b/PayBack - CEN3031 Scrum.xlsx
@@ -1924,6 +1924,12 @@
     <xf numFmtId="0" fontId="2" fillId="41" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="42" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="37" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1974,12 +1980,6 @@
     </xf>
     <xf numFmtId="0" fontId="28" fillId="17" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="42" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="37" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -2233,12 +2233,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="237650304"/>
-        <c:axId val="237652224"/>
+        <c:axId val="228204928"/>
+        <c:axId val="228206848"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="237650304"/>
+        <c:axId val="228204928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2265,7 +2264,7 @@
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="cross"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="237652224"/>
+        <c:crossAx val="228206848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2273,7 +2272,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="237652224"/>
+        <c:axId val="228206848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2315,7 +2314,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="237650304"/>
+        <c:crossAx val="228204928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2329,7 +2328,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2811,13 +2810,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="26.25" customHeight="1">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="86" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="85"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
+      <c r="B1" s="87"/>
+      <c r="C1" s="86"/>
+      <c r="D1" s="86"/>
+      <c r="E1" s="86"/>
     </row>
     <row r="2" spans="1:22" ht="22.5" customHeight="1">
       <c r="A2" s="3" t="s">
@@ -3779,10 +3778,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="24" customHeight="1">
-      <c r="A1" s="86" t="s">
+      <c r="A1" s="88" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="86"/>
+      <c r="B1" s="88"/>
       <c r="C1" s="16"/>
       <c r="D1" s="16"/>
     </row>
@@ -4702,8 +4701,8 @@
   <dimension ref="A1:P36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
+      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1"/>
@@ -4731,21 +4730,21 @@
       <c r="G1" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="87" t="s">
+      <c r="H1" s="89" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="88"/>
-      <c r="J1" s="89"/>
-      <c r="K1" s="90" t="s">
+      <c r="I1" s="90"/>
+      <c r="J1" s="91"/>
+      <c r="K1" s="92" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="91"/>
-      <c r="M1" s="92"/>
-      <c r="N1" s="90" t="s">
+      <c r="L1" s="93"/>
+      <c r="M1" s="94"/>
+      <c r="N1" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="O1" s="91"/>
-      <c r="P1" s="92"/>
+      <c r="O1" s="93"/>
+      <c r="P1" s="94"/>
     </row>
     <row r="2" spans="1:16" ht="25.5">
       <c r="A2" s="32" t="s">
@@ -5304,7 +5303,7 @@
       </c>
     </row>
     <row r="14" spans="1:16" ht="24" customHeight="1">
-      <c r="A14" s="102" t="s">
+      <c r="A14" s="85" t="s">
         <v>212</v>
       </c>
       <c r="B14" s="50">
@@ -5316,8 +5315,8 @@
       <c r="D14" s="50" t="s">
         <v>193</v>
       </c>
-      <c r="E14" s="75" t="s">
-        <v>194</v>
+      <c r="E14" s="67" t="s">
+        <v>28</v>
       </c>
       <c r="F14" s="50"/>
       <c r="G14" s="56"/>
@@ -5408,7 +5407,7 @@
       <c r="D16" s="50" t="s">
         <v>191</v>
       </c>
-      <c r="E16" s="101" t="s">
+      <c r="E16" s="84" t="s">
         <v>194</v>
       </c>
       <c r="F16" s="50"/>
@@ -5855,30 +5854,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="25.5" customHeight="1">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="95" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="93"/>
-      <c r="C1" s="93"/>
-      <c r="D1" s="93"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="94"/>
-      <c r="G1" s="94"/>
-      <c r="H1" s="94"/>
-      <c r="I1" s="94"/>
-      <c r="J1" s="94"/>
+      <c r="B1" s="95"/>
+      <c r="C1" s="95"/>
+      <c r="D1" s="95"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="96"/>
+      <c r="I1" s="96"/>
+      <c r="J1" s="96"/>
     </row>
     <row r="2" spans="1:10" ht="14.25">
       <c r="A2" s="10"/>
-      <c r="B2" s="95"/>
-      <c r="C2" s="96"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="99"/>
-      <c r="G2" s="100"/>
-      <c r="H2" s="98"/>
-      <c r="I2" s="99"/>
-      <c r="J2" s="100"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="100"/>
+      <c r="F2" s="101"/>
+      <c r="G2" s="102"/>
+      <c r="H2" s="100"/>
+      <c r="I2" s="101"/>
+      <c r="J2" s="102"/>
     </row>
     <row r="3" spans="1:10" ht="14.25">
       <c r="A3" s="1" t="s">

</xml_diff>

<commit_message>
contact page sequence updates
</commit_message>
<xml_diff>
--- a/PayBack - CEN3031 Scrum.xlsx
+++ b/PayBack - CEN3031 Scrum.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="615" windowWidth="11295" windowHeight="7455" tabRatio="885" activeTab="4"/>
+    <workbookView xWindow="390" yWindow="615" windowWidth="11295" windowHeight="7455" tabRatio="885" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="User Stories" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,6 @@
     <sheet name="Sprint 2 Burndown" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -196,7 +195,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="235">
   <si>
     <t>User Stories</t>
   </si>
@@ -898,17 +897,27 @@
   </si>
   <si>
     <t>Minor aesthetic improvements</t>
+  </si>
+  <si>
+    <t>Create "add contact" page sequence</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="53" x14ac:knownFonts="1">
+  <fonts count="54" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1832,411 +1841,417 @@
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="136">
+  <cellXfs count="138">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="14" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="15" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="22" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="23" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="16" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="16" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="33" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="20" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="20" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="46" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="48" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="49" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="50" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="40" borderId="0" xfId="4" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="40" borderId="0" xfId="4" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="38" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="38" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="37" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="37" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="40" borderId="0" xfId="4" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="38" borderId="0" xfId="2" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="37" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="40" borderId="0" xfId="4" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="40" borderId="0" xfId="4" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="38" borderId="0" xfId="2" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="37" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="40" borderId="0" xfId="4" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="38" borderId="0" xfId="2" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="38" borderId="0" xfId="2" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="38" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="38" borderId="0" xfId="2" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="38" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="38" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="41" borderId="0" xfId="5" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="41" borderId="0" xfId="5" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="41" borderId="0" xfId="5" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="41" borderId="0" xfId="5" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="41" borderId="0" xfId="5" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="41" borderId="0" xfId="5" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="37" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="37" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="37" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="37" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="37" borderId="11" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="37" borderId="11" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="37" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="37" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="41" borderId="0" xfId="5" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="41" borderId="0" xfId="5" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="41" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="41" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="41" borderId="17" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="41" borderId="17" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="41" borderId="23" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="41" borderId="23" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="38" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="38" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="38" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="38" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="38" borderId="11" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="38" borderId="11" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="38" borderId="9" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="38" borderId="9" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="39" borderId="0" xfId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="39" borderId="0" xfId="3" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="39" borderId="11" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="39" borderId="11" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="39" borderId="9" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="39" borderId="9" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="42" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="42" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="39" borderId="0" xfId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="39" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="37" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="38" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="37" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="38" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="39" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="39" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="41" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="41" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="34" fillId="20" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="50" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="41" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="33" fillId="20" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="39" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="41" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="43" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="38" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="37" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="37" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="41" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="38" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="49" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="39" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="41" borderId="0" xfId="5" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="8" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="45" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="25" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="41" borderId="17" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="41" borderId="23" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="41" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="41" borderId="11" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="41" borderId="9" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="41" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="38" borderId="11" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="38" borderId="9" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="38" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="37" borderId="11" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="37" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="37" borderId="17" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="37" borderId="23" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="39" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="39" borderId="11" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="39" borderId="9" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="37" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="41" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="38" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="37" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="39" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="15" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="41" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="39" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="3" fontId="15" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="41" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="43" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="38" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="37" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="37" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="36" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="41" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="24" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="38" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="21" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="43" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="39" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="41" borderId="0" xfId="5" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="27" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="19" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="15" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="25" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="41" borderId="17" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="41" borderId="23" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="41" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="41" borderId="11" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="41" borderId="9" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="41" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="38" borderId="11" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="38" borderId="9" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="38" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="37" borderId="11" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="37" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="37" borderId="17" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="37" borderId="23" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="39" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="39" borderId="11" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="39" borderId="9" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="37" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="36" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="24" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="21" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="27" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="19" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="15" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="17" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="17" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="41" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="38" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="37" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="39" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="14" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="14" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="41" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -2295,7 +2310,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2521,11 +2535,11 @@
             </a:ln>
           </c:spPr>
         </c:dropLines>
-        <c:axId val="57280000"/>
-        <c:axId val="57281920"/>
+        <c:axId val="120736000"/>
+        <c:axId val="120742272"/>
       </c:areaChart>
       <c:dateAx>
-        <c:axId val="57280000"/>
+        <c:axId val="120736000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2559,21 +2573,20 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="low"/>
-        <c:crossAx val="57281920"/>
+        <c:crossAx val="120742272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="57281920"/>
+        <c:axId val="120742272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2596,7 +2609,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -2618,14 +2630,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="57280000"/>
+        <c:crossAx val="120736000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2748,31 +2759,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>95</c:v>
+                  <c:v>103</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>93</c:v>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>93</c:v>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>93</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>93</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>93</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>93</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>93</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>93</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2847,30 +2858,52 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>95</c:v>
+                  <c:v>103</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>83.125</c:v>
+                  <c:v>90.125</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>71.25</c:v>
+                  <c:v>77.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>59.375</c:v>
+                  <c:v>64.375</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>47.5</c:v>
+                  <c:v>51.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>35.625</c:v>
+                  <c:v>38.625</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>23.75</c:v>
+                  <c:v>25.75</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11.875</c:v>
+                  <c:v>12.875</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Id</c:v>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 2 Burndown'!$L$7:$M$7</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2896,11 +2929,11 @@
             </a:ln>
           </c:spPr>
         </c:dropLines>
-        <c:axId val="58373632"/>
-        <c:axId val="58375552"/>
+        <c:axId val="121612544"/>
+        <c:axId val="121614720"/>
       </c:areaChart>
       <c:dateAx>
-        <c:axId val="58373632"/>
+        <c:axId val="121612544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2941,14 +2974,14 @@
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="low"/>
-        <c:crossAx val="58375552"/>
+        <c:crossAx val="121614720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="58375552"/>
+        <c:axId val="121614720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2993,7 +3026,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="58373632"/>
+        <c:crossAx val="121612544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3525,13 +3558,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="109" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="110"/>
-      <c r="C1" s="109"/>
-      <c r="D1" s="109"/>
-      <c r="E1" s="109"/>
+      <c r="A1" s="118" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="119"/>
+      <c r="C1" s="118"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="118"/>
     </row>
     <row r="2" spans="1:22" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
@@ -4481,8 +4514,8 @@
   <dimension ref="A1:E90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E80" sqref="E80"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4494,10 +4527,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="111" t="s">
+      <c r="A1" s="120" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="111"/>
+      <c r="B1" s="120"/>
       <c r="C1" s="81"/>
       <c r="D1" s="81"/>
     </row>
@@ -4816,11 +4849,11 @@
       <c r="A21" s="83" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="68" t="s">
-        <v>197</v>
+      <c r="B21" s="137" t="s">
+        <v>234</v>
       </c>
       <c r="C21" s="47">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D21" s="79" t="s">
         <v>8</v>
@@ -4831,10 +4864,10 @@
         <v>30</v>
       </c>
       <c r="B22" s="68" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C22" s="47">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D22" s="79" t="s">
         <v>8</v>
@@ -4845,10 +4878,10 @@
         <v>30</v>
       </c>
       <c r="B23" s="68" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C23" s="47">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D23" s="79" t="s">
         <v>8</v>
@@ -4859,7 +4892,7 @@
         <v>30</v>
       </c>
       <c r="B24" s="68" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C24" s="47">
         <v>2</v>
@@ -4873,13 +4906,13 @@
         <v>30</v>
       </c>
       <c r="B25" s="68" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C25" s="47">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D25" s="79" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4887,13 +4920,13 @@
         <v>30</v>
       </c>
       <c r="B26" s="68" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C26" s="47">
         <v>4</v>
       </c>
       <c r="D26" s="79" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4901,26 +4934,26 @@
         <v>30</v>
       </c>
       <c r="B27" s="68" t="s">
+        <v>202</v>
+      </c>
+      <c r="C27" s="47">
+        <v>4</v>
+      </c>
+      <c r="D27" s="79" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="83" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="68" t="s">
         <v>203</v>
       </c>
-      <c r="C27" s="47">
-        <v>8</v>
-      </c>
-      <c r="D27" s="79" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="47" t="s">
-        <v>30</v>
-      </c>
-      <c r="B28" s="74" t="s">
-        <v>138</v>
-      </c>
       <c r="C28" s="47">
-        <v>2</v>
-      </c>
-      <c r="D28" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" s="79" t="s">
         <v>9</v>
       </c>
     </row>
@@ -4928,8 +4961,8 @@
       <c r="A29" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="B29" s="40" t="s">
-        <v>139</v>
+      <c r="B29" s="74" t="s">
+        <v>138</v>
       </c>
       <c r="C29" s="47">
         <v>2</v>
@@ -4942,28 +4975,28 @@
       <c r="A30" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="135" t="s">
-        <v>233</v>
+      <c r="B30" s="40" t="s">
+        <v>139</v>
       </c>
       <c r="C30" s="47">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D30" s="47" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="51" t="s">
-        <v>49</v>
-      </c>
-      <c r="B31" s="38" t="s">
-        <v>146</v>
-      </c>
-      <c r="C31" s="51">
-        <v>2</v>
-      </c>
-      <c r="D31" s="51" t="s">
-        <v>6</v>
+      <c r="A31" s="47" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" s="117" t="s">
+        <v>233</v>
+      </c>
+      <c r="C31" s="47">
+        <v>4</v>
+      </c>
+      <c r="D31" s="47" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4971,13 +5004,13 @@
         <v>49</v>
       </c>
       <c r="B32" s="38" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C32" s="51">
         <v>2</v>
       </c>
       <c r="D32" s="51" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4985,13 +5018,13 @@
         <v>49</v>
       </c>
       <c r="B33" s="38" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C33" s="51">
         <v>2</v>
       </c>
       <c r="D33" s="51" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4999,10 +5032,10 @@
         <v>49</v>
       </c>
       <c r="B34" s="38" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C34" s="51">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D34" s="51" t="s">
         <v>6</v>
@@ -5013,13 +5046,13 @@
         <v>49</v>
       </c>
       <c r="B35" s="38" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C35" s="51">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D35" s="51" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5027,10 +5060,10 @@
         <v>49</v>
       </c>
       <c r="B36" s="38" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C36" s="51">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D36" s="51" t="s">
         <v>9</v>
@@ -5041,7 +5074,7 @@
         <v>49</v>
       </c>
       <c r="B37" s="38" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C37" s="51">
         <v>4</v>
@@ -5055,13 +5088,13 @@
         <v>49</v>
       </c>
       <c r="B38" s="38" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C38" s="51">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D38" s="51" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5069,13 +5102,13 @@
         <v>49</v>
       </c>
       <c r="B39" s="38" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C39" s="51">
         <v>2</v>
       </c>
       <c r="D39" s="51" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5083,13 +5116,13 @@
         <v>49</v>
       </c>
       <c r="B40" s="38" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C40" s="51">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D40" s="51" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5097,10 +5130,10 @@
         <v>49</v>
       </c>
       <c r="B41" s="38" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C41" s="51">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D41" s="51" t="s">
         <v>6</v>
@@ -5111,13 +5144,13 @@
         <v>49</v>
       </c>
       <c r="B42" s="38" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C42" s="51">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D42" s="51" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5125,10 +5158,10 @@
         <v>49</v>
       </c>
       <c r="B43" s="38" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C43" s="51">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D43" s="51" t="s">
         <v>9</v>
@@ -5139,7 +5172,7 @@
         <v>49</v>
       </c>
       <c r="B44" s="38" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C44" s="51">
         <v>4</v>
@@ -5153,13 +5186,13 @@
         <v>49</v>
       </c>
       <c r="B45" s="38" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C45" s="51">
         <v>4</v>
       </c>
       <c r="D45" s="51" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5167,13 +5200,13 @@
         <v>49</v>
       </c>
       <c r="B46" s="38" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C46" s="51">
         <v>4</v>
       </c>
       <c r="D46" s="51" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5181,13 +5214,13 @@
         <v>49</v>
       </c>
       <c r="B47" s="38" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C47" s="51">
         <v>4</v>
       </c>
       <c r="D47" s="51" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5195,13 +5228,13 @@
         <v>49</v>
       </c>
       <c r="B48" s="38" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C48" s="51">
         <v>4</v>
       </c>
       <c r="D48" s="51" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5209,13 +5242,13 @@
         <v>49</v>
       </c>
       <c r="B49" s="38" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C49" s="51">
         <v>4</v>
       </c>
       <c r="D49" s="51" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5223,27 +5256,27 @@
         <v>49</v>
       </c>
       <c r="B50" s="38" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C50" s="51">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D50" s="51" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="B51" s="76" t="s">
-        <v>215</v>
+      <c r="B51" s="38" t="s">
+        <v>165</v>
       </c>
       <c r="C51" s="51">
         <v>8</v>
       </c>
-      <c r="D51" s="80" t="s">
-        <v>8</v>
+      <c r="D51" s="51" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5251,10 +5284,10 @@
         <v>49</v>
       </c>
       <c r="B52" s="76" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C52" s="51">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D52" s="80" t="s">
         <v>8</v>
@@ -5265,10 +5298,10 @@
         <v>49</v>
       </c>
       <c r="B53" s="76" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C53" s="51">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D53" s="80" t="s">
         <v>8</v>
@@ -5279,10 +5312,10 @@
         <v>49</v>
       </c>
       <c r="B54" s="76" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C54" s="51">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="D54" s="80" t="s">
         <v>8</v>
@@ -5293,26 +5326,26 @@
         <v>49</v>
       </c>
       <c r="B55" s="76" t="s">
+        <v>218</v>
+      </c>
+      <c r="C55" s="51">
+        <v>2</v>
+      </c>
+      <c r="D55" s="80" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="51" t="s">
+        <v>49</v>
+      </c>
+      <c r="B56" s="76" t="s">
         <v>219</v>
       </c>
-      <c r="C55" s="51">
-        <v>4</v>
-      </c>
-      <c r="D55" s="80" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="44" t="s">
-        <v>92</v>
-      </c>
-      <c r="B56" s="43" t="s">
-        <v>223</v>
-      </c>
-      <c r="C56" s="44">
-        <v>2</v>
-      </c>
-      <c r="D56" s="44" t="s">
+      <c r="C56" s="51">
+        <v>4</v>
+      </c>
+      <c r="D56" s="80" t="s">
         <v>8</v>
       </c>
     </row>
@@ -5321,7 +5354,7 @@
         <v>92</v>
       </c>
       <c r="B57" s="43" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C57" s="44">
         <v>2</v>
@@ -5335,13 +5368,13 @@
         <v>92</v>
       </c>
       <c r="B58" s="43" t="s">
-        <v>167</v>
+        <v>224</v>
       </c>
       <c r="C58" s="44">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D58" s="44" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5349,16 +5382,13 @@
         <v>92</v>
       </c>
       <c r="B59" s="43" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C59" s="44">
         <v>4</v>
       </c>
       <c r="D59" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="E59" s="61" t="s">
-        <v>188</v>
+        <v>6</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5366,10 +5396,10 @@
         <v>92</v>
       </c>
       <c r="B60" s="43" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C60" s="44">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D60" s="44" t="s">
         <v>8</v>
@@ -5383,10 +5413,10 @@
         <v>92</v>
       </c>
       <c r="B61" s="43" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C61" s="44">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D61" s="44" t="s">
         <v>8</v>
@@ -5400,13 +5430,16 @@
         <v>92</v>
       </c>
       <c r="B62" s="43" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C62" s="44">
         <v>4</v>
       </c>
       <c r="D62" s="44" t="s">
         <v>8</v>
+      </c>
+      <c r="E62" s="61" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5414,16 +5447,13 @@
         <v>92</v>
       </c>
       <c r="B63" s="43" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C63" s="44">
         <v>4</v>
       </c>
       <c r="D63" s="44" t="s">
         <v>8</v>
-      </c>
-      <c r="E63" s="61" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5431,13 +5461,16 @@
         <v>92</v>
       </c>
       <c r="B64" s="43" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C64" s="44">
         <v>4</v>
       </c>
       <c r="D64" s="44" t="s">
         <v>8</v>
+      </c>
+      <c r="E64" s="61" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5445,16 +5478,13 @@
         <v>92</v>
       </c>
       <c r="B65" s="43" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C65" s="44">
         <v>4</v>
       </c>
       <c r="D65" s="44" t="s">
         <v>8</v>
-      </c>
-      <c r="E65" s="61" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5462,13 +5492,13 @@
         <v>92</v>
       </c>
       <c r="B66" s="43" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C66" s="44">
         <v>4</v>
       </c>
       <c r="D66" s="44" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E66" s="61" t="s">
         <v>188</v>
@@ -5479,13 +5509,16 @@
         <v>92</v>
       </c>
       <c r="B67" s="43" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C67" s="44">
         <v>4</v>
       </c>
       <c r="D67" s="44" t="s">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="E67" s="61" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5493,16 +5526,13 @@
         <v>92</v>
       </c>
       <c r="B68" s="43" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C68" s="44">
         <v>4</v>
       </c>
       <c r="D68" s="44" t="s">
         <v>8</v>
-      </c>
-      <c r="E68" s="61" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5510,13 +5540,16 @@
         <v>92</v>
       </c>
       <c r="B69" s="43" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C69" s="44">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D69" s="44" t="s">
         <v>8</v>
+      </c>
+      <c r="E69" s="61" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5524,13 +5557,13 @@
         <v>92</v>
       </c>
       <c r="B70" s="43" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C70" s="44">
         <v>8</v>
       </c>
       <c r="D70" s="44" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5538,7 +5571,7 @@
         <v>92</v>
       </c>
       <c r="B71" s="43" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C71" s="44">
         <v>8</v>
@@ -5552,10 +5585,10 @@
         <v>92</v>
       </c>
       <c r="B72" s="43" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C72" s="44">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D72" s="44" t="s">
         <v>9</v>
@@ -5566,7 +5599,7 @@
         <v>92</v>
       </c>
       <c r="B73" s="43" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C73" s="44">
         <v>4</v>
@@ -5579,8 +5612,8 @@
       <c r="A74" s="44" t="s">
         <v>92</v>
       </c>
-      <c r="B74" s="77" t="s">
-        <v>221</v>
+      <c r="B74" s="43" t="s">
+        <v>182</v>
       </c>
       <c r="C74" s="44">
         <v>4</v>
@@ -5590,31 +5623,28 @@
       </c>
     </row>
     <row r="75" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="82" t="s">
-        <v>210</v>
-      </c>
-      <c r="B75" s="66" t="s">
-        <v>191</v>
-      </c>
-      <c r="C75" s="62">
-        <v>16</v>
-      </c>
-      <c r="D75" s="82" t="s">
-        <v>8</v>
-      </c>
-      <c r="E75" s="61" t="s">
-        <v>188</v>
+      <c r="A75" s="44" t="s">
+        <v>92</v>
+      </c>
+      <c r="B75" s="77" t="s">
+        <v>221</v>
+      </c>
+      <c r="C75" s="44">
+        <v>4</v>
+      </c>
+      <c r="D75" s="44" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="82" t="s">
         <v>210</v>
       </c>
-      <c r="B76" s="57" t="s">
-        <v>189</v>
+      <c r="B76" s="66" t="s">
+        <v>191</v>
       </c>
       <c r="C76" s="62">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="D76" s="82" t="s">
         <v>8</v>
@@ -5627,11 +5657,11 @@
       <c r="A77" s="82" t="s">
         <v>210</v>
       </c>
-      <c r="B77" s="66" t="s">
-        <v>193</v>
+      <c r="B77" s="57" t="s">
+        <v>189</v>
       </c>
       <c r="C77" s="62">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D77" s="82" t="s">
         <v>8</v>
@@ -5644,14 +5674,17 @@
       <c r="A78" s="82" t="s">
         <v>210</v>
       </c>
-      <c r="B78" s="73" t="s">
-        <v>211</v>
+      <c r="B78" s="66" t="s">
+        <v>193</v>
       </c>
       <c r="C78" s="62">
         <v>2</v>
       </c>
       <c r="D78" s="82" t="s">
         <v>8</v>
+      </c>
+      <c r="E78" s="61" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5659,7 +5692,7 @@
         <v>210</v>
       </c>
       <c r="B79" s="73" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C79" s="62">
         <v>2</v>
@@ -5673,30 +5706,43 @@
         <v>210</v>
       </c>
       <c r="B80" s="73" t="s">
+        <v>212</v>
+      </c>
+      <c r="C80" s="62">
+        <v>2</v>
+      </c>
+      <c r="D80" s="82" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="82" t="s">
+        <v>210</v>
+      </c>
+      <c r="B81" s="73" t="s">
         <v>213</v>
       </c>
-      <c r="C80" s="62">
-        <v>2</v>
-      </c>
-      <c r="D80" s="82" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="81" spans="3:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C81" s="20">
-        <f>SUM(C3:C80)</f>
-        <v>307</v>
-      </c>
-    </row>
-    <row r="82" spans="3:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="83" spans="3:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="84" spans="3:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="85" spans="3:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="86" spans="3:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="87" spans="3:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="88" spans="3:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="89" spans="3:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="90" spans="3:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="C81" s="62">
+        <v>2</v>
+      </c>
+      <c r="D81" s="82" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C82" s="20">
+        <f>SUM(C3:C81)</f>
+        <v>311</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="84" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="85" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="86" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="87" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="88" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="89" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="90" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
@@ -5707,12 +5753,18 @@
   <legacyDrawing r:id="rId3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="81" yWindow="476" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="81" yWindow="476" count="2">
         <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="validationFailedClick and enter a value from range 'User Stories'!A3:A15">
           <x14:formula1>
             <xm:f>'User Stories'!A3:A15</xm:f>
           </x14:formula1>
-          <xm:sqref>A19:A27</xm:sqref>
+          <xm:sqref>A19:A21</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="validationFailedClick and enter a value from range 'User Stories'!A3:A15">
+          <x14:formula1>
+            <xm:f>'User Stories'!A5:A17</xm:f>
+          </x14:formula1>
+          <xm:sqref>A22:A28</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -5754,21 +5806,21 @@
       <c r="G1" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="112" t="s">
+      <c r="H1" s="121" t="s">
         <v>205</v>
       </c>
-      <c r="I1" s="113"/>
-      <c r="J1" s="114"/>
-      <c r="K1" s="115" t="s">
+      <c r="I1" s="122"/>
+      <c r="J1" s="123"/>
+      <c r="K1" s="124" t="s">
         <v>206</v>
       </c>
-      <c r="L1" s="116"/>
-      <c r="M1" s="117"/>
-      <c r="N1" s="115" t="s">
+      <c r="L1" s="125"/>
+      <c r="M1" s="126"/>
+      <c r="N1" s="124" t="s">
         <v>207</v>
       </c>
-      <c r="O1" s="116"/>
-      <c r="P1" s="117"/>
+      <c r="O1" s="125"/>
+      <c r="P1" s="126"/>
     </row>
     <row r="2" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A2" s="26" t="s">
@@ -6290,7 +6342,7 @@
       <c r="C13" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="127" t="s">
+      <c r="D13" s="109" t="s">
         <v>186</v>
       </c>
       <c r="E13" s="61" t="s">
@@ -6336,7 +6388,7 @@
       <c r="C14" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="127" t="s">
+      <c r="D14" s="109" t="s">
         <v>186</v>
       </c>
       <c r="E14" s="61" t="s">
@@ -6382,7 +6434,7 @@
       <c r="C15" s="93" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="127" t="s">
+      <c r="D15" s="109" t="s">
         <v>186</v>
       </c>
       <c r="E15" s="61" t="s">
@@ -6428,7 +6480,7 @@
       <c r="C16" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="127" t="s">
+      <c r="D16" s="109" t="s">
         <v>186</v>
       </c>
       <c r="E16" s="61" t="s">
@@ -6474,7 +6526,7 @@
       <c r="C17" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="127" t="s">
+      <c r="D17" s="109" t="s">
         <v>186</v>
       </c>
       <c r="E17" s="61" t="s">
@@ -7214,30 +7266,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="127" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="118"/>
-      <c r="C1" s="118"/>
-      <c r="D1" s="118"/>
-      <c r="E1" s="119"/>
-      <c r="F1" s="119"/>
-      <c r="G1" s="119"/>
-      <c r="H1" s="119"/>
-      <c r="I1" s="119"/>
-      <c r="J1" s="119"/>
+      <c r="B1" s="127"/>
+      <c r="C1" s="127"/>
+      <c r="D1" s="127"/>
+      <c r="E1" s="128"/>
+      <c r="F1" s="128"/>
+      <c r="G1" s="128"/>
+      <c r="H1" s="128"/>
+      <c r="I1" s="128"/>
+      <c r="J1" s="128"/>
     </row>
     <row r="2" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="8"/>
-      <c r="B2" s="120"/>
-      <c r="C2" s="121"/>
-      <c r="D2" s="122"/>
-      <c r="E2" s="123"/>
-      <c r="F2" s="124"/>
-      <c r="G2" s="125"/>
-      <c r="H2" s="123"/>
-      <c r="I2" s="124"/>
-      <c r="J2" s="125"/>
+      <c r="B2" s="129"/>
+      <c r="C2" s="130"/>
+      <c r="D2" s="131"/>
+      <c r="E2" s="132"/>
+      <c r="F2" s="133"/>
+      <c r="G2" s="134"/>
+      <c r="H2" s="132"/>
+      <c r="I2" s="133"/>
+      <c r="J2" s="134"/>
     </row>
     <row r="3" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
@@ -7303,31 +7355,31 @@
     </row>
     <row r="5" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="25"/>
-      <c r="B5" s="133">
+      <c r="B5" s="115">
         <v>1</v>
       </c>
-      <c r="C5" s="134">
-        <v>2</v>
-      </c>
-      <c r="D5" s="134">
+      <c r="C5" s="116">
+        <v>2</v>
+      </c>
+      <c r="D5" s="116">
         <v>3</v>
       </c>
-      <c r="E5" s="134">
-        <v>4</v>
-      </c>
-      <c r="F5" s="134">
+      <c r="E5" s="116">
+        <v>4</v>
+      </c>
+      <c r="F5" s="116">
         <v>5</v>
       </c>
-      <c r="G5" s="134">
+      <c r="G5" s="116">
         <v>6</v>
       </c>
-      <c r="H5" s="134">
+      <c r="H5" s="116">
         <v>7</v>
       </c>
-      <c r="I5" s="134">
-        <v>8</v>
-      </c>
-      <c r="J5" s="133">
+      <c r="I5" s="116">
+        <v>8</v>
+      </c>
+      <c r="J5" s="115">
         <v>9</v>
       </c>
       <c r="K5" s="10"/>
@@ -7336,39 +7388,39 @@
       <c r="A6" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="134">
+      <c r="B6" s="116">
         <f>SUM('Sprint 1'!H3:H29)</f>
         <v>95</v>
       </c>
-      <c r="C6" s="134">
+      <c r="C6" s="116">
         <f>SUM('Sprint 1'!I3:I29)</f>
         <v>82</v>
       </c>
-      <c r="D6" s="134">
+      <c r="D6" s="116">
         <f>SUM('Sprint 1'!J3:J29)</f>
         <v>71</v>
       </c>
-      <c r="E6" s="134">
+      <c r="E6" s="116">
         <f>SUM('Sprint 1'!K3:K29)</f>
         <v>59</v>
       </c>
-      <c r="F6" s="134">
+      <c r="F6" s="116">
         <f>SUM('Sprint 1'!L3:L29)</f>
         <v>43</v>
       </c>
-      <c r="G6" s="134">
+      <c r="G6" s="116">
         <f>SUM('Sprint 1'!M3:M29)</f>
         <v>28</v>
       </c>
-      <c r="H6" s="134">
+      <c r="H6" s="116">
         <f>SUM('Sprint 1'!N3:N29)</f>
         <v>16</v>
       </c>
-      <c r="I6" s="134">
+      <c r="I6" s="116">
         <f>SUM('Sprint 1'!O3:O29)</f>
         <v>12</v>
       </c>
-      <c r="J6" s="133">
+      <c r="J6" s="115">
         <f>SUM('Sprint 1'!P3:P29)</f>
         <v>6</v>
       </c>
@@ -7378,39 +7430,39 @@
       <c r="A7" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="131">
+      <c r="B7" s="113">
         <f>SUM('Sprint 1'!$B$3:$B$29)-(((B5-1)*SUM('Sprint 1'!$B$3:$B$29))/($J$5-1))</f>
         <v>95</v>
       </c>
-      <c r="C7" s="131">
+      <c r="C7" s="113">
         <f>SUM('Sprint 1'!$B$3:$B$29)-(((C5-1)*SUM('Sprint 1'!$B$3:$B$29))/($J$5-1))</f>
         <v>83.125</v>
       </c>
-      <c r="D7" s="131">
+      <c r="D7" s="113">
         <f>SUM('Sprint 1'!$B$3:$B$29)-(((D5-1)*SUM('Sprint 1'!$B$3:$B$29))/($J$5-1))</f>
         <v>71.25</v>
       </c>
-      <c r="E7" s="131">
+      <c r="E7" s="113">
         <f>SUM('Sprint 1'!$B$3:$B$29)-(((E5-1)*SUM('Sprint 1'!$B$3:$B$29))/($J$5-1))</f>
         <v>59.375</v>
       </c>
-      <c r="F7" s="131">
+      <c r="F7" s="113">
         <f>SUM('Sprint 1'!$B$3:$B$29)-(((F5-1)*SUM('Sprint 1'!$B$3:$B$29))/($J$5-1))</f>
         <v>47.5</v>
       </c>
-      <c r="G7" s="131">
+      <c r="G7" s="113">
         <f>SUM('Sprint 1'!$B$3:$B$29)-(((G5-1)*SUM('Sprint 1'!$B$3:$B$29))/($J$5-1))</f>
         <v>35.625</v>
       </c>
-      <c r="H7" s="131">
+      <c r="H7" s="113">
         <f>SUM('Sprint 1'!$B$3:$B$29)-(((H5-1)*SUM('Sprint 1'!$B$3:$B$29))/($J$5-1))</f>
         <v>23.75</v>
       </c>
-      <c r="I7" s="131">
+      <c r="I7" s="113">
         <f>SUM('Sprint 1'!$B$3:$B$29)-(((I5-1)*SUM('Sprint 1'!$B$3:$B$29))/($J$5-1))</f>
         <v>11.875</v>
       </c>
-      <c r="J7" s="132">
+      <c r="J7" s="114">
         <f>SUM('Sprint 1'!$B$3:$B$29)-(((J5-1)*SUM('Sprint 1'!$B$3:$B$29))/($J$5-1))</f>
         <v>0</v>
       </c>
@@ -7589,9 +7641,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R18" sqref="R18"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7612,6 +7664,7 @@
     <col min="14" max="14" width="3.5703125" customWidth="1"/>
     <col min="15" max="15" width="4.5703125" customWidth="1"/>
     <col min="16" max="16" width="4.7109375" customWidth="1"/>
+    <col min="18" max="26" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -7626,21 +7679,21 @@
       <c r="G1" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="115" t="s">
+      <c r="H1" s="124" t="s">
         <v>225</v>
       </c>
-      <c r="I1" s="116"/>
-      <c r="J1" s="117"/>
-      <c r="K1" s="115" t="s">
+      <c r="I1" s="125"/>
+      <c r="J1" s="126"/>
+      <c r="K1" s="124" t="s">
         <v>226</v>
       </c>
-      <c r="L1" s="116"/>
-      <c r="M1" s="117"/>
-      <c r="N1" s="115" t="s">
+      <c r="L1" s="125"/>
+      <c r="M1" s="126"/>
+      <c r="N1" s="124" t="s">
         <v>232</v>
       </c>
-      <c r="O1" s="116"/>
-      <c r="P1" s="117"/>
+      <c r="O1" s="125"/>
+      <c r="P1" s="126"/>
     </row>
     <row r="2" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A2" s="26" t="s">
@@ -7702,7 +7755,7 @@
       <c r="C3" s="79" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="127" t="s">
+      <c r="D3" s="109" t="s">
         <v>231</v>
       </c>
       <c r="E3" s="52" t="s">
@@ -7743,13 +7796,13 @@
         <v>196</v>
       </c>
       <c r="B4" s="47">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C4" s="79" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="127" t="s">
-        <v>187</v>
+      <c r="D4" s="136" t="s">
+        <v>186</v>
       </c>
       <c r="E4" s="52" t="s">
         <v>25</v>
@@ -7757,36 +7810,36 @@
       <c r="F4" s="47"/>
       <c r="G4" s="88"/>
       <c r="H4" s="42">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="I4" s="42">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="J4" s="49">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="K4" s="50">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="L4" s="48">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="M4" s="49">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="N4" s="50">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="O4" s="48">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="P4" s="48">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="68" t="s">
-        <v>202</v>
+      <c r="A5" s="137" t="s">
+        <v>234</v>
       </c>
       <c r="B5" s="47">
         <v>4</v>
@@ -7794,8 +7847,8 @@
       <c r="C5" s="79" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="127" t="s">
-        <v>231</v>
+      <c r="D5" s="136" t="s">
+        <v>186</v>
       </c>
       <c r="E5" s="52" t="s">
         <v>25</v>
@@ -7831,17 +7884,17 @@
       </c>
     </row>
     <row r="6" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="40" t="s">
-        <v>143</v>
+      <c r="A6" s="68" t="s">
+        <v>202</v>
       </c>
       <c r="B6" s="47">
-        <v>1</v>
-      </c>
-      <c r="C6" s="47" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="127" t="s">
-        <v>186</v>
+        <v>4</v>
+      </c>
+      <c r="C6" s="79" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="109" t="s">
+        <v>231</v>
       </c>
       <c r="E6" s="52" t="s">
         <v>25</v>
@@ -7849,183 +7902,183 @@
       <c r="F6" s="47"/>
       <c r="G6" s="88"/>
       <c r="H6" s="42">
+        <v>4</v>
+      </c>
+      <c r="I6" s="42">
+        <v>4</v>
+      </c>
+      <c r="J6" s="49">
+        <v>4</v>
+      </c>
+      <c r="K6" s="50">
+        <v>4</v>
+      </c>
+      <c r="L6" s="48">
+        <v>4</v>
+      </c>
+      <c r="M6" s="49">
+        <v>4</v>
+      </c>
+      <c r="N6" s="50">
+        <v>4</v>
+      </c>
+      <c r="O6" s="48">
+        <v>4</v>
+      </c>
+      <c r="P6" s="48">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="40" t="s">
+        <v>143</v>
+      </c>
+      <c r="B7" s="47">
         <v>1</v>
-      </c>
-      <c r="I6" s="42">
-        <v>1</v>
-      </c>
-      <c r="J6" s="49">
-        <v>1</v>
-      </c>
-      <c r="K6" s="50">
-        <v>1</v>
-      </c>
-      <c r="L6" s="48">
-        <v>1</v>
-      </c>
-      <c r="M6" s="49">
-        <v>1</v>
-      </c>
-      <c r="N6" s="50">
-        <v>1</v>
-      </c>
-      <c r="O6" s="48">
-        <v>1</v>
-      </c>
-      <c r="P6" s="48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="74" t="s">
-        <v>138</v>
-      </c>
-      <c r="B7" s="47">
-        <v>2</v>
       </c>
       <c r="C7" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="127" t="s">
+      <c r="D7" s="109" t="s">
         <v>186</v>
       </c>
-      <c r="E7" s="52" t="s">
-        <v>25</v>
+      <c r="E7" s="61" t="s">
+        <v>188</v>
       </c>
       <c r="F7" s="47"/>
       <c r="G7" s="88"/>
       <c r="H7" s="42">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I7" s="42">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J7" s="49">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K7" s="50">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L7" s="48">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M7" s="49">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N7" s="50">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O7" s="48">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P7" s="48">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="135" t="s">
-        <v>233</v>
+      <c r="A8" s="74" t="s">
+        <v>138</v>
       </c>
       <c r="B8" s="47">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C8" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="127" t="s">
+      <c r="D8" s="109" t="s">
         <v>186</v>
       </c>
-      <c r="E8" s="52" t="s">
-        <v>25</v>
+      <c r="E8" s="61" t="s">
+        <v>188</v>
       </c>
       <c r="F8" s="47"/>
       <c r="G8" s="88"/>
       <c r="H8" s="42">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I8" s="42">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J8" s="49">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K8" s="50">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L8" s="48">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M8" s="49">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="N8" s="50">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="O8" s="48">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="P8" s="48">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="76" t="s">
-        <v>217</v>
-      </c>
-      <c r="B9" s="51">
-        <v>16</v>
-      </c>
-      <c r="C9" s="80" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="128" t="s">
-        <v>229</v>
+      <c r="A9" s="117" t="s">
+        <v>233</v>
+      </c>
+      <c r="B9" s="47">
+        <v>4</v>
+      </c>
+      <c r="C9" s="47" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="109" t="s">
+        <v>186</v>
       </c>
       <c r="E9" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="51"/>
-      <c r="G9" s="94"/>
-      <c r="H9" s="39">
-        <v>16</v>
-      </c>
-      <c r="I9" s="39">
-        <v>16</v>
-      </c>
-      <c r="J9" s="55">
-        <v>16</v>
-      </c>
-      <c r="K9" s="56">
-        <v>16</v>
-      </c>
-      <c r="L9" s="54">
-        <v>16</v>
-      </c>
-      <c r="M9" s="55">
-        <v>16</v>
-      </c>
-      <c r="N9" s="56">
-        <v>16</v>
-      </c>
-      <c r="O9" s="54">
-        <v>16</v>
-      </c>
-      <c r="P9" s="54">
-        <v>16</v>
+      <c r="F9" s="47"/>
+      <c r="G9" s="88"/>
+      <c r="H9" s="42">
+        <v>4</v>
+      </c>
+      <c r="I9" s="42">
+        <v>4</v>
+      </c>
+      <c r="J9" s="49">
+        <v>4</v>
+      </c>
+      <c r="K9" s="50">
+        <v>3</v>
+      </c>
+      <c r="L9" s="48">
+        <v>3</v>
+      </c>
+      <c r="M9" s="49">
+        <v>3</v>
+      </c>
+      <c r="N9" s="50">
+        <v>3</v>
+      </c>
+      <c r="O9" s="48">
+        <v>3</v>
+      </c>
+      <c r="P9" s="48">
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="76" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B10" s="51">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C10" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="128" t="s">
-        <v>183</v>
+      <c r="D10" s="110" t="s">
+        <v>229</v>
       </c>
       <c r="E10" s="52" t="s">
         <v>25</v>
@@ -8033,44 +8086,44 @@
       <c r="F10" s="51"/>
       <c r="G10" s="94"/>
       <c r="H10" s="39">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="I10" s="39">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="J10" s="55">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="K10" s="56">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="L10" s="54">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="M10" s="55">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="N10" s="56">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="O10" s="54">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="P10" s="54">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="76" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B11" s="51">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C11" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="128" t="s">
+      <c r="D11" s="110" t="s">
         <v>183</v>
       </c>
       <c r="E11" s="52" t="s">
@@ -8079,36 +8132,36 @@
       <c r="F11" s="51"/>
       <c r="G11" s="94"/>
       <c r="H11" s="39">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="I11" s="39">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="J11" s="55">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="K11" s="56">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L11" s="54">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M11" s="55">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="N11" s="56">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="O11" s="54">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="P11" s="54">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="76" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B12" s="51">
         <v>4</v>
@@ -8116,8 +8169,8 @@
       <c r="C12" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="128" t="s">
-        <v>229</v>
+      <c r="D12" s="110" t="s">
+        <v>183</v>
       </c>
       <c r="E12" s="52" t="s">
         <v>25</v>
@@ -8128,41 +8181,41 @@
         <v>4</v>
       </c>
       <c r="I12" s="39">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J12" s="55">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K12" s="56">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L12" s="54">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M12" s="55">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N12" s="56">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O12" s="54">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P12" s="54">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="38" t="s">
-        <v>153</v>
+      <c r="A13" s="76" t="s">
+        <v>219</v>
       </c>
       <c r="B13" s="51">
-        <v>2</v>
-      </c>
-      <c r="C13" s="51" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="128" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="80" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="110" t="s">
         <v>229</v>
       </c>
       <c r="E13" s="52" t="s">
@@ -8171,44 +8224,44 @@
       <c r="F13" s="51"/>
       <c r="G13" s="94"/>
       <c r="H13" s="39">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I13" s="39">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J13" s="55">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K13" s="56">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L13" s="54">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M13" s="55">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N13" s="56">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="O13" s="54">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P13" s="54">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="38" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B14" s="51">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C14" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="128" t="s">
+      <c r="D14" s="110" t="s">
         <v>229</v>
       </c>
       <c r="E14" s="52" t="s">
@@ -8217,44 +8270,44 @@
       <c r="F14" s="51"/>
       <c r="G14" s="94"/>
       <c r="H14" s="39">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I14" s="39">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J14" s="55">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K14" s="56">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L14" s="54">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M14" s="55">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N14" s="56">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O14" s="54">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P14" s="54">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="38" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="B15" s="51">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C15" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="128" t="s">
+      <c r="D15" s="110" t="s">
         <v>229</v>
       </c>
       <c r="E15" s="52" t="s">
@@ -8263,44 +8316,44 @@
       <c r="F15" s="51"/>
       <c r="G15" s="94"/>
       <c r="H15" s="39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I15" s="39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J15" s="55">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K15" s="56">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L15" s="54">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M15" s="55">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N15" s="56">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O15" s="54">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P15" s="54">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="38" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B16" s="51">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C16" s="51" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" s="128" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="110" t="s">
         <v>229</v>
       </c>
       <c r="E16" s="52" t="s">
@@ -8309,91 +8362,91 @@
       <c r="F16" s="51"/>
       <c r="G16" s="94"/>
       <c r="H16" s="39">
+        <v>2</v>
+      </c>
+      <c r="I16" s="39">
+        <v>2</v>
+      </c>
+      <c r="J16" s="55">
+        <v>2</v>
+      </c>
+      <c r="K16" s="56">
+        <v>2</v>
+      </c>
+      <c r="L16" s="54">
+        <v>2</v>
+      </c>
+      <c r="M16" s="55">
+        <v>2</v>
+      </c>
+      <c r="N16" s="56">
+        <v>2</v>
+      </c>
+      <c r="O16" s="54">
+        <v>2</v>
+      </c>
+      <c r="P16" s="54">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="38" t="s">
+        <v>147</v>
+      </c>
+      <c r="B17" s="51">
         <v>1</v>
       </c>
-      <c r="I16" s="39">
+      <c r="C17" s="51" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="110" t="s">
+        <v>229</v>
+      </c>
+      <c r="E17" s="52" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" s="51"/>
+      <c r="G17" s="94"/>
+      <c r="H17" s="39">
         <v>1</v>
       </c>
-      <c r="J16" s="55">
+      <c r="I17" s="39">
         <v>1</v>
       </c>
-      <c r="K16" s="56">
+      <c r="J17" s="55">
         <v>1</v>
       </c>
-      <c r="L16" s="54">
+      <c r="K17" s="56">
         <v>1</v>
       </c>
-      <c r="M16" s="55">
+      <c r="L17" s="54">
         <v>1</v>
       </c>
-      <c r="N16" s="56">
+      <c r="M17" s="55">
         <v>1</v>
       </c>
-      <c r="O16" s="54">
+      <c r="N17" s="56">
         <v>1</v>
       </c>
-      <c r="P16" s="54">
+      <c r="O17" s="54">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="43" t="s">
-        <v>222</v>
-      </c>
-      <c r="B17" s="44">
-        <v>16</v>
-      </c>
-      <c r="C17" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" s="129" t="s">
-        <v>230</v>
-      </c>
-      <c r="E17" s="53" t="s">
-        <v>25</v>
-      </c>
-      <c r="F17" s="44"/>
-      <c r="G17" s="97"/>
-      <c r="H17" s="43">
-        <v>16</v>
-      </c>
-      <c r="I17" s="43">
-        <v>16</v>
-      </c>
-      <c r="J17" s="45">
-        <v>16</v>
-      </c>
-      <c r="K17" s="46">
-        <v>16</v>
-      </c>
-      <c r="L17" s="43">
-        <v>16</v>
-      </c>
-      <c r="M17" s="45">
-        <v>16</v>
-      </c>
-      <c r="N17" s="46">
-        <v>16</v>
-      </c>
-      <c r="O17" s="43">
-        <v>16</v>
-      </c>
-      <c r="P17" s="43">
-        <v>16</v>
+      <c r="P17" s="54">
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="43" t="s">
-        <v>178</v>
+        <v>222</v>
       </c>
       <c r="B18" s="44">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C18" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="D18" s="129" t="s">
-        <v>185</v>
+      <c r="D18" s="111" t="s">
+        <v>230</v>
       </c>
       <c r="E18" s="53" t="s">
         <v>25</v>
@@ -8401,44 +8454,44 @@
       <c r="F18" s="44"/>
       <c r="G18" s="97"/>
       <c r="H18" s="43">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="I18" s="43">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="J18" s="45">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="K18" s="46">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="L18" s="43">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="M18" s="45">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="N18" s="46">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="O18" s="43">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="P18" s="43">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="43" t="s">
-        <v>223</v>
+        <v>178</v>
       </c>
       <c r="B19" s="44">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C19" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="129" t="s">
+      <c r="D19" s="111" t="s">
         <v>185</v>
       </c>
       <c r="E19" s="53" t="s">
@@ -8447,36 +8500,36 @@
       <c r="F19" s="44"/>
       <c r="G19" s="97"/>
       <c r="H19" s="43">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="I19" s="43">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J19" s="45">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="K19" s="46">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="L19" s="43">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="M19" s="45">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="N19" s="46">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="O19" s="43">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="P19" s="43">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="43" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B20" s="44">
         <v>2</v>
@@ -8484,11 +8537,11 @@
       <c r="C20" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="D20" s="129" t="s">
+      <c r="D20" s="111" t="s">
         <v>185</v>
       </c>
-      <c r="E20" s="53" t="s">
-        <v>25</v>
+      <c r="E20" s="61" t="s">
+        <v>188</v>
       </c>
       <c r="F20" s="44"/>
       <c r="G20" s="97"/>
@@ -8499,38 +8552,38 @@
         <v>2</v>
       </c>
       <c r="J20" s="45">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K20" s="46">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L20" s="43">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M20" s="45">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N20" s="46">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O20" s="43">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P20" s="43">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="43" t="s">
-        <v>175</v>
+        <v>224</v>
       </c>
       <c r="B21" s="44">
         <v>2</v>
       </c>
       <c r="C21" s="44" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" s="129" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="111" t="s">
         <v>185</v>
       </c>
       <c r="E21" s="61" t="s">
@@ -8542,7 +8595,7 @@
         <v>2</v>
       </c>
       <c r="I21" s="43">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J21" s="45">
         <v>0</v>
@@ -8568,53 +8621,53 @@
     </row>
     <row r="22" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="43" t="s">
-        <v>221</v>
+        <v>175</v>
       </c>
       <c r="B22" s="44">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C22" s="44" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22" s="129" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="111" t="s">
         <v>185</v>
       </c>
-      <c r="E22" s="53" t="s">
-        <v>25</v>
+      <c r="E22" s="61" t="s">
+        <v>188</v>
       </c>
       <c r="F22" s="44"/>
       <c r="G22" s="97"/>
       <c r="H22" s="43">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I22" s="43">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J22" s="45">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K22" s="46">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L22" s="43">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M22" s="45">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="N22" s="46">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="O22" s="43">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="P22" s="43">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="77" t="s">
-        <v>176</v>
+      <c r="A23" s="43" t="s">
+        <v>221</v>
       </c>
       <c r="B23" s="44">
         <v>4</v>
@@ -8622,7 +8675,7 @@
       <c r="C23" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="D23" s="129" t="s">
+      <c r="D23" s="111" t="s">
         <v>185</v>
       </c>
       <c r="E23" s="53" t="s">
@@ -8659,61 +8712,106 @@
       </c>
     </row>
     <row r="24" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="73" t="s">
-        <v>211</v>
-      </c>
-      <c r="B24" s="62">
-        <v>2</v>
-      </c>
-      <c r="C24" s="62" t="s">
-        <v>8</v>
-      </c>
-      <c r="D24" s="130" t="s">
-        <v>186</v>
+      <c r="A24" s="77" t="s">
+        <v>176</v>
+      </c>
+      <c r="B24" s="44">
+        <v>4</v>
+      </c>
+      <c r="C24" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="111" t="s">
+        <v>185</v>
       </c>
       <c r="E24" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="F24" s="62"/>
-      <c r="G24" s="102"/>
-      <c r="H24" s="57">
-        <v>2</v>
-      </c>
-      <c r="I24" s="57">
-        <v>2</v>
-      </c>
-      <c r="J24" s="58">
-        <v>2</v>
-      </c>
-      <c r="K24" s="59">
-        <v>2</v>
-      </c>
-      <c r="L24" s="57">
-        <v>2</v>
-      </c>
-      <c r="M24" s="58">
-        <v>2</v>
-      </c>
-      <c r="N24" s="59">
-        <v>2</v>
-      </c>
-      <c r="O24" s="57">
-        <v>2</v>
-      </c>
-      <c r="P24" s="57">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F25" s="104" t="s">
+      <c r="F24" s="44"/>
+      <c r="G24" s="97"/>
+      <c r="H24" s="43">
+        <v>4</v>
+      </c>
+      <c r="I24" s="43">
+        <v>4</v>
+      </c>
+      <c r="J24" s="45">
+        <v>4</v>
+      </c>
+      <c r="K24" s="46">
+        <v>4</v>
+      </c>
+      <c r="L24" s="43">
+        <v>4</v>
+      </c>
+      <c r="M24" s="45">
+        <v>4</v>
+      </c>
+      <c r="N24" s="46">
+        <v>4</v>
+      </c>
+      <c r="O24" s="43">
+        <v>4</v>
+      </c>
+      <c r="P24" s="43">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="73" t="s">
+        <v>211</v>
+      </c>
+      <c r="B25" s="62">
+        <v>2</v>
+      </c>
+      <c r="C25" s="62" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="112" t="s">
+        <v>186</v>
+      </c>
+      <c r="E25" s="53" t="s">
+        <v>25</v>
+      </c>
+      <c r="F25" s="62"/>
+      <c r="G25" s="102"/>
+      <c r="H25" s="57">
+        <v>2</v>
+      </c>
+      <c r="I25" s="57">
+        <v>2</v>
+      </c>
+      <c r="J25" s="58">
+        <v>2</v>
+      </c>
+      <c r="K25" s="59">
+        <v>2</v>
+      </c>
+      <c r="L25" s="57">
+        <v>2</v>
+      </c>
+      <c r="M25" s="58">
+        <v>2</v>
+      </c>
+      <c r="N25" s="59">
+        <v>2</v>
+      </c>
+      <c r="O25" s="57">
+        <v>2</v>
+      </c>
+      <c r="P25" s="57">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F26" s="104" t="s">
         <v>204</v>
       </c>
-      <c r="H25">
-        <f>SUM(H3:H24)</f>
-        <v>95</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="H26">
+        <f>SUM(H3:H25)</f>
+        <v>103</v>
+      </c>
+    </row>
     <row r="27" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="28" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="29" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8730,8 +8828,8 @@
     <mergeCell ref="K1:M1"/>
     <mergeCell ref="N1:P1"/>
   </mergeCells>
-  <conditionalFormatting sqref="H6:P6">
-    <cfRule type="iconSet" priority="19">
+  <conditionalFormatting sqref="H7:P7">
+    <cfRule type="iconSet" priority="21">
       <iconSet iconSet="3Symbols" reverse="1">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="0" gte="0"/>
@@ -8739,7 +8837,16 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H6:P6">
+  <conditionalFormatting sqref="H7:P7">
+    <cfRule type="iconSet" priority="14">
+      <iconSet iconSet="3Symbols" reverse="1">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="0" gte="0"/>
+        <cfvo type="percent" val="&quot;B3&quot;"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3:P3">
     <cfRule type="iconSet" priority="12">
       <iconSet iconSet="3Symbols" reverse="1">
         <cfvo type="percent" val="0"/>
@@ -8749,6 +8856,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:P3">
+    <cfRule type="iconSet" priority="11">
+      <iconSet iconSet="3Symbols" reverse="1">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="0" gte="0"/>
+        <cfvo type="percent" val="&quot;B3&quot;"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H6:P6">
     <cfRule type="iconSet" priority="10">
       <iconSet iconSet="3Symbols" reverse="1">
         <cfvo type="percent" val="0"/>
@@ -8757,7 +8873,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H3:P3">
+  <conditionalFormatting sqref="H6:P6">
     <cfRule type="iconSet" priority="9">
       <iconSet iconSet="3Symbols" reverse="1">
         <cfvo type="percent" val="0"/>
@@ -8766,7 +8882,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H5:P5">
+  <conditionalFormatting sqref="H8:P8">
     <cfRule type="iconSet" priority="8">
       <iconSet iconSet="3Symbols" reverse="1">
         <cfvo type="percent" val="0"/>
@@ -8775,7 +8891,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H5:P5">
+  <conditionalFormatting sqref="H8:P8">
     <cfRule type="iconSet" priority="7">
       <iconSet iconSet="3Symbols" reverse="1">
         <cfvo type="percent" val="0"/>
@@ -8784,7 +8900,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H7:P7">
+  <conditionalFormatting sqref="H4:P4">
     <cfRule type="iconSet" priority="6">
       <iconSet iconSet="3Symbols" reverse="1">
         <cfvo type="percent" val="0"/>
@@ -8793,7 +8909,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H7:P7">
+  <conditionalFormatting sqref="H4:P4">
     <cfRule type="iconSet" priority="5">
       <iconSet iconSet="3Symbols" reverse="1">
         <cfvo type="percent" val="0"/>
@@ -8802,7 +8918,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H4:P4">
+  <conditionalFormatting sqref="H9:P9">
     <cfRule type="iconSet" priority="4">
       <iconSet iconSet="3Symbols" reverse="1">
         <cfvo type="percent" val="0"/>
@@ -8811,7 +8927,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H4:P4">
+  <conditionalFormatting sqref="H9:P9">
     <cfRule type="iconSet" priority="3">
       <iconSet iconSet="3Symbols" reverse="1">
         <cfvo type="percent" val="0"/>
@@ -8820,7 +8936,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H8:P8">
+  <conditionalFormatting sqref="H5:P5">
     <cfRule type="iconSet" priority="2">
       <iconSet iconSet="3Symbols" reverse="1">
         <cfvo type="percent" val="0"/>
@@ -8829,7 +8945,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H8:P8">
+  <conditionalFormatting sqref="H5:P5">
     <cfRule type="iconSet" priority="1">
       <iconSet iconSet="3Symbols" reverse="1">
         <cfvo type="percent" val="0"/>
@@ -8839,17 +8955,18 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G33" sqref="G33"/>
+      <selection pane="bottomLeft" activeCell="N12" sqref="K12:N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8857,33 +8974,33 @@
     <col min="2" max="10" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="126" t="s">
+    <row r="1" spans="1:13" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="135" t="s">
         <v>228</v>
       </c>
-      <c r="B1" s="118"/>
-      <c r="C1" s="118"/>
-      <c r="D1" s="118"/>
-      <c r="E1" s="119"/>
-      <c r="F1" s="119"/>
-      <c r="G1" s="119"/>
-      <c r="H1" s="119"/>
-      <c r="I1" s="119"/>
-      <c r="J1" s="119"/>
-    </row>
-    <row r="2" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="B1" s="127"/>
+      <c r="C1" s="127"/>
+      <c r="D1" s="127"/>
+      <c r="E1" s="128"/>
+      <c r="F1" s="128"/>
+      <c r="G1" s="128"/>
+      <c r="H1" s="128"/>
+      <c r="I1" s="128"/>
+      <c r="J1" s="128"/>
+    </row>
+    <row r="2" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="8"/>
-      <c r="B2" s="120"/>
-      <c r="C2" s="121"/>
-      <c r="D2" s="122"/>
-      <c r="E2" s="123"/>
-      <c r="F2" s="124"/>
-      <c r="G2" s="125"/>
-      <c r="H2" s="123"/>
-      <c r="I2" s="124"/>
-      <c r="J2" s="125"/>
-    </row>
-    <row r="3" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="B2" s="129"/>
+      <c r="C2" s="130"/>
+      <c r="D2" s="131"/>
+      <c r="E2" s="132"/>
+      <c r="F2" s="133"/>
+      <c r="G2" s="134"/>
+      <c r="H2" s="132"/>
+      <c r="I2" s="133"/>
+      <c r="J2" s="134"/>
+    </row>
+    <row r="3" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>208</v>
       </c>
@@ -8915,7 +9032,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="69">
         <v>41556</v>
@@ -8945,7 +9062,7 @@
         <v>41575</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="25"/>
       <c r="B5" s="22">
         <v>1</v>
@@ -8983,92 +9100,106 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="21" t="s">
         <v>27</v>
       </c>
       <c r="B6" s="10">
-        <f>SUM('Sprint 2'!H3:H24)</f>
-        <v>95</v>
+        <f>SUM('Sprint 2'!H3:H25)</f>
+        <v>103</v>
       </c>
       <c r="C6" s="15">
         <f>SUM('Sprint 2'!I3:I31)</f>
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="D6" s="28">
         <f>SUM('Sprint 2'!J3:J31)</f>
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E6" s="10">
         <f>SUM('Sprint 2'!K3:K31)</f>
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F6" s="15">
         <f>SUM('Sprint 2'!L3:L31)</f>
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="G6" s="28">
         <f>SUM('Sprint 2'!M3:M31)</f>
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="H6" s="10">
         <f>SUM('Sprint 2'!N3:N31)</f>
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="I6" s="15">
         <f>SUM('Sprint 2'!O3:O31)</f>
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="J6" s="28">
         <f>SUM('Sprint 2'!P3:P31)</f>
-        <v>93</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+      <c r="L6" s="69">
+        <v>41556</v>
+      </c>
+      <c r="M6" s="71">
+        <v>41575</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="21" t="s">
         <v>28</v>
       </c>
       <c r="B7" s="5">
         <f>SUM('Sprint 2'!$B$3:$B$31)-(((B5-1)*SUM('Sprint 2'!$B$3:$B$31))/($J$5-1))</f>
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="C7" s="16">
         <f>SUM('Sprint 2'!$B$3:$B$31)-(((C5-1)*SUM('Sprint 2'!$B$3:$B$31))/($J$5-1))</f>
-        <v>83.125</v>
+        <v>90.125</v>
       </c>
       <c r="D7" s="11">
         <f>SUM('Sprint 2'!$B$3:$B$31)-(((D5-1)*SUM('Sprint 2'!$B$3:$B$31))/($J$5-1))</f>
-        <v>71.25</v>
+        <v>77.25</v>
       </c>
       <c r="E7" s="5">
         <f>SUM('Sprint 2'!$B$3:$B$31)-(((E5-1)*SUM('Sprint 2'!$B$3:$B$31))/($J$5-1))</f>
-        <v>59.375</v>
+        <v>64.375</v>
       </c>
       <c r="F7" s="16">
         <f>SUM('Sprint 2'!$B$3:$B$31)-(((F5-1)*SUM('Sprint 2'!$B$3:$B$31))/($J$5-1))</f>
-        <v>47.5</v>
+        <v>51.5</v>
       </c>
       <c r="G7" s="11">
         <f>SUM('Sprint 2'!$B$3:$B$31)-(((G5-1)*SUM('Sprint 2'!$B$3:$B$31))/($J$5-1))</f>
-        <v>35.625</v>
+        <v>38.625</v>
       </c>
       <c r="H7" s="5">
         <f>SUM('Sprint 2'!$B$3:$B$31)-(((H5-1)*SUM('Sprint 2'!$B$3:$B$31))/($J$5-1))</f>
-        <v>23.75</v>
+        <v>25.75</v>
       </c>
       <c r="I7" s="16">
         <f>SUM('Sprint 2'!$B$3:$B$31)-(((I5-1)*SUM('Sprint 2'!$B$3:$B$31))/($J$5-1))</f>
-        <v>11.875</v>
+        <v>12.875</v>
       </c>
       <c r="J7" s="11">
         <f>SUM('Sprint 2'!$B$3:$B$31)-(((J5-1)*SUM('Sprint 2'!$B$3:$B$31))/($J$5-1))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L7" s="5">
+        <f>SUM('Sprint 2'!$B$3:$B$31)-(((B5-1)*SUM('Sprint 2'!$B$3:$B$31))/($J$5-1))</f>
+        <v>103</v>
+      </c>
+      <c r="M7" s="11">
+        <f>SUM('Sprint 2'!$B$3:$B$31)-(((J5-1)*SUM('Sprint 2'!$B$3:$B$31))/($J$5-1))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="15" t="s">
         <v>29</v>
       </c>
@@ -9078,7 +9209,7 @@
       <c r="F11" s="15"/>
       <c r="G11" s="15"/>
     </row>
-    <row r="12" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="15"/>
       <c r="C12" s="15"/>
       <c r="D12" s="15"/>
@@ -9086,7 +9217,7 @@
       <c r="F12" s="15"/>
       <c r="G12" s="15"/>
     </row>
-    <row r="13" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="15"/>
       <c r="C13" s="15"/>
       <c r="D13" s="15"/>
@@ -9094,7 +9225,7 @@
       <c r="F13" s="15"/>
       <c r="G13" s="15"/>
     </row>
-    <row r="14" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="15"/>
       <c r="C14" s="15"/>
       <c r="D14" s="15"/>
@@ -9102,7 +9233,7 @@
       <c r="F14" s="15"/>
       <c r="G14" s="15"/>
     </row>
-    <row r="15" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
@@ -9110,7 +9241,7 @@
       <c r="F15" s="15"/>
       <c r="G15" s="15"/>
     </row>
-    <row r="16" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="15"/>
       <c r="C16" s="15"/>
       <c r="D16" s="15"/>

</xml_diff>

<commit_message>
Updated Doc 	modified:   PayBack - CEN3031 Scrum.xlsx
</commit_message>
<xml_diff>
--- a/PayBack - CEN3031 Scrum.xlsx
+++ b/PayBack - CEN3031 Scrum.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HJeon\Documents\GitHub\PayBack\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="390" yWindow="615" windowWidth="11295" windowHeight="7455" tabRatio="885" activeTab="4"/>
   </bookViews>
@@ -19,7 +14,7 @@
     <sheet name="Sprint 2" sheetId="6" r:id="rId5"/>
     <sheet name="Sprint 2 Burndown" sheetId="7" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -29,7 +24,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="V1" authorId="0" shapeId="0">
+    <comment ref="V1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -52,7 +47,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -75,7 +70,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="B2" authorId="0" shapeId="0">
+    <comment ref="B2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -91,7 +86,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C2" authorId="0" shapeId="0">
+    <comment ref="C2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -104,7 +99,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D2" authorId="0" shapeId="0">
+    <comment ref="D2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -117,7 +112,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E2" authorId="0" shapeId="0">
+    <comment ref="E2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -140,7 +135,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="B2" authorId="0" shapeId="0">
+    <comment ref="B2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -156,7 +151,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C2" authorId="0" shapeId="0">
+    <comment ref="C2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -169,7 +164,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D2" authorId="0" shapeId="0">
+    <comment ref="D2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -182,7 +177,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E2" authorId="0" shapeId="0">
+    <comment ref="E2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -200,7 +195,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="848" uniqueCount="249">
   <si>
     <t>User Stories</t>
   </si>
@@ -953,18 +948,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="58" x14ac:knownFonts="1">
+  <fonts count="57" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1916,450 +1904,447 @@
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="149">
+  <cellXfs count="148">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="18" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="17" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="26" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="25" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="16" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="16" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="20" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="20" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="48" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="52" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="51" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="53" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="52" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="40" borderId="0" xfId="4" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="40" borderId="0" xfId="4" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="38" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="38" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="37" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="37" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="40" borderId="0" xfId="4" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="38" borderId="0" xfId="2" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="37" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="40" borderId="0" xfId="4" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="40" borderId="0" xfId="4" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="38" borderId="0" xfId="2" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="37" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="40" borderId="0" xfId="4" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="38" borderId="0" xfId="2" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="38" borderId="0" xfId="2" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="38" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="38" borderId="0" xfId="2" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="38" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="38" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="41" borderId="0" xfId="5" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="41" borderId="0" xfId="5" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="41" borderId="0" xfId="5" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="41" borderId="0" xfId="5" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="41" borderId="0" xfId="5" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="41" borderId="0" xfId="5" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="37" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="37" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="37" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="37" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="37" borderId="11" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="37" borderId="11" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="37" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="37" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="41" borderId="0" xfId="5" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="41" borderId="0" xfId="5" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="41" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="41" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="41" borderId="17" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="41" borderId="17" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="41" borderId="23" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="41" borderId="23" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="38" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="38" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="38" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="38" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="38" borderId="11" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="38" borderId="11" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="38" borderId="9" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="38" borderId="9" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="39" borderId="0" xfId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="39" borderId="0" xfId="3" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="39" borderId="11" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="39" borderId="11" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="39" borderId="9" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="39" borderId="9" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="42" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="42" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="39" borderId="0" xfId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="39" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="37" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="38" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="37" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="38" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="39" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="39" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="41" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="41" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="41" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="37" fillId="20" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="53" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="12" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="41" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="39" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="36" fillId="20" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="52" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="11" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="41" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="39" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="41" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="41" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="43" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="43" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="38" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="38" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="37" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="37" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="37" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="41" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="38" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="39" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="41" borderId="0" xfId="5" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="25" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="41" borderId="17" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="41" borderId="23" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="41" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="41" borderId="11" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="41" borderId="9" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="37" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="41" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="38" borderId="11" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="38" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="38" borderId="9" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="39" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="38" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="41" borderId="0" xfId="5" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="37" borderId="11" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="51" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="37" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="25" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="37" borderId="17" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="37" borderId="23" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="41" borderId="17" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="39" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="41" borderId="23" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="39" borderId="11" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="41" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="39" borderId="9" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="41" borderId="11" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="41" borderId="9" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="41" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="38" borderId="11" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="38" borderId="9" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="38" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="37" borderId="11" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="37" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="37" borderId="17" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="37" borderId="23" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="39" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="39" borderId="11" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="39" borderId="9" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="37" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="41" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="38" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="37" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="39" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="18" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="18" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="41" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="41" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="38" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="37" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="39" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="17" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="17" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="41" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="41" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="41" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="37" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="38" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="38" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="57" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="37" borderId="28" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="37" borderId="28" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="37" borderId="23" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="37" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="37" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="38" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="38" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="56" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="37" borderId="28" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="42" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="37" borderId="28" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="37" borderId="23" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="37" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="37" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="56" fillId="36" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="24" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="21" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="54" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="27" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="19" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="15" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="17" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="42" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="36" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="24" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="21" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="27" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="19" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="15" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="17" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -2646,11 +2631,11 @@
             </a:ln>
           </c:spPr>
         </c:dropLines>
-        <c:axId val="252101264"/>
-        <c:axId val="252100480"/>
+        <c:axId val="61224064"/>
+        <c:axId val="70764032"/>
       </c:areaChart>
       <c:dateAx>
-        <c:axId val="252101264"/>
+        <c:axId val="61224064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2690,14 +2675,14 @@
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="low"/>
-        <c:crossAx val="252100480"/>
+        <c:crossAx val="70764032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="252100480"/>
+        <c:axId val="70764032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2741,7 +2726,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="252101264"/>
+        <c:crossAx val="61224064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2813,23 +2798,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1500" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -2991,10 +2959,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>11</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>16</c:v>
@@ -3090,6 +3058,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3176,22 +3145,22 @@
                   <c:v>87</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>83</c:v>
+                  <c:v>82</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>65</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>60</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>54</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>54</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>54</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3315,11 +3284,11 @@
             </a:ln>
           </c:spPr>
         </c:dropLines>
-        <c:axId val="254649416"/>
-        <c:axId val="254647456"/>
+        <c:axId val="81426304"/>
+        <c:axId val="81453056"/>
       </c:areaChart>
       <c:dateAx>
-        <c:axId val="254649416"/>
+        <c:axId val="81426304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3353,20 +3322,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="low"/>
-        <c:crossAx val="254647456"/>
+        <c:crossAx val="81453056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="254647456"/>
+        <c:axId val="81453056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3389,6 +3359,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -3410,13 +3381,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="254649416"/>
+        <c:crossAx val="81426304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4279,7 +4251,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4314,7 +4286,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5493,11 +5465,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E90"/>
+  <dimension ref="A1:E95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
+      <pane ySplit="2" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6619,112 +6591,207 @@
       </c>
     </row>
     <row r="76" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="82" t="s">
+      <c r="A76" s="44" t="s">
+        <v>92</v>
+      </c>
+      <c r="B76" s="126" t="s">
+        <v>236</v>
+      </c>
+      <c r="C76" s="44">
+        <v>4</v>
+      </c>
+      <c r="D76" s="44" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="44" t="s">
+        <v>92</v>
+      </c>
+      <c r="B77" s="126" t="s">
+        <v>239</v>
+      </c>
+      <c r="C77" s="44">
+        <v>1</v>
+      </c>
+      <c r="D77" s="44" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="44" t="s">
+        <v>92</v>
+      </c>
+      <c r="B78" s="126" t="s">
+        <v>240</v>
+      </c>
+      <c r="C78" s="44">
+        <v>2</v>
+      </c>
+      <c r="D78" s="44" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="44" t="s">
+        <v>92</v>
+      </c>
+      <c r="B79" s="126" t="s">
+        <v>244</v>
+      </c>
+      <c r="C79" s="44">
+        <v>1</v>
+      </c>
+      <c r="D79" s="44" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="44" t="s">
+        <v>92</v>
+      </c>
+      <c r="B80" s="126" t="s">
+        <v>242</v>
+      </c>
+      <c r="C80" s="44">
+        <v>4</v>
+      </c>
+      <c r="D80" s="44" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="44" t="s">
+        <v>92</v>
+      </c>
+      <c r="B81" s="126" t="s">
+        <v>243</v>
+      </c>
+      <c r="C81" s="44">
+        <v>4</v>
+      </c>
+      <c r="D81" s="44" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="82" t="s">
         <v>210</v>
       </c>
-      <c r="B76" s="66" t="s">
+      <c r="B82" s="66" t="s">
         <v>191</v>
       </c>
-      <c r="C76" s="62">
+      <c r="C82" s="62">
         <v>16</v>
       </c>
-      <c r="D76" s="82" t="s">
-        <v>8</v>
-      </c>
-      <c r="E76" s="61" t="s">
+      <c r="D82" s="82" t="s">
+        <v>8</v>
+      </c>
+      <c r="E82" s="61" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="77" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="82" t="s">
+    <row r="83" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="82" t="s">
         <v>210</v>
       </c>
-      <c r="B77" s="57" t="s">
+      <c r="B83" s="57" t="s">
         <v>189</v>
       </c>
-      <c r="C77" s="62">
+      <c r="C83" s="62">
         <v>1</v>
       </c>
-      <c r="D77" s="82" t="s">
-        <v>8</v>
-      </c>
-      <c r="E77" s="61" t="s">
+      <c r="D83" s="82" t="s">
+        <v>8</v>
+      </c>
+      <c r="E83" s="61" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="82" t="s">
+    <row r="84" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="82" t="s">
         <v>210</v>
       </c>
-      <c r="B78" s="66" t="s">
+      <c r="B84" s="66" t="s">
         <v>193</v>
       </c>
-      <c r="C78" s="62">
-        <v>2</v>
-      </c>
-      <c r="D78" s="82" t="s">
-        <v>8</v>
-      </c>
-      <c r="E78" s="61" t="s">
+      <c r="C84" s="62">
+        <v>2</v>
+      </c>
+      <c r="D84" s="82" t="s">
+        <v>8</v>
+      </c>
+      <c r="E84" s="61" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="79" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="82" t="s">
+    <row r="85" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="82" t="s">
         <v>210</v>
       </c>
-      <c r="B79" s="73" t="s">
+      <c r="B85" s="73" t="s">
         <v>211</v>
       </c>
-      <c r="C79" s="62">
-        <v>2</v>
-      </c>
-      <c r="D79" s="82" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="82" t="s">
+      <c r="C85" s="62">
+        <v>2</v>
+      </c>
+      <c r="D85" s="82" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="82" t="s">
         <v>210</v>
       </c>
-      <c r="B80" s="73" t="s">
+      <c r="B86" s="73" t="s">
         <v>212</v>
       </c>
-      <c r="C80" s="62">
-        <v>2</v>
-      </c>
-      <c r="D80" s="82" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="82" t="s">
+      <c r="C86" s="62">
+        <v>2</v>
+      </c>
+      <c r="D86" s="82" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="82" t="s">
         <v>210</v>
       </c>
-      <c r="B81" s="73" t="s">
+      <c r="B87" s="73" t="s">
         <v>213</v>
       </c>
-      <c r="C81" s="62">
-        <v>2</v>
-      </c>
-      <c r="D81" s="82" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C82" s="20">
-        <f>SUM(C3:C81)</f>
-        <v>311</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="84" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="85" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="86" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="87" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="88" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="89" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="90" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="C87" s="62">
+        <v>2</v>
+      </c>
+      <c r="D87" s="82" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C88" s="20">
+        <f>SUM(C3:C87)</f>
+        <v>327</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="90" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A90"/>
+    </row>
+    <row r="91" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A91"/>
+    </row>
+    <row r="92" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A92"/>
+    </row>
+    <row r="93" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A93"/>
+    </row>
+    <row r="94" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A94"/>
+    </row>
+    <row r="95" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A95"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
@@ -8623,9 +8690,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q24" sqref="Q24"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8775,7 +8842,7 @@
       </c>
       <c r="R3">
         <f>SUM(P3:P9)</f>
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -8837,8 +8904,8 @@
       <c r="D5" s="117" t="s">
         <v>186</v>
       </c>
-      <c r="E5" s="52" t="s">
-        <v>25</v>
+      <c r="E5" s="61" t="s">
+        <v>188</v>
       </c>
       <c r="F5" s="47"/>
       <c r="G5" s="88"/>
@@ -8858,16 +8925,16 @@
         <v>2</v>
       </c>
       <c r="M5" s="49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N5" s="50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O5" s="48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P5" s="48">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -9101,7 +9168,7 @@
       </c>
       <c r="R10">
         <f>SUM(P10:P17)</f>
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -9117,8 +9184,8 @@
       <c r="D11" s="121" t="s">
         <v>186</v>
       </c>
-      <c r="E11" s="52" t="s">
-        <v>25</v>
+      <c r="E11" s="61" t="s">
+        <v>188</v>
       </c>
       <c r="F11" s="51"/>
       <c r="G11" s="94"/>
@@ -9138,16 +9205,16 @@
         <v>4</v>
       </c>
       <c r="M11" s="55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N11" s="56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O11" s="54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P11" s="54">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -9347,8 +9414,8 @@
       <c r="D16" s="121" t="s">
         <v>186</v>
       </c>
-      <c r="E16" s="52" t="s">
-        <v>25</v>
+      <c r="E16" s="129" t="s">
+        <v>188</v>
       </c>
       <c r="F16" s="51"/>
       <c r="G16" s="94"/>
@@ -9362,22 +9429,22 @@
         <v>2</v>
       </c>
       <c r="K16" s="56">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L16" s="54">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M16" s="55">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N16" s="56">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O16" s="54">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P16" s="54">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -9439,8 +9506,8 @@
       <c r="D18" s="110" t="s">
         <v>229</v>
       </c>
-      <c r="E18" s="148" t="s">
-        <v>188</v>
+      <c r="E18" s="128" t="s">
+        <v>25</v>
       </c>
       <c r="F18" s="127" t="s">
         <v>241</v>
@@ -9537,8 +9604,8 @@
       <c r="D20" s="127" t="s">
         <v>187</v>
       </c>
-      <c r="E20" s="128" t="s">
-        <v>25</v>
+      <c r="E20" s="129" t="s">
+        <v>188</v>
       </c>
       <c r="F20" s="44"/>
       <c r="G20" s="123"/>
@@ -9893,7 +9960,7 @@
       </c>
       <c r="R27">
         <f>SUM(R3)</f>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="S27" t="s">
         <v>247</v>
@@ -9946,7 +10013,7 @@
       </c>
       <c r="R28">
         <f>SUM(R10)</f>
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="S28" t="s">
         <v>246</v>
@@ -10378,27 +10445,27 @@
       </c>
       <c r="E6" s="10">
         <f>SUM('Sprint 2'!K3:K37)</f>
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F6" s="15">
         <f>SUM('Sprint 2'!L3:L37)</f>
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G6" s="28">
         <f>SUM('Sprint 2'!M3:M37)</f>
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H6" s="10">
         <f>SUM('Sprint 2'!N3:N37)</f>
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="I6" s="15">
         <f>SUM('Sprint 2'!O3:O37)</f>
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="J6" s="28">
         <f>SUM('Sprint 2'!P3:P37)</f>
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Updated sprint 2 doc again
</commit_message>
<xml_diff>
--- a/PayBack - CEN3031 Scrum.xlsx
+++ b/PayBack - CEN3031 Scrum.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Orr\Documents\GitHub\PayBack\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="390" yWindow="615" windowWidth="11295" windowHeight="7455" tabRatio="885" activeTab="4"/>
+    <workbookView xWindow="390" yWindow="620" windowWidth="11300" windowHeight="7460" tabRatio="885" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="User Stories" sheetId="1" r:id="rId1"/>
@@ -14,7 +19,7 @@
     <sheet name="Sprint 2" sheetId="6" r:id="rId5"/>
     <sheet name="Sprint 2 Burndown" sheetId="7" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -24,7 +29,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="V1" authorId="0">
+    <comment ref="V1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -47,7 +52,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -70,7 +75,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="B2" authorId="0">
+    <comment ref="B2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -86,7 +91,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C2" authorId="0">
+    <comment ref="C2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -99,7 +104,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D2" authorId="0">
+    <comment ref="D2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -112,7 +117,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E2" authorId="0">
+    <comment ref="E2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -135,7 +140,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="B2" authorId="0">
+    <comment ref="B2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -151,7 +156,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C2" authorId="0">
+    <comment ref="C2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -164,7 +169,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D2" authorId="0">
+    <comment ref="D2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -177,7 +182,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E2" authorId="0">
+    <comment ref="E2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -948,11 +953,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="57" x14ac:knownFonts="1">
+  <fonts count="58" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1321,7 +1333,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="44">
+  <fills count="45">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1577,6 +1589,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1904,447 +1922,450 @@
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="148">
+  <cellXfs count="149">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="17" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="18" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="25" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="26" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="16" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="16" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="20" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="20" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="48" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="49" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="51" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="52" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="52" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="53" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="54" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="40" borderId="0" xfId="4" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="40" borderId="0" xfId="4" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="38" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="38" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="37" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="37" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="40" borderId="0" xfId="4" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="38" borderId="0" xfId="2" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="37" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="40" borderId="0" xfId="4" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="40" borderId="0" xfId="4" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="38" borderId="0" xfId="2" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="37" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="40" borderId="0" xfId="4" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="38" borderId="0" xfId="2" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="38" borderId="0" xfId="2" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="38" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="38" borderId="0" xfId="2" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="38" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="38" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="41" borderId="0" xfId="5" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="41" borderId="0" xfId="5" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="41" borderId="0" xfId="5" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="41" borderId="0" xfId="5" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="41" borderId="0" xfId="5" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="41" borderId="0" xfId="5" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="37" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="37" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="37" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="37" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="37" borderId="11" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="37" borderId="11" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="37" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="37" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="41" borderId="0" xfId="5" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="41" borderId="0" xfId="5" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="41" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="41" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="41" borderId="17" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="41" borderId="17" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="41" borderId="23" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="41" borderId="23" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="38" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="38" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="38" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="38" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="38" borderId="11" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="38" borderId="11" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="38" borderId="9" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="38" borderId="9" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="39" borderId="0" xfId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="39" borderId="0" xfId="3" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="39" borderId="11" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="39" borderId="11" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="39" borderId="9" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="39" borderId="9" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="42" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="42" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="39" borderId="0" xfId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="39" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="37" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="38" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="37" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="38" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="39" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="39" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="41" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="41" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="37" fillId="20" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="53" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="12" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="41" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="36" fillId="20" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="39" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="41" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="43" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="38" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="37" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="37" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="41" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="38" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="52" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="39" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="41" borderId="0" xfId="5" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="11" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="48" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="25" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="41" borderId="17" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="41" borderId="23" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="41" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="41" borderId="11" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="41" borderId="9" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="41" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="38" borderId="11" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="38" borderId="9" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="38" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="37" borderId="11" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="37" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="37" borderId="17" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="37" borderId="23" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="39" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="39" borderId="11" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="39" borderId="9" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="37" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="41" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="38" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="37" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="39" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="18" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="41" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="39" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="3" fontId="18" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="41" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="43" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="38" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="37" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="37" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="41" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="38" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="39" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="41" borderId="0" xfId="5" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="25" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="41" borderId="17" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="41" borderId="23" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="41" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="41" borderId="11" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="41" borderId="9" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="41" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="38" borderId="11" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="38" borderId="9" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="38" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="37" borderId="11" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="37" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="37" borderId="17" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="37" borderId="23" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="39" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="39" borderId="11" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="39" borderId="9" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="37" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="41" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="38" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="41" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="37" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="38" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="38" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="37" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="57" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="37" borderId="28" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="39" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="17" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="17" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="41" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="41" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="41" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="37" borderId="28" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="37" borderId="23" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="37" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="38" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="38" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="37" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="56" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="37" borderId="28" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="37" borderId="28" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="37" borderId="23" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="37" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="37" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="42" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="42" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="56" fillId="36" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="43" fillId="24" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="36" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="21" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="24" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="46" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="27" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="19" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="15" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="17" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="44" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="21" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="27" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="19" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="15" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="17" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -2406,6 +2427,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2631,11 +2653,11 @@
             </a:ln>
           </c:spPr>
         </c:dropLines>
-        <c:axId val="61224064"/>
-        <c:axId val="70764032"/>
+        <c:axId val="205944592"/>
+        <c:axId val="205941848"/>
       </c:areaChart>
       <c:dateAx>
-        <c:axId val="61224064"/>
+        <c:axId val="205944592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2669,20 +2691,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="low"/>
-        <c:crossAx val="70764032"/>
+        <c:crossAx val="205941848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="70764032"/>
+        <c:axId val="205941848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2705,6 +2728,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -2726,13 +2750,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="61224064"/>
+        <c:crossAx val="205944592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2798,6 +2823,23 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1500" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -2959,7 +3001,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>22</c:v>
@@ -3154,13 +3196,13 @@
                   <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>50</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>50</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>50</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3284,11 +3326,11 @@
             </a:ln>
           </c:spPr>
         </c:dropLines>
-        <c:axId val="81426304"/>
-        <c:axId val="81453056"/>
+        <c:axId val="205944984"/>
+        <c:axId val="205942632"/>
       </c:areaChart>
       <c:dateAx>
-        <c:axId val="81426304"/>
+        <c:axId val="205944984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3329,14 +3371,14 @@
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="low"/>
-        <c:crossAx val="81453056"/>
+        <c:crossAx val="205942632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="81453056"/>
+        <c:axId val="205942632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3381,7 +3423,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="81426304"/>
+        <c:crossAx val="205944984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4251,7 +4293,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4286,7 +4328,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4502,16 +4544,16 @@
       <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="17.1796875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.7265625" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" customWidth="1"/>
-    <col min="4" max="4" width="60.7109375" customWidth="1"/>
-    <col min="5" max="5" width="60.85546875" customWidth="1"/>
+    <col min="3" max="3" width="20.26953125" customWidth="1"/>
+    <col min="4" max="4" width="60.7265625" customWidth="1"/>
+    <col min="5" max="5" width="60.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="130" t="s">
         <v>0</v>
       </c>
@@ -4520,7 +4562,7 @@
       <c r="D1" s="130"/>
       <c r="E1" s="130"/>
     </row>
-    <row r="2" spans="1:22" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -4538,7 +4580,7 @@
       </c>
       <c r="F2" s="37"/>
     </row>
-    <row r="3" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="32" t="s">
         <v>30</v>
       </c>
@@ -4556,7 +4598,7 @@
       </c>
       <c r="F3" s="37"/>
     </row>
-    <row r="4" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="29" t="s">
         <v>30</v>
       </c>
@@ -4574,7 +4616,7 @@
       </c>
       <c r="F4" s="37"/>
     </row>
-    <row r="5" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="29" t="s">
         <v>30</v>
       </c>
@@ -4592,7 +4634,7 @@
       </c>
       <c r="F5" s="37"/>
     </row>
-    <row r="6" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="32" t="s">
         <v>30</v>
       </c>
@@ -4610,7 +4652,7 @@
       </c>
       <c r="F6" s="65"/>
     </row>
-    <row r="7" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="32" t="s">
         <v>30</v>
       </c>
@@ -4628,7 +4670,7 @@
       </c>
       <c r="F7" s="37"/>
     </row>
-    <row r="8" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="32" t="s">
         <v>30</v>
       </c>
@@ -4646,7 +4688,7 @@
       </c>
       <c r="F8" s="37"/>
     </row>
-    <row r="9" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="32" t="s">
         <v>30</v>
       </c>
@@ -4664,7 +4706,7 @@
       </c>
       <c r="F9" s="37"/>
     </row>
-    <row r="10" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="32" t="s">
         <v>30</v>
       </c>
@@ -4682,7 +4724,7 @@
       </c>
       <c r="F10" s="37"/>
     </row>
-    <row r="11" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="32" t="s">
         <v>30</v>
       </c>
@@ -4700,7 +4742,7 @@
       </c>
       <c r="F11" s="37"/>
     </row>
-    <row r="12" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="29" t="s">
         <v>30</v>
       </c>
@@ -4718,7 +4760,7 @@
       </c>
       <c r="F12" s="37"/>
     </row>
-    <row r="13" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="33" t="s">
         <v>49</v>
       </c>
@@ -4736,7 +4778,7 @@
       </c>
       <c r="F13" s="37"/>
     </row>
-    <row r="14" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="33" t="s">
         <v>49</v>
       </c>
@@ -4754,7 +4796,7 @@
       </c>
       <c r="F14" s="37"/>
     </row>
-    <row r="15" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="30" t="s">
         <v>49</v>
       </c>
@@ -4772,7 +4814,7 @@
       </c>
       <c r="F15" s="37"/>
     </row>
-    <row r="16" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="30" t="s">
         <v>49</v>
       </c>
@@ -4790,7 +4832,7 @@
       </c>
       <c r="F16" s="37"/>
     </row>
-    <row r="17" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="33" t="s">
         <v>49</v>
       </c>
@@ -4808,7 +4850,7 @@
       </c>
       <c r="F17" s="37"/>
     </row>
-    <row r="18" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="33" t="s">
         <v>49</v>
       </c>
@@ -4826,7 +4868,7 @@
       </c>
       <c r="F18" s="37"/>
     </row>
-    <row r="19" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="33" t="s">
         <v>49</v>
       </c>
@@ -4844,7 +4886,7 @@
       </c>
       <c r="F19" s="37"/>
     </row>
-    <row r="20" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="33" t="s">
         <v>49</v>
       </c>
@@ -4862,7 +4904,7 @@
       </c>
       <c r="F20" s="37"/>
     </row>
-    <row r="21" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="33" t="s">
         <v>49</v>
       </c>
@@ -4880,7 +4922,7 @@
       </c>
       <c r="F21" s="37"/>
     </row>
-    <row r="22" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="33" t="s">
         <v>49</v>
       </c>
@@ -4898,7 +4940,7 @@
       </c>
       <c r="F22" s="37"/>
     </row>
-    <row r="23" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="33" t="s">
         <v>49</v>
       </c>
@@ -4916,7 +4958,7 @@
       </c>
       <c r="F23" s="37"/>
     </row>
-    <row r="24" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="33" t="s">
         <v>49</v>
       </c>
@@ -4934,7 +4976,7 @@
       </c>
       <c r="F24" s="37"/>
     </row>
-    <row r="25" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="33" t="s">
         <v>49</v>
       </c>
@@ -4952,7 +4994,7 @@
       </c>
       <c r="F25" s="37"/>
     </row>
-    <row r="26" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="33" t="s">
         <v>49</v>
       </c>
@@ -4970,7 +5012,7 @@
       </c>
       <c r="F26" s="37"/>
     </row>
-    <row r="27" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="33" t="s">
         <v>49</v>
       </c>
@@ -4988,7 +5030,7 @@
       </c>
       <c r="F27" s="37"/>
     </row>
-    <row r="28" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="33" t="s">
         <v>49</v>
       </c>
@@ -5006,7 +5048,7 @@
       </c>
       <c r="F28" s="37"/>
     </row>
-    <row r="29" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="30" t="s">
         <v>49</v>
       </c>
@@ -5024,7 +5066,7 @@
       </c>
       <c r="F29" s="37"/>
     </row>
-    <row r="30" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="33" t="s">
         <v>49</v>
       </c>
@@ -5042,7 +5084,7 @@
       </c>
       <c r="F30" s="37"/>
     </row>
-    <row r="31" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="33" t="s">
         <v>49</v>
       </c>
@@ -5060,7 +5102,7 @@
       </c>
       <c r="F31" s="37"/>
     </row>
-    <row r="32" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="33" t="s">
         <v>49</v>
       </c>
@@ -5078,7 +5120,7 @@
       </c>
       <c r="F32" s="37"/>
     </row>
-    <row r="33" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="30" t="s">
         <v>49</v>
       </c>
@@ -5096,7 +5138,7 @@
       </c>
       <c r="F33" s="37"/>
     </row>
-    <row r="34" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="34" t="s">
         <v>92</v>
       </c>
@@ -5113,7 +5155,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="34" t="s">
         <v>92</v>
       </c>
@@ -5130,7 +5172,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="34" t="s">
         <v>92</v>
       </c>
@@ -5147,7 +5189,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="31" t="s">
         <v>92</v>
       </c>
@@ -5164,7 +5206,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="34" t="s">
         <v>92</v>
       </c>
@@ -5181,7 +5223,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="34" t="s">
         <v>92</v>
       </c>
@@ -5198,7 +5240,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="34" t="s">
         <v>92</v>
       </c>
@@ -5215,7 +5257,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="34" t="s">
         <v>92</v>
       </c>
@@ -5232,7 +5274,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="34" t="s">
         <v>92</v>
       </c>
@@ -5249,7 +5291,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="34" t="s">
         <v>92</v>
       </c>
@@ -5266,7 +5308,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="31" t="s">
         <v>92</v>
       </c>
@@ -5283,7 +5325,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="31" t="s">
         <v>92</v>
       </c>
@@ -5300,7 +5342,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="34" t="s">
         <v>92</v>
       </c>
@@ -5317,7 +5359,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="34" t="s">
         <v>92</v>
       </c>
@@ -5334,7 +5376,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="34" t="s">
         <v>92</v>
       </c>
@@ -5351,7 +5393,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="34" t="s">
         <v>92</v>
       </c>
@@ -5368,7 +5410,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="34" t="s">
         <v>92</v>
       </c>
@@ -5385,7 +5427,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="34" t="s">
         <v>92</v>
       </c>
@@ -5402,7 +5444,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="34" t="s">
         <v>92</v>
       </c>
@@ -5419,7 +5461,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="34" t="s">
         <v>92</v>
       </c>
@@ -5436,7 +5478,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="34" t="s">
         <v>92</v>
       </c>
@@ -5472,15 +5514,15 @@
       <selection pane="bottomLeft" activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="17.1796875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" style="20" customWidth="1"/>
-    <col min="2" max="2" width="78.140625" customWidth="1"/>
-    <col min="3" max="3" width="6.42578125" style="20" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" style="20"/>
+    <col min="1" max="1" width="16.7265625" style="20" customWidth="1"/>
+    <col min="2" max="2" width="78.1796875" customWidth="1"/>
+    <col min="3" max="3" width="6.453125" style="20" customWidth="1"/>
+    <col min="4" max="4" width="17.1796875" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="132" t="s">
         <v>11</v>
       </c>
@@ -5488,7 +5530,7 @@
       <c r="C1" s="81"/>
       <c r="D1" s="81"/>
     </row>
-    <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
         <v>1</v>
       </c>
@@ -5502,7 +5544,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="47" t="s">
         <v>30</v>
       </c>
@@ -5519,7 +5561,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="47" t="s">
         <v>30</v>
       </c>
@@ -5536,7 +5578,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="47" t="s">
         <v>30</v>
       </c>
@@ -5553,7 +5595,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="47" t="s">
         <v>30</v>
       </c>
@@ -5570,7 +5612,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="47" t="s">
         <v>30</v>
       </c>
@@ -5587,7 +5629,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="47" t="s">
         <v>30</v>
       </c>
@@ -5604,7 +5646,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="47" t="s">
         <v>30</v>
       </c>
@@ -5621,7 +5663,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="47" t="s">
         <v>30</v>
       </c>
@@ -5638,7 +5680,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="47" t="s">
         <v>30</v>
       </c>
@@ -5655,7 +5697,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="47" t="s">
         <v>30</v>
       </c>
@@ -5669,7 +5711,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="47" t="s">
         <v>30</v>
       </c>
@@ -5686,7 +5728,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="47" t="s">
         <v>30</v>
       </c>
@@ -5703,7 +5745,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="47" t="s">
         <v>30</v>
       </c>
@@ -5720,7 +5762,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="47" t="s">
         <v>30</v>
       </c>
@@ -5737,7 +5779,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="47" t="s">
         <v>30</v>
       </c>
@@ -5754,7 +5796,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="47" t="s">
         <v>30</v>
       </c>
@@ -5771,7 +5813,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="83" t="s">
         <v>30</v>
       </c>
@@ -5785,7 +5827,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="83" t="s">
         <v>30</v>
       </c>
@@ -5799,7 +5841,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="83" t="s">
         <v>30</v>
       </c>
@@ -5813,7 +5855,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="83" t="s">
         <v>30</v>
       </c>
@@ -5827,7 +5869,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="83" t="s">
         <v>30</v>
       </c>
@@ -5841,7 +5883,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="83" t="s">
         <v>30</v>
       </c>
@@ -5855,7 +5897,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="83" t="s">
         <v>30</v>
       </c>
@@ -5869,7 +5911,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="83" t="s">
         <v>30</v>
       </c>
@@ -5883,7 +5925,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="83" t="s">
         <v>30</v>
       </c>
@@ -5897,7 +5939,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="83" t="s">
         <v>30</v>
       </c>
@@ -5911,7 +5953,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="47" t="s">
         <v>30</v>
       </c>
@@ -5925,7 +5967,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="47" t="s">
         <v>30</v>
       </c>
@@ -5939,7 +5981,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="47" t="s">
         <v>30</v>
       </c>
@@ -5953,7 +5995,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="51" t="s">
         <v>49</v>
       </c>
@@ -5967,7 +6009,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="51" t="s">
         <v>49</v>
       </c>
@@ -5981,7 +6023,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="51" t="s">
         <v>49</v>
       </c>
@@ -5995,7 +6037,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="51" t="s">
         <v>49</v>
       </c>
@@ -6009,7 +6051,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="51" t="s">
         <v>49</v>
       </c>
@@ -6023,7 +6065,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="51" t="s">
         <v>49</v>
       </c>
@@ -6037,7 +6079,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="51" t="s">
         <v>49</v>
       </c>
@@ -6051,7 +6093,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="51" t="s">
         <v>49</v>
       </c>
@@ -6065,7 +6107,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="51" t="s">
         <v>49</v>
       </c>
@@ -6079,7 +6121,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="51" t="s">
         <v>49</v>
       </c>
@@ -6093,7 +6135,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="51" t="s">
         <v>49</v>
       </c>
@@ -6107,7 +6149,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="51" t="s">
         <v>49</v>
       </c>
@@ -6121,7 +6163,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="51" t="s">
         <v>49</v>
       </c>
@@ -6135,7 +6177,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="51" t="s">
         <v>49</v>
       </c>
@@ -6149,7 +6191,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="51" t="s">
         <v>49</v>
       </c>
@@ -6163,7 +6205,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="51" t="s">
         <v>49</v>
       </c>
@@ -6177,7 +6219,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="51" t="s">
         <v>49</v>
       </c>
@@ -6191,7 +6233,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="51" t="s">
         <v>49</v>
       </c>
@@ -6205,7 +6247,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="51" t="s">
         <v>49</v>
       </c>
@@ -6219,7 +6261,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="51" t="s">
         <v>49</v>
       </c>
@@ -6233,7 +6275,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="51" t="s">
         <v>49</v>
       </c>
@@ -6247,7 +6289,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="51" t="s">
         <v>49</v>
       </c>
@@ -6261,7 +6303,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="51" t="s">
         <v>49</v>
       </c>
@@ -6275,7 +6317,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="51" t="s">
         <v>49</v>
       </c>
@@ -6289,7 +6331,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="51" t="s">
         <v>49</v>
       </c>
@@ -6303,7 +6345,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="44" t="s">
         <v>92</v>
       </c>
@@ -6317,7 +6359,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="44" t="s">
         <v>92</v>
       </c>
@@ -6331,7 +6373,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="44" t="s">
         <v>92</v>
       </c>
@@ -6345,7 +6387,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="44" t="s">
         <v>92</v>
       </c>
@@ -6362,7 +6404,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="44" t="s">
         <v>92</v>
       </c>
@@ -6379,7 +6421,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="44" t="s">
         <v>92</v>
       </c>
@@ -6396,7 +6438,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="44" t="s">
         <v>92</v>
       </c>
@@ -6410,7 +6452,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="44" t="s">
         <v>92</v>
       </c>
@@ -6427,7 +6469,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="44" t="s">
         <v>92</v>
       </c>
@@ -6441,7 +6483,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="44" t="s">
         <v>92</v>
       </c>
@@ -6458,7 +6500,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" s="44" t="s">
         <v>92</v>
       </c>
@@ -6475,7 +6517,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" s="44" t="s">
         <v>92</v>
       </c>
@@ -6489,7 +6531,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="44" t="s">
         <v>92</v>
       </c>
@@ -6506,7 +6548,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="44" t="s">
         <v>92</v>
       </c>
@@ -6520,7 +6562,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="44" t="s">
         <v>92</v>
       </c>
@@ -6534,7 +6576,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" s="44" t="s">
         <v>92</v>
       </c>
@@ -6548,7 +6590,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="73" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A73" s="44" t="s">
         <v>92</v>
       </c>
@@ -6562,7 +6604,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74" s="44" t="s">
         <v>92</v>
       </c>
@@ -6576,7 +6618,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" s="44" t="s">
         <v>92</v>
       </c>
@@ -6590,7 +6632,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" s="44" t="s">
         <v>92</v>
       </c>
@@ -6604,7 +6646,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="77" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A77" s="44" t="s">
         <v>92</v>
       </c>
@@ -6618,7 +6660,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A78" s="44" t="s">
         <v>92</v>
       </c>
@@ -6632,7 +6674,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="79" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A79" s="44" t="s">
         <v>92</v>
       </c>
@@ -6646,7 +6688,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="80" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A80" s="44" t="s">
         <v>92</v>
       </c>
@@ -6660,7 +6702,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="81" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A81" s="44" t="s">
         <v>92</v>
       </c>
@@ -6674,7 +6716,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="82" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" s="82" t="s">
         <v>210</v>
       </c>
@@ -6691,7 +6733,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="83" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" s="82" t="s">
         <v>210</v>
       </c>
@@ -6708,7 +6750,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="84" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A84" s="82" t="s">
         <v>210</v>
       </c>
@@ -6725,7 +6767,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A85" s="82" t="s">
         <v>210</v>
       </c>
@@ -6739,7 +6781,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="86" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A86" s="82" t="s">
         <v>210</v>
       </c>
@@ -6753,7 +6795,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="87" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A87" s="82" t="s">
         <v>210</v>
       </c>
@@ -6767,29 +6809,29 @@
         <v>8</v>
       </c>
     </row>
-    <row r="88" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C88" s="20">
         <f>SUM(C3:C87)</f>
         <v>327</v>
       </c>
     </row>
-    <row r="89" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="90" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="90" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90"/>
     </row>
-    <row r="91" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91"/>
     </row>
-    <row r="92" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92"/>
     </row>
-    <row r="93" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93"/>
     </row>
-    <row r="94" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94"/>
     </row>
-    <row r="95" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95"/>
     </row>
   </sheetData>
@@ -6830,20 +6872,20 @@
       <selection pane="bottomLeft" activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="17.1796875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="80.85546875" customWidth="1"/>
-    <col min="2" max="2" width="4.140625" style="20" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" style="20" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" style="20" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" style="20" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" style="20" customWidth="1"/>
-    <col min="7" max="7" width="4.85546875" style="20" customWidth="1"/>
-    <col min="8" max="8" width="3.7109375" style="20" customWidth="1"/>
-    <col min="9" max="16" width="3.5703125" style="20" customWidth="1"/>
+    <col min="1" max="1" width="80.81640625" customWidth="1"/>
+    <col min="2" max="2" width="4.1796875" style="20" customWidth="1"/>
+    <col min="3" max="3" width="9.7265625" style="20" customWidth="1"/>
+    <col min="4" max="4" width="14.54296875" style="20" customWidth="1"/>
+    <col min="5" max="5" width="13.81640625" style="20" customWidth="1"/>
+    <col min="6" max="6" width="20.1796875" style="20" customWidth="1"/>
+    <col min="7" max="7" width="4.81640625" style="20" customWidth="1"/>
+    <col min="8" max="8" width="3.7265625" style="20" customWidth="1"/>
+    <col min="9" max="16" width="3.54296875" style="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="26" t="s">
         <v>15</v>
       </c>
@@ -6871,7 +6913,7 @@
       <c r="O1" s="137"/>
       <c r="P1" s="138"/>
     </row>
-    <row r="2" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" ht="26" x14ac:dyDescent="0.3">
       <c r="A2" s="26" t="s">
         <v>17</v>
       </c>
@@ -6921,7 +6963,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="67" t="s">
         <v>194</v>
       </c>
@@ -6967,7 +7009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="40" t="s">
         <v>129</v>
       </c>
@@ -7013,7 +7055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="40" t="s">
         <v>130</v>
       </c>
@@ -7059,7 +7101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="40" t="s">
         <v>137</v>
       </c>
@@ -7105,7 +7147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="40" t="s">
         <v>133</v>
       </c>
@@ -7151,7 +7193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="40" t="s">
         <v>135</v>
       </c>
@@ -7197,7 +7239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="40" t="s">
         <v>134</v>
       </c>
@@ -7243,7 +7285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="41" t="s">
         <v>136</v>
       </c>
@@ -7289,7 +7331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="41" t="s">
         <v>132</v>
       </c>
@@ -7335,7 +7377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="40" t="s">
         <v>131</v>
       </c>
@@ -7381,7 +7423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="40" t="s">
         <v>144</v>
       </c>
@@ -7427,7 +7469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="40" t="s">
         <v>140</v>
       </c>
@@ -7473,7 +7515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="40" t="s">
         <v>141</v>
       </c>
@@ -7519,7 +7561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="40" t="s">
         <v>142</v>
       </c>
@@ -7565,7 +7607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="40" t="s">
         <v>145</v>
       </c>
@@ -7611,7 +7653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="38" t="s">
         <v>146</v>
       </c>
@@ -7658,7 +7700,7 @@
       </c>
       <c r="Q18" s="20"/>
     </row>
-    <row r="19" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="43" t="s">
         <v>168</v>
       </c>
@@ -7705,7 +7747,7 @@
       </c>
       <c r="Q19" s="20"/>
     </row>
-    <row r="20" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="43" t="s">
         <v>169</v>
       </c>
@@ -7752,7 +7794,7 @@
       </c>
       <c r="Q20" s="20"/>
     </row>
-    <row r="21" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="43" t="s">
         <v>170</v>
       </c>
@@ -7798,7 +7840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="43" t="s">
         <v>172</v>
       </c>
@@ -7844,7 +7886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="43" t="s">
         <v>173</v>
       </c>
@@ -7890,7 +7932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="43" t="s">
         <v>174</v>
       </c>
@@ -7936,7 +7978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="77" t="s">
         <v>220</v>
       </c>
@@ -7982,7 +8024,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="77" t="s">
         <v>177</v>
       </c>
@@ -8028,7 +8070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="66" t="s">
         <v>191</v>
       </c>
@@ -8074,7 +8116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="66" t="s">
         <v>193</v>
       </c>
@@ -8120,7 +8162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="57" t="s">
         <v>189</v>
       </c>
@@ -8166,7 +8208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F30" s="104" t="s">
         <v>204</v>
       </c>
@@ -8175,16 +8217,16 @@
         <v>95</v>
       </c>
     </row>
-    <row r="31" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="33" spans="12:16" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="34" spans="12:16" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="35" spans="12:16" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="12:16" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" spans="12:16" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="12:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L35" s="105"/>
       <c r="O35" s="19"/>
       <c r="P35" s="19"/>
     </row>
-    <row r="36" spans="12:16" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="12:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L36" s="105"/>
       <c r="O36" s="19"/>
       <c r="P36" s="19"/>
@@ -8309,12 +8351,12 @@
       <selection pane="bottomLeft" activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="17.1796875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="10" width="9.7109375" customWidth="1"/>
+    <col min="2" max="10" width="9.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="139" t="s">
         <v>26</v>
       </c>
@@ -8328,7 +8370,7 @@
       <c r="I1" s="140"/>
       <c r="J1" s="140"/>
     </row>
-    <row r="2" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
       <c r="B2" s="141"/>
       <c r="C2" s="142"/>
@@ -8340,7 +8382,7 @@
       <c r="I2" s="145"/>
       <c r="J2" s="146"/>
     </row>
-    <row r="3" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>208</v>
       </c>
@@ -8372,7 +8414,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="69">
         <v>41535</v>
@@ -8402,7 +8444,7 @@
         <v>41554</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="25"/>
       <c r="B5" s="114">
         <v>1</v>
@@ -8433,7 +8475,7 @@
       </c>
       <c r="K5" s="10"/>
     </row>
-    <row r="6" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
         <v>27</v>
       </c>
@@ -8475,7 +8517,7 @@
       </c>
       <c r="K6" s="10"/>
     </row>
-    <row r="7" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
         <v>28</v>
       </c>
@@ -8517,10 +8559,10 @@
       </c>
       <c r="K7" s="5"/>
     </row>
-    <row r="8" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="15" t="s">
         <v>29</v>
       </c>
@@ -8530,7 +8572,7 @@
       <c r="F11" s="15"/>
       <c r="G11" s="15"/>
     </row>
-    <row r="12" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="15"/>
       <c r="C12" s="15"/>
       <c r="D12" s="15"/>
@@ -8538,7 +8580,7 @@
       <c r="F12" s="15"/>
       <c r="G12" s="15"/>
     </row>
-    <row r="13" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="15"/>
       <c r="C13" s="15"/>
       <c r="D13" s="15"/>
@@ -8546,7 +8588,7 @@
       <c r="F13" s="15"/>
       <c r="G13" s="15"/>
     </row>
-    <row r="14" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="15"/>
       <c r="C14" s="15"/>
       <c r="D14" s="15"/>
@@ -8554,7 +8596,7 @@
       <c r="F14" s="15"/>
       <c r="G14" s="15"/>
     </row>
-    <row r="15" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
@@ -8562,7 +8604,7 @@
       <c r="F15" s="15"/>
       <c r="G15" s="15"/>
     </row>
-    <row r="16" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="15"/>
       <c r="C16" s="15"/>
       <c r="D16" s="15"/>
@@ -8570,7 +8612,7 @@
       <c r="F16" s="15"/>
       <c r="G16" s="15"/>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:7" ht="13" x14ac:dyDescent="0.25">
       <c r="B17" s="15"/>
       <c r="C17" s="15"/>
       <c r="D17" s="15"/>
@@ -8578,7 +8620,7 @@
       <c r="F17" s="15"/>
       <c r="G17" s="15"/>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:7" ht="13" x14ac:dyDescent="0.25">
       <c r="B18" s="15"/>
       <c r="C18" s="15"/>
       <c r="D18" s="15"/>
@@ -8586,7 +8628,7 @@
       <c r="F18" s="15"/>
       <c r="G18" s="15"/>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:7" ht="13" x14ac:dyDescent="0.25">
       <c r="B19" s="15"/>
       <c r="C19" s="15"/>
       <c r="D19" s="15"/>
@@ -8594,7 +8636,7 @@
       <c r="F19" s="15"/>
       <c r="G19" s="15"/>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:7" ht="13" x14ac:dyDescent="0.25">
       <c r="B20" s="15"/>
       <c r="C20" s="15"/>
       <c r="D20" s="15"/>
@@ -8602,7 +8644,7 @@
       <c r="F20" s="15"/>
       <c r="G20" s="15"/>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:7" ht="13" x14ac:dyDescent="0.25">
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>
       <c r="D21" s="15"/>
@@ -8610,7 +8652,7 @@
       <c r="F21" s="15"/>
       <c r="G21" s="15"/>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:7" ht="13" x14ac:dyDescent="0.25">
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
       <c r="D22" s="15"/>
@@ -8618,7 +8660,7 @@
       <c r="F22" s="15"/>
       <c r="G22" s="15"/>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:7" ht="13" x14ac:dyDescent="0.25">
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
       <c r="D23" s="15"/>
@@ -8626,7 +8668,7 @@
       <c r="F23" s="15"/>
       <c r="G23" s="15"/>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:7" ht="13" x14ac:dyDescent="0.25">
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
       <c r="D24" s="15"/>
@@ -8634,7 +8676,7 @@
       <c r="F24" s="15"/>
       <c r="G24" s="15"/>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:7" ht="13" x14ac:dyDescent="0.25">
       <c r="B25" s="15"/>
       <c r="C25" s="15"/>
       <c r="D25" s="15"/>
@@ -8642,7 +8684,7 @@
       <c r="F25" s="15"/>
       <c r="G25" s="15"/>
     </row>
-    <row r="26" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="15"/>
       <c r="C26" s="15"/>
       <c r="D26" s="15"/>
@@ -8650,7 +8692,7 @@
       <c r="F26" s="15"/>
       <c r="G26" s="15"/>
     </row>
-    <row r="27" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="15"/>
       <c r="C27" s="15"/>
       <c r="D27" s="15"/>
@@ -8658,7 +8700,7 @@
       <c r="F27" s="15"/>
       <c r="G27" s="15"/>
     </row>
-    <row r="28" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="15"/>
       <c r="C28" s="15"/>
       <c r="D28" s="15"/>
@@ -8666,7 +8708,7 @@
       <c r="F28" s="15"/>
       <c r="G28" s="15"/>
     </row>
-    <row r="29" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="15"/>
       <c r="C29" s="15"/>
       <c r="D29" s="15"/>
@@ -8692,32 +8734,32 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q21" sqref="Q21"/>
+      <selection pane="bottomLeft" activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="17.1796875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="90.140625" customWidth="1"/>
-    <col min="2" max="2" width="4.85546875" style="20" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" style="20" customWidth="1"/>
+    <col min="1" max="1" width="90.1796875" customWidth="1"/>
+    <col min="2" max="2" width="4.81640625" style="20" customWidth="1"/>
+    <col min="3" max="3" width="9.7265625" style="20" customWidth="1"/>
     <col min="4" max="4" width="21" style="20" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" style="20" customWidth="1"/>
-    <col min="6" max="6" width="25.85546875" style="20" customWidth="1"/>
-    <col min="7" max="7" width="5.28515625" style="20" customWidth="1"/>
-    <col min="8" max="8" width="4.5703125" customWidth="1"/>
-    <col min="9" max="9" width="3.5703125" customWidth="1"/>
-    <col min="10" max="10" width="4.140625" customWidth="1"/>
-    <col min="11" max="11" width="3.5703125" customWidth="1"/>
-    <col min="12" max="13" width="4.7109375" customWidth="1"/>
-    <col min="14" max="14" width="3.5703125" customWidth="1"/>
-    <col min="15" max="15" width="4.5703125" customWidth="1"/>
-    <col min="16" max="16" width="4.7109375" customWidth="1"/>
-    <col min="18" max="18" width="5.7109375" customWidth="1"/>
-    <col min="19" max="19" width="31.140625" customWidth="1"/>
-    <col min="20" max="26" width="5.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.81640625" style="20" customWidth="1"/>
+    <col min="6" max="6" width="25.81640625" style="20" customWidth="1"/>
+    <col min="7" max="7" width="5.26953125" style="20" customWidth="1"/>
+    <col min="8" max="8" width="4.54296875" customWidth="1"/>
+    <col min="9" max="9" width="3.54296875" customWidth="1"/>
+    <col min="10" max="10" width="4.1796875" customWidth="1"/>
+    <col min="11" max="11" width="3.54296875" customWidth="1"/>
+    <col min="12" max="13" width="4.7265625" customWidth="1"/>
+    <col min="14" max="14" width="3.54296875" customWidth="1"/>
+    <col min="15" max="15" width="4.54296875" customWidth="1"/>
+    <col min="16" max="16" width="4.7265625" customWidth="1"/>
+    <col min="18" max="18" width="5.7265625" customWidth="1"/>
+    <col min="19" max="19" width="31.1796875" customWidth="1"/>
+    <col min="20" max="26" width="5.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="122" t="s">
         <v>226</v>
       </c>
@@ -8745,7 +8787,7 @@
       <c r="O1" s="137"/>
       <c r="P1" s="138"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="26" t="s">
         <v>17</v>
       </c>
@@ -8795,7 +8837,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="68" t="s">
         <v>199</v>
       </c>
@@ -8808,8 +8850,8 @@
       <c r="D3" s="108" t="s">
         <v>230</v>
       </c>
-      <c r="E3" s="52" t="s">
-        <v>25</v>
+      <c r="E3" s="148" t="s">
+        <v>188</v>
       </c>
       <c r="F3" s="47"/>
       <c r="G3" s="88"/>
@@ -8832,20 +8874,20 @@
         <v>2</v>
       </c>
       <c r="N3" s="50">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O3" s="48">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P3" s="48">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R3">
         <f>SUM(P3:P9)</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="68" t="s">
         <v>196</v>
       </c>
@@ -8891,7 +8933,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="118" t="s">
         <v>233</v>
       </c>
@@ -8937,7 +8979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="68" t="s">
         <v>202</v>
       </c>
@@ -8983,7 +9025,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="40" t="s">
         <v>143</v>
       </c>
@@ -9029,7 +9071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="74" t="s">
         <v>138</v>
       </c>
@@ -9075,7 +9117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="116" t="s">
         <v>232</v>
       </c>
@@ -9121,7 +9163,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="76" t="s">
         <v>217</v>
       </c>
@@ -9171,7 +9213,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="120" t="s">
         <v>235</v>
       </c>
@@ -9217,7 +9259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="76" t="s">
         <v>215</v>
       </c>
@@ -9263,7 +9305,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="76" t="s">
         <v>219</v>
       </c>
@@ -9309,7 +9351,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="38" t="s">
         <v>153</v>
       </c>
@@ -9355,7 +9397,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="38" t="s">
         <v>156</v>
       </c>
@@ -9401,7 +9443,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="38" t="s">
         <v>146</v>
       </c>
@@ -9447,7 +9489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="38" t="s">
         <v>147</v>
       </c>
@@ -9493,7 +9535,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="119" t="s">
         <v>234</v>
       </c>
@@ -9545,7 +9587,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="126" t="s">
         <v>236</v>
       </c>
@@ -9591,7 +9633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="126" t="s">
         <v>239</v>
       </c>
@@ -9637,7 +9679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="126" t="s">
         <v>240</v>
       </c>
@@ -9683,7 +9725,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="126" t="s">
         <v>244</v>
       </c>
@@ -9729,7 +9771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="126" t="s">
         <v>242</v>
       </c>
@@ -9775,7 +9817,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="126" t="s">
         <v>243</v>
       </c>
@@ -9821,7 +9863,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="43" t="s">
         <v>178</v>
       </c>
@@ -9867,7 +9909,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="43" t="s">
         <v>222</v>
       </c>
@@ -9913,7 +9955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="43" t="s">
         <v>223</v>
       </c>
@@ -9960,13 +10002,13 @@
       </c>
       <c r="R27">
         <f>SUM(R3)</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="S27" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="28" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="43" t="s">
         <v>175</v>
       </c>
@@ -10019,7 +10061,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="29" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="77" t="s">
         <v>176</v>
       </c>
@@ -10072,7 +10114,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="30" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="73" t="s">
         <v>211</v>
       </c>
@@ -10125,7 +10167,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="31" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F31" s="104" t="s">
         <v>204</v>
       </c>
@@ -10138,16 +10180,16 @@
         <v>103</v>
       </c>
     </row>
-    <row r="32" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="33" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="34" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="35" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="36" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="37" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="38" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="39" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="40" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="41" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="H1:J1"/>
@@ -10296,12 +10338,12 @@
       <selection pane="bottomLeft" activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="17.1796875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="10" width="9.7109375" customWidth="1"/>
+    <col min="2" max="10" width="9.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="147" t="s">
         <v>227</v>
       </c>
@@ -10315,7 +10357,7 @@
       <c r="I1" s="140"/>
       <c r="J1" s="140"/>
     </row>
-    <row r="2" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
       <c r="B2" s="141"/>
       <c r="C2" s="142"/>
@@ -10327,7 +10369,7 @@
       <c r="I2" s="145"/>
       <c r="J2" s="146"/>
     </row>
-    <row r="3" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>208</v>
       </c>
@@ -10359,7 +10401,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="69">
         <v>41556</v>
@@ -10389,7 +10431,7 @@
         <v>41575</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="25"/>
       <c r="B5" s="22">
         <v>1</v>
@@ -10427,7 +10469,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
         <v>27</v>
       </c>
@@ -10457,18 +10499,18 @@
       </c>
       <c r="H6" s="10">
         <f>SUM('Sprint 2'!N3:N37)</f>
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I6" s="15">
         <f>SUM('Sprint 2'!O3:O37)</f>
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J6" s="28">
         <f>SUM('Sprint 2'!P3:P37)</f>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
         <v>28</v>
       </c>
@@ -10509,10 +10551,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="15" t="s">
         <v>29</v>
       </c>
@@ -10522,7 +10564,7 @@
       <c r="F11" s="15"/>
       <c r="G11" s="15"/>
     </row>
-    <row r="12" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="15"/>
       <c r="C12" s="15"/>
       <c r="D12" s="15"/>
@@ -10530,7 +10572,7 @@
       <c r="F12" s="15"/>
       <c r="G12" s="15"/>
     </row>
-    <row r="13" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="15"/>
       <c r="C13" s="15"/>
       <c r="D13" s="15"/>
@@ -10538,7 +10580,7 @@
       <c r="F13" s="15"/>
       <c r="G13" s="15"/>
     </row>
-    <row r="14" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="15"/>
       <c r="C14" s="15"/>
       <c r="D14" s="15"/>
@@ -10546,7 +10588,7 @@
       <c r="F14" s="15"/>
       <c r="G14" s="15"/>
     </row>
-    <row r="15" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
@@ -10554,7 +10596,7 @@
       <c r="F15" s="15"/>
       <c r="G15" s="15"/>
     </row>
-    <row r="16" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="15"/>
       <c r="C16" s="15"/>
       <c r="D16" s="15"/>
@@ -10562,7 +10604,7 @@
       <c r="F16" s="15"/>
       <c r="G16" s="15"/>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:7" ht="13" x14ac:dyDescent="0.25">
       <c r="B17" s="15"/>
       <c r="C17" s="15"/>
       <c r="D17" s="15"/>
@@ -10570,7 +10612,7 @@
       <c r="F17" s="15"/>
       <c r="G17" s="15"/>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:7" ht="13" x14ac:dyDescent="0.25">
       <c r="B18" s="15"/>
       <c r="C18" s="15"/>
       <c r="D18" s="15"/>
@@ -10578,7 +10620,7 @@
       <c r="F18" s="15"/>
       <c r="G18" s="15"/>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:7" ht="13" x14ac:dyDescent="0.25">
       <c r="B19" s="15"/>
       <c r="C19" s="15"/>
       <c r="D19" s="15"/>
@@ -10586,7 +10628,7 @@
       <c r="F19" s="15"/>
       <c r="G19" s="15"/>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:7" ht="13" x14ac:dyDescent="0.25">
       <c r="B20" s="15"/>
       <c r="C20" s="15"/>
       <c r="D20" s="15"/>
@@ -10594,7 +10636,7 @@
       <c r="F20" s="15"/>
       <c r="G20" s="15"/>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:7" ht="13" x14ac:dyDescent="0.25">
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>
       <c r="D21" s="15"/>
@@ -10602,7 +10644,7 @@
       <c r="F21" s="15"/>
       <c r="G21" s="15"/>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:7" ht="13" x14ac:dyDescent="0.25">
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
       <c r="D22" s="15"/>
@@ -10610,7 +10652,7 @@
       <c r="F22" s="15"/>
       <c r="G22" s="15"/>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:7" ht="13" x14ac:dyDescent="0.25">
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
       <c r="D23" s="15"/>
@@ -10618,7 +10660,7 @@
       <c r="F23" s="15"/>
       <c r="G23" s="15"/>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:7" ht="13" x14ac:dyDescent="0.25">
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
       <c r="D24" s="15"/>
@@ -10626,7 +10668,7 @@
       <c r="F24" s="15"/>
       <c r="G24" s="15"/>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:7" ht="13" x14ac:dyDescent="0.25">
       <c r="B25" s="15"/>
       <c r="C25" s="15"/>
       <c r="D25" s="15"/>
@@ -10634,7 +10676,7 @@
       <c r="F25" s="15"/>
       <c r="G25" s="15"/>
     </row>
-    <row r="26" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="15"/>
       <c r="C26" s="15"/>
       <c r="D26" s="15"/>
@@ -10642,7 +10684,7 @@
       <c r="F26" s="15"/>
       <c r="G26" s="15"/>
     </row>
-    <row r="27" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="15"/>
       <c r="C27" s="15"/>
       <c r="D27" s="15"/>
@@ -10650,7 +10692,7 @@
       <c r="F27" s="15"/>
       <c r="G27" s="15"/>
     </row>
-    <row r="28" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="15"/>
       <c r="C28" s="15"/>
       <c r="D28" s="15"/>
@@ -10658,7 +10700,7 @@
       <c r="F28" s="15"/>
       <c r="G28" s="15"/>
     </row>
-    <row r="29" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="15"/>
       <c r="C29" s="15"/>
       <c r="D29" s="15"/>

</xml_diff>

<commit_message>
Updated Scrum Doc 	modified:   PayBack - CEN3031 Scrum.xlsx
</commit_message>
<xml_diff>
--- a/PayBack - CEN3031 Scrum.xlsx
+++ b/PayBack - CEN3031 Scrum.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="615" windowWidth="11295" windowHeight="7455" tabRatio="885" activeTab="4"/>
+    <workbookView xWindow="390" yWindow="615" windowWidth="11295" windowHeight="7455" tabRatio="885" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="User Stories" sheetId="1" r:id="rId1"/>
@@ -195,7 +195,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="848" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="872" uniqueCount="252">
   <si>
     <t>User Stories</t>
   </si>
@@ -848,9 +848,6 @@
     <t>Provide method for authentication of logins/accounts</t>
   </si>
   <si>
-    <t>Create intents for transaction parameters through Transaction pages 1 - 5</t>
-  </si>
-  <si>
     <t>Provide method for pushing transaction object to database.</t>
   </si>
   <si>
@@ -899,9 +896,6 @@
     <t>Create "add contact" page sequence</t>
   </si>
   <si>
-    <t>Communication between android/database</t>
-  </si>
-  <si>
     <t>Edit code for android 2.3.3</t>
   </si>
   <si>
@@ -920,9 +914,6 @@
     <t>Install Apache and PHP on Desktop</t>
   </si>
   <si>
-    <t>This is a category header</t>
-  </si>
-  <si>
     <t>PHP server code for account creation</t>
   </si>
   <si>
@@ -942,17 +933,42 @@
   </si>
   <si>
     <t>Report</t>
+  </si>
+  <si>
+    <t>Create transaction page 2 + 4 (Contact selection / borrower's share)</t>
+  </si>
+  <si>
+    <t>Create transaction page 3 ( Lender's share) debt division selection</t>
+  </si>
+  <si>
+    <t>Create transaction page 5 ( Summary)</t>
+  </si>
+  <si>
+    <t>Create transaction page 1 (Information gather)</t>
+  </si>
+  <si>
+    <t>Capture Adding friend by email address</t>
+  </si>
+  <si>
+    <t>Will</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="57" x14ac:knownFonts="1">
+  <fonts count="58" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1904,447 +1920,450 @@
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="148">
+  <cellXfs count="149">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="17" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="18" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="25" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="26" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="16" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="16" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="20" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="20" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="48" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="49" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="51" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="52" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="52" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="53" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="54" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="40" borderId="0" xfId="4" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="40" borderId="0" xfId="4" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="38" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="38" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="37" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="37" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="40" borderId="0" xfId="4" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="38" borderId="0" xfId="2" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="37" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="40" borderId="0" xfId="4" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="40" borderId="0" xfId="4" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="38" borderId="0" xfId="2" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="37" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="40" borderId="0" xfId="4" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="38" borderId="0" xfId="2" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="38" borderId="0" xfId="2" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="38" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="38" borderId="0" xfId="2" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="38" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="38" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="41" borderId="0" xfId="5" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="41" borderId="0" xfId="5" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="41" borderId="0" xfId="5" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="41" borderId="0" xfId="5" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="41" borderId="0" xfId="5" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="41" borderId="0" xfId="5" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="37" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="37" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="37" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="37" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="37" borderId="11" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="37" borderId="11" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="37" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="37" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="41" borderId="0" xfId="5" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="41" borderId="0" xfId="5" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="41" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="41" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="41" borderId="17" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="41" borderId="17" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="41" borderId="23" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="41" borderId="23" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="38" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="38" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="38" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="38" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="38" borderId="11" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="38" borderId="11" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="38" borderId="9" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="38" borderId="9" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="39" borderId="0" xfId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="39" borderId="0" xfId="3" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="39" borderId="11" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="39" borderId="11" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="39" borderId="9" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="39" borderId="9" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="42" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="42" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="39" borderId="0" xfId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="39" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="37" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="38" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="37" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="38" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="39" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="39" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="41" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="41" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="37" fillId="20" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="53" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="12" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="41" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="36" fillId="20" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="39" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="41" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="43" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="38" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="37" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="37" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="41" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="38" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="52" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="39" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="41" borderId="0" xfId="5" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="11" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="48" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="25" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="41" borderId="17" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="41" borderId="23" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="41" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="41" borderId="11" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="41" borderId="9" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="41" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="38" borderId="11" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="38" borderId="9" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="38" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="37" borderId="11" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="37" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="37" borderId="17" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="37" borderId="23" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="39" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="39" borderId="11" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="39" borderId="9" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="37" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="41" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="38" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="37" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="39" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="18" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="41" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="39" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="3" fontId="18" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="41" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="43" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="38" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="37" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="37" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="41" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="38" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="39" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="41" borderId="0" xfId="5" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="25" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="41" borderId="17" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="41" borderId="23" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="41" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="41" borderId="11" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="41" borderId="9" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="41" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="38" borderId="11" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="38" borderId="9" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="38" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="37" borderId="11" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="37" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="37" borderId="17" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="37" borderId="23" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="39" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="39" borderId="11" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="39" borderId="9" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="37" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="41" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="38" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="41" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="38" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="38" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="37" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="57" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="37" borderId="28" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="39" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="17" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="17" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="41" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="41" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="41" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="37" borderId="28" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="37" borderId="23" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="37" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="38" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="38" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="37" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="56" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="42" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="56" fillId="36" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="24" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="21" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="27" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="19" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="15" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="17" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="38" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="37" borderId="28" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="38" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="37" borderId="28" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="37" borderId="23" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="37" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="37" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="42" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="36" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="24" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="21" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="27" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="19" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="15" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="17" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -2962,7 +2981,7 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>22</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>16</c:v>
@@ -3136,31 +3155,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>103</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>98</c:v>
+                  <c:v>110</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>87</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>82</c:v>
+                  <c:v>86</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>64</c:v>
+                  <c:v>74</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>57</c:v>
+                  <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>50</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>50</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>50</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3235,28 +3254,28 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>103</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>90.125</c:v>
+                  <c:v>100.625</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>77.25</c:v>
+                  <c:v>86.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>64.375</c:v>
+                  <c:v>71.875</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>51.5</c:v>
+                  <c:v>57.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>38.625</c:v>
+                  <c:v>43.125</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>25.75</c:v>
+                  <c:v>28.75</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>12.875</c:v>
+                  <c:v>14.375</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -4512,13 +4531,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="130" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="131"/>
-      <c r="C1" s="130"/>
-      <c r="D1" s="130"/>
-      <c r="E1" s="130"/>
+      <c r="A1" s="129" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="130"/>
+      <c r="C1" s="129"/>
+      <c r="D1" s="129"/>
+      <c r="E1" s="129"/>
     </row>
     <row r="2" spans="1:22" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
@@ -5465,11 +5484,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E95"/>
+  <dimension ref="A1:E98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G41" sqref="G41"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5481,10 +5500,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="132" t="s">
+      <c r="A1" s="131" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="132"/>
+      <c r="B1" s="131"/>
       <c r="C1" s="81"/>
       <c r="D1" s="81"/>
     </row>
@@ -5668,6 +5687,9 @@
       <c r="D12" s="47" t="s">
         <v>9</v>
       </c>
+      <c r="E12" s="61" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="13" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="47" t="s">
@@ -5804,7 +5826,7 @@
         <v>30</v>
       </c>
       <c r="B21" s="118" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C21" s="47">
         <v>4</v>
@@ -5944,7 +5966,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="116" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C31" s="47">
         <v>4</v>
@@ -5972,13 +5994,13 @@
         <v>49</v>
       </c>
       <c r="B33" s="38" t="s">
-        <v>147</v>
+        <v>250</v>
       </c>
       <c r="C33" s="51">
         <v>2</v>
       </c>
       <c r="D33" s="51" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5986,13 +6008,13 @@
         <v>49</v>
       </c>
       <c r="B34" s="38" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C34" s="51">
         <v>2</v>
       </c>
       <c r="D34" s="51" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6000,10 +6022,10 @@
         <v>49</v>
       </c>
       <c r="B35" s="38" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C35" s="51">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D35" s="51" t="s">
         <v>6</v>
@@ -6014,13 +6036,13 @@
         <v>49</v>
       </c>
       <c r="B36" s="38" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C36" s="51">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D36" s="51" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6028,10 +6050,10 @@
         <v>49</v>
       </c>
       <c r="B37" s="38" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C37" s="51">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D37" s="51" t="s">
         <v>9</v>
@@ -6042,7 +6064,7 @@
         <v>49</v>
       </c>
       <c r="B38" s="38" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C38" s="51">
         <v>4</v>
@@ -6056,13 +6078,13 @@
         <v>49</v>
       </c>
       <c r="B39" s="38" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C39" s="51">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D39" s="51" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6070,13 +6092,13 @@
         <v>49</v>
       </c>
       <c r="B40" s="38" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C40" s="51">
         <v>2</v>
       </c>
       <c r="D40" s="51" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6084,13 +6106,13 @@
         <v>49</v>
       </c>
       <c r="B41" s="38" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C41" s="51">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D41" s="51" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6098,10 +6120,10 @@
         <v>49</v>
       </c>
       <c r="B42" s="38" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C42" s="51">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D42" s="51" t="s">
         <v>6</v>
@@ -6112,13 +6134,13 @@
         <v>49</v>
       </c>
       <c r="B43" s="38" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C43" s="51">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D43" s="51" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6126,10 +6148,10 @@
         <v>49</v>
       </c>
       <c r="B44" s="38" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C44" s="51">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D44" s="51" t="s">
         <v>9</v>
@@ -6140,7 +6162,7 @@
         <v>49</v>
       </c>
       <c r="B45" s="38" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C45" s="51">
         <v>4</v>
@@ -6154,13 +6176,13 @@
         <v>49</v>
       </c>
       <c r="B46" s="38" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C46" s="51">
         <v>4</v>
       </c>
       <c r="D46" s="51" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6168,13 +6190,13 @@
         <v>49</v>
       </c>
       <c r="B47" s="38" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C47" s="51">
         <v>4</v>
       </c>
       <c r="D47" s="51" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6182,13 +6204,13 @@
         <v>49</v>
       </c>
       <c r="B48" s="38" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C48" s="51">
         <v>4</v>
       </c>
       <c r="D48" s="51" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6196,13 +6218,13 @@
         <v>49</v>
       </c>
       <c r="B49" s="38" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C49" s="51">
         <v>4</v>
       </c>
       <c r="D49" s="51" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6210,13 +6232,13 @@
         <v>49</v>
       </c>
       <c r="B50" s="38" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C50" s="51">
         <v>4</v>
       </c>
       <c r="D50" s="51" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6224,27 +6246,27 @@
         <v>49</v>
       </c>
       <c r="B51" s="38" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C51" s="51">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D51" s="51" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="B52" s="76" t="s">
-        <v>215</v>
+      <c r="B52" s="38" t="s">
+        <v>165</v>
       </c>
       <c r="C52" s="51">
         <v>8</v>
       </c>
-      <c r="D52" s="80" t="s">
-        <v>8</v>
+      <c r="D52" s="51" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6252,10 +6274,10 @@
         <v>49</v>
       </c>
       <c r="B53" s="76" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C53" s="51">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D53" s="80" t="s">
         <v>8</v>
@@ -6266,10 +6288,10 @@
         <v>49</v>
       </c>
       <c r="B54" s="76" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C54" s="51">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D54" s="80" t="s">
         <v>8</v>
@@ -6279,10 +6301,10 @@
       <c r="A55" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="B55" s="76" t="s">
-        <v>218</v>
-      </c>
-      <c r="C55" s="51">
+      <c r="B55" s="147" t="s">
+        <v>249</v>
+      </c>
+      <c r="C55" s="109">
         <v>2</v>
       </c>
       <c r="D55" s="80" t="s">
@@ -6293,73 +6315,70 @@
       <c r="A56" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="B56" s="76" t="s">
-        <v>219</v>
-      </c>
-      <c r="C56" s="51">
-        <v>4</v>
+      <c r="B56" s="147" t="s">
+        <v>246</v>
+      </c>
+      <c r="C56" s="109">
+        <v>16</v>
       </c>
       <c r="D56" s="80" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="44" t="s">
-        <v>92</v>
-      </c>
-      <c r="B57" s="43" t="s">
-        <v>222</v>
-      </c>
-      <c r="C57" s="44">
-        <v>2</v>
-      </c>
-      <c r="D57" s="44" t="s">
+      <c r="A57" s="51" t="s">
+        <v>49</v>
+      </c>
+      <c r="B57" s="147" t="s">
+        <v>247</v>
+      </c>
+      <c r="C57" s="109">
+        <v>4</v>
+      </c>
+      <c r="D57" s="80" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="44" t="s">
-        <v>92</v>
-      </c>
-      <c r="B58" s="43" t="s">
-        <v>223</v>
-      </c>
-      <c r="C58" s="44">
-        <v>2</v>
-      </c>
-      <c r="D58" s="44" t="s">
+      <c r="A58" s="51" t="s">
+        <v>49</v>
+      </c>
+      <c r="B58" s="147" t="s">
+        <v>248</v>
+      </c>
+      <c r="C58" s="109">
+        <v>4</v>
+      </c>
+      <c r="D58" s="80" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="44" t="s">
-        <v>92</v>
-      </c>
-      <c r="B59" s="43" t="s">
-        <v>167</v>
-      </c>
-      <c r="C59" s="44">
-        <v>4</v>
-      </c>
-      <c r="D59" s="44" t="s">
-        <v>6</v>
+      <c r="A59" s="51" t="s">
+        <v>49</v>
+      </c>
+      <c r="B59" s="76" t="s">
+        <v>217</v>
+      </c>
+      <c r="C59" s="51">
+        <v>2</v>
+      </c>
+      <c r="D59" s="80" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="44" t="s">
-        <v>92</v>
-      </c>
-      <c r="B60" s="43" t="s">
-        <v>168</v>
-      </c>
-      <c r="C60" s="44">
-        <v>4</v>
-      </c>
-      <c r="D60" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="E60" s="61" t="s">
-        <v>188</v>
+      <c r="A60" s="51" t="s">
+        <v>49</v>
+      </c>
+      <c r="B60" s="76" t="s">
+        <v>218</v>
+      </c>
+      <c r="C60" s="51">
+        <v>4</v>
+      </c>
+      <c r="D60" s="80" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6367,16 +6386,13 @@
         <v>92</v>
       </c>
       <c r="B61" s="43" t="s">
-        <v>169</v>
+        <v>221</v>
       </c>
       <c r="C61" s="44">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D61" s="44" t="s">
         <v>8</v>
-      </c>
-      <c r="E61" s="61" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6384,16 +6400,13 @@
         <v>92</v>
       </c>
       <c r="B62" s="43" t="s">
-        <v>170</v>
+        <v>222</v>
       </c>
       <c r="C62" s="44">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D62" s="44" t="s">
         <v>8</v>
-      </c>
-      <c r="E62" s="61" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6401,13 +6414,13 @@
         <v>92</v>
       </c>
       <c r="B63" s="43" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C63" s="44">
         <v>4</v>
       </c>
       <c r="D63" s="44" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6415,7 +6428,7 @@
         <v>92</v>
       </c>
       <c r="B64" s="43" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C64" s="44">
         <v>4</v>
@@ -6432,13 +6445,16 @@
         <v>92</v>
       </c>
       <c r="B65" s="43" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C65" s="44">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D65" s="44" t="s">
         <v>8</v>
+      </c>
+      <c r="E65" s="61" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6446,7 +6462,7 @@
         <v>92</v>
       </c>
       <c r="B66" s="43" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C66" s="44">
         <v>4</v>
@@ -6463,16 +6479,13 @@
         <v>92</v>
       </c>
       <c r="B67" s="43" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C67" s="44">
         <v>4</v>
       </c>
       <c r="D67" s="44" t="s">
-        <v>6</v>
-      </c>
-      <c r="E67" s="61" t="s">
-        <v>188</v>
+        <v>8</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6480,13 +6493,16 @@
         <v>92</v>
       </c>
       <c r="B68" s="43" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C68" s="44">
         <v>4</v>
       </c>
       <c r="D68" s="44" t="s">
         <v>8</v>
+      </c>
+      <c r="E68" s="61" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6494,16 +6510,13 @@
         <v>92</v>
       </c>
       <c r="B69" s="43" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C69" s="44">
         <v>4</v>
       </c>
       <c r="D69" s="44" t="s">
         <v>8</v>
-      </c>
-      <c r="E69" s="61" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6511,13 +6524,16 @@
         <v>92</v>
       </c>
       <c r="B70" s="43" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C70" s="44">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D70" s="44" t="s">
         <v>8</v>
+      </c>
+      <c r="E70" s="61" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6525,13 +6541,16 @@
         <v>92</v>
       </c>
       <c r="B71" s="43" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C71" s="44">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D71" s="44" t="s">
-        <v>9</v>
+        <v>6</v>
+      </c>
+      <c r="E71" s="61" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6539,13 +6558,13 @@
         <v>92</v>
       </c>
       <c r="B72" s="43" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C72" s="44">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D72" s="44" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6553,13 +6572,16 @@
         <v>92</v>
       </c>
       <c r="B73" s="43" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C73" s="44">
         <v>4</v>
       </c>
       <c r="D73" s="44" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="E73" s="61" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6567,24 +6589,24 @@
         <v>92</v>
       </c>
       <c r="B74" s="43" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C74" s="44">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D74" s="44" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="44" t="s">
         <v>92</v>
       </c>
-      <c r="B75" s="77" t="s">
-        <v>221</v>
+      <c r="B75" s="43" t="s">
+        <v>179</v>
       </c>
       <c r="C75" s="44">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D75" s="44" t="s">
         <v>9</v>
@@ -6594,64 +6616,64 @@
       <c r="A76" s="44" t="s">
         <v>92</v>
       </c>
-      <c r="B76" s="126" t="s">
-        <v>236</v>
+      <c r="B76" s="43" t="s">
+        <v>180</v>
       </c>
       <c r="C76" s="44">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D76" s="44" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="44" t="s">
         <v>92</v>
       </c>
-      <c r="B77" s="126" t="s">
-        <v>239</v>
+      <c r="B77" s="43" t="s">
+        <v>181</v>
       </c>
       <c r="C77" s="44">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D77" s="44" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="44" t="s">
         <v>92</v>
       </c>
-      <c r="B78" s="126" t="s">
-        <v>240</v>
+      <c r="B78" s="43" t="s">
+        <v>182</v>
       </c>
       <c r="C78" s="44">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D78" s="44" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="44" t="s">
         <v>92</v>
       </c>
-      <c r="B79" s="126" t="s">
-        <v>244</v>
+      <c r="B79" s="77" t="s">
+        <v>220</v>
       </c>
       <c r="C79" s="44">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D79" s="44" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="44" t="s">
         <v>92</v>
       </c>
-      <c r="B80" s="126" t="s">
-        <v>242</v>
+      <c r="B80" s="125" t="s">
+        <v>234</v>
       </c>
       <c r="C80" s="44">
         <v>4</v>
@@ -6664,78 +6686,69 @@
       <c r="A81" s="44" t="s">
         <v>92</v>
       </c>
-      <c r="B81" s="126" t="s">
-        <v>243</v>
+      <c r="B81" s="125" t="s">
+        <v>237</v>
       </c>
       <c r="C81" s="44">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D81" s="44" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="82" t="s">
-        <v>210</v>
-      </c>
-      <c r="B82" s="66" t="s">
-        <v>191</v>
-      </c>
-      <c r="C82" s="62">
-        <v>16</v>
-      </c>
-      <c r="D82" s="82" t="s">
-        <v>8</v>
-      </c>
-      <c r="E82" s="61" t="s">
-        <v>188</v>
+      <c r="A82" s="44" t="s">
+        <v>92</v>
+      </c>
+      <c r="B82" s="125" t="s">
+        <v>238</v>
+      </c>
+      <c r="C82" s="44">
+        <v>2</v>
+      </c>
+      <c r="D82" s="44" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="82" t="s">
-        <v>210</v>
-      </c>
-      <c r="B83" s="57" t="s">
-        <v>189</v>
-      </c>
-      <c r="C83" s="62">
+      <c r="A83" s="44" t="s">
+        <v>92</v>
+      </c>
+      <c r="B83" s="125" t="s">
+        <v>241</v>
+      </c>
+      <c r="C83" s="44">
         <v>1</v>
       </c>
-      <c r="D83" s="82" t="s">
-        <v>8</v>
-      </c>
-      <c r="E83" s="61" t="s">
-        <v>188</v>
+      <c r="D83" s="44" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="82" t="s">
-        <v>210</v>
-      </c>
-      <c r="B84" s="66" t="s">
-        <v>193</v>
-      </c>
-      <c r="C84" s="62">
-        <v>2</v>
-      </c>
-      <c r="D84" s="82" t="s">
-        <v>8</v>
-      </c>
-      <c r="E84" s="61" t="s">
-        <v>188</v>
+      <c r="A84" s="44" t="s">
+        <v>92</v>
+      </c>
+      <c r="B84" s="125" t="s">
+        <v>239</v>
+      </c>
+      <c r="C84" s="44">
+        <v>4</v>
+      </c>
+      <c r="D84" s="44" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="82" t="s">
-        <v>210</v>
-      </c>
-      <c r="B85" s="73" t="s">
-        <v>211</v>
-      </c>
-      <c r="C85" s="62">
-        <v>2</v>
-      </c>
-      <c r="D85" s="82" t="s">
+      <c r="A85" s="44" t="s">
+        <v>92</v>
+      </c>
+      <c r="B85" s="125" t="s">
+        <v>240</v>
+      </c>
+      <c r="C85" s="44">
+        <v>4</v>
+      </c>
+      <c r="D85" s="44" t="s">
         <v>8</v>
       </c>
     </row>
@@ -6743,45 +6756,100 @@
       <c r="A86" s="82" t="s">
         <v>210</v>
       </c>
-      <c r="B86" s="73" t="s">
-        <v>212</v>
+      <c r="B86" s="66" t="s">
+        <v>191</v>
       </c>
       <c r="C86" s="62">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="D86" s="82" t="s">
         <v>8</v>
+      </c>
+      <c r="E86" s="61" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="82" t="s">
         <v>210</v>
       </c>
-      <c r="B87" s="73" t="s">
+      <c r="B87" s="57" t="s">
+        <v>189</v>
+      </c>
+      <c r="C87" s="62">
+        <v>1</v>
+      </c>
+      <c r="D87" s="82" t="s">
+        <v>8</v>
+      </c>
+      <c r="E87" s="61" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="82" t="s">
+        <v>210</v>
+      </c>
+      <c r="B88" s="66" t="s">
+        <v>193</v>
+      </c>
+      <c r="C88" s="62">
+        <v>2</v>
+      </c>
+      <c r="D88" s="82" t="s">
+        <v>8</v>
+      </c>
+      <c r="E88" s="61" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="82" t="s">
+        <v>210</v>
+      </c>
+      <c r="B89" s="73" t="s">
+        <v>211</v>
+      </c>
+      <c r="C89" s="62">
+        <v>2</v>
+      </c>
+      <c r="D89" s="82" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="82" t="s">
+        <v>210</v>
+      </c>
+      <c r="B90" s="73" t="s">
+        <v>212</v>
+      </c>
+      <c r="C90" s="62">
+        <v>2</v>
+      </c>
+      <c r="D90" s="82" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="82" t="s">
+        <v>210</v>
+      </c>
+      <c r="B91" s="73" t="s">
         <v>213</v>
       </c>
-      <c r="C87" s="62">
-        <v>2</v>
-      </c>
-      <c r="D87" s="82" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C88" s="20">
-        <f>SUM(C3:C87)</f>
-        <v>327</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="90" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90"/>
-    </row>
-    <row r="91" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91"/>
+      <c r="C91" s="62">
+        <v>2</v>
+      </c>
+      <c r="D91" s="82" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="92" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92"/>
+      <c r="C92" s="20">
+        <f>SUM(C3:C91)</f>
+        <v>339</v>
+      </c>
     </row>
     <row r="93" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93"/>
@@ -6791,6 +6859,15 @@
     </row>
     <row r="95" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95"/>
+    </row>
+    <row r="96" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A96"/>
+    </row>
+    <row r="97" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A97"/>
+    </row>
+    <row r="98" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A98"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -6855,21 +6932,21 @@
       <c r="G1" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="133" t="s">
+      <c r="H1" s="132" t="s">
         <v>205</v>
       </c>
-      <c r="I1" s="134"/>
-      <c r="J1" s="135"/>
-      <c r="K1" s="136" t="s">
+      <c r="I1" s="133"/>
+      <c r="J1" s="134"/>
+      <c r="K1" s="135" t="s">
         <v>206</v>
       </c>
-      <c r="L1" s="137"/>
-      <c r="M1" s="138"/>
-      <c r="N1" s="136" t="s">
+      <c r="L1" s="136"/>
+      <c r="M1" s="137"/>
+      <c r="N1" s="135" t="s">
         <v>207</v>
       </c>
-      <c r="O1" s="137"/>
-      <c r="P1" s="138"/>
+      <c r="O1" s="136"/>
+      <c r="P1" s="137"/>
     </row>
     <row r="2" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A2" s="26" t="s">
@@ -7938,7 +8015,7 @@
     </row>
     <row r="25" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="77" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B25" s="44">
         <v>4</v>
@@ -8315,30 +8392,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="139" t="s">
+      <c r="A1" s="138" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="139"/>
-      <c r="C1" s="139"/>
-      <c r="D1" s="139"/>
-      <c r="E1" s="140"/>
-      <c r="F1" s="140"/>
-      <c r="G1" s="140"/>
-      <c r="H1" s="140"/>
-      <c r="I1" s="140"/>
-      <c r="J1" s="140"/>
+      <c r="B1" s="138"/>
+      <c r="C1" s="138"/>
+      <c r="D1" s="138"/>
+      <c r="E1" s="139"/>
+      <c r="F1" s="139"/>
+      <c r="G1" s="139"/>
+      <c r="H1" s="139"/>
+      <c r="I1" s="139"/>
+      <c r="J1" s="139"/>
     </row>
     <row r="2" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="8"/>
-      <c r="B2" s="141"/>
-      <c r="C2" s="142"/>
-      <c r="D2" s="143"/>
-      <c r="E2" s="144"/>
-      <c r="F2" s="145"/>
-      <c r="G2" s="146"/>
-      <c r="H2" s="144"/>
-      <c r="I2" s="145"/>
-      <c r="J2" s="146"/>
+      <c r="B2" s="140"/>
+      <c r="C2" s="141"/>
+      <c r="D2" s="142"/>
+      <c r="E2" s="143"/>
+      <c r="F2" s="144"/>
+      <c r="G2" s="145"/>
+      <c r="H2" s="143"/>
+      <c r="I2" s="144"/>
+      <c r="J2" s="145"/>
     </row>
     <row r="3" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
@@ -8690,9 +8767,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q21" sqref="Q21"/>
+      <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8718,8 +8795,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="122" t="s">
-        <v>226</v>
+      <c r="A1" s="121" t="s">
+        <v>225</v>
       </c>
       <c r="B1" s="84"/>
       <c r="C1" s="85"/>
@@ -8729,21 +8806,21 @@
       <c r="G1" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="136" t="s">
+      <c r="H1" s="135" t="s">
+        <v>223</v>
+      </c>
+      <c r="I1" s="136"/>
+      <c r="J1" s="137"/>
+      <c r="K1" s="135" t="s">
         <v>224</v>
       </c>
-      <c r="I1" s="137"/>
-      <c r="J1" s="138"/>
-      <c r="K1" s="136" t="s">
-        <v>225</v>
-      </c>
-      <c r="L1" s="137"/>
-      <c r="M1" s="138"/>
-      <c r="N1" s="136" t="s">
-        <v>231</v>
-      </c>
-      <c r="O1" s="137"/>
-      <c r="P1" s="138"/>
+      <c r="L1" s="136"/>
+      <c r="M1" s="137"/>
+      <c r="N1" s="135" t="s">
+        <v>230</v>
+      </c>
+      <c r="O1" s="136"/>
+      <c r="P1" s="137"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="26" t="s">
@@ -8806,7 +8883,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="108" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E3" s="52" t="s">
         <v>25</v>
@@ -8893,7 +8970,7 @@
     </row>
     <row r="5" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="118" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B5" s="47">
         <v>4</v>
@@ -8948,7 +9025,7 @@
         <v>8</v>
       </c>
       <c r="D6" s="108" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E6" s="52" t="s">
         <v>25</v>
@@ -9077,7 +9154,7 @@
     </row>
     <row r="9" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="116" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B9" s="47">
         <v>4</v>
@@ -9122,17 +9199,17 @@
       </c>
     </row>
     <row r="10" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="76" t="s">
-        <v>217</v>
-      </c>
-      <c r="B10" s="51">
-        <v>16</v>
-      </c>
-      <c r="C10" s="80" t="s">
+      <c r="A10" s="147" t="s">
+        <v>249</v>
+      </c>
+      <c r="B10" s="109">
+        <v>2</v>
+      </c>
+      <c r="C10" s="109" t="s">
         <v>8</v>
       </c>
       <c r="D10" s="109" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E10" s="52" t="s">
         <v>25</v>
@@ -9140,95 +9217,95 @@
       <c r="F10" s="51"/>
       <c r="G10" s="94"/>
       <c r="H10" s="39">
+        <v>2</v>
+      </c>
+      <c r="I10" s="39">
+        <v>2</v>
+      </c>
+      <c r="J10" s="55">
+        <v>2</v>
+      </c>
+      <c r="K10" s="56">
+        <v>2</v>
+      </c>
+      <c r="L10" s="54">
+        <v>2</v>
+      </c>
+      <c r="M10" s="55">
+        <v>2</v>
+      </c>
+      <c r="N10" s="56">
+        <v>2</v>
+      </c>
+      <c r="O10" s="54">
+        <v>2</v>
+      </c>
+      <c r="P10" s="54">
+        <v>2</v>
+      </c>
+      <c r="R10">
+        <f>SUM(P10:P21)</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="147" t="s">
+        <v>246</v>
+      </c>
+      <c r="B11" s="109">
         <v>16</v>
       </c>
-      <c r="I10" s="39">
-        <v>16</v>
-      </c>
-      <c r="J10" s="55">
-        <v>16</v>
-      </c>
-      <c r="K10" s="56">
-        <v>16</v>
-      </c>
-      <c r="L10" s="54">
-        <v>8</v>
-      </c>
-      <c r="M10" s="55">
-        <v>8</v>
-      </c>
-      <c r="N10" s="56">
-        <v>8</v>
-      </c>
-      <c r="O10" s="54">
-        <v>8</v>
-      </c>
-      <c r="P10" s="54">
-        <v>8</v>
-      </c>
-      <c r="R10">
-        <f>SUM(P10:P17)</f>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="120" t="s">
-        <v>235</v>
-      </c>
-      <c r="B11" s="51">
-        <v>8</v>
-      </c>
-      <c r="C11" s="80" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="121" t="s">
-        <v>186</v>
-      </c>
-      <c r="E11" s="61" t="s">
-        <v>188</v>
+      <c r="C11" s="109" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="109" t="s">
+        <v>227</v>
+      </c>
+      <c r="E11" s="52" t="s">
+        <v>25</v>
       </c>
       <c r="F11" s="51"/>
       <c r="G11" s="94"/>
       <c r="H11" s="39">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="I11" s="39">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="J11" s="55">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="K11" s="56">
         <v>8</v>
       </c>
       <c r="L11" s="54">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="M11" s="55">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N11" s="56">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="O11" s="54">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="P11" s="54">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="76" t="s">
-        <v>215</v>
-      </c>
-      <c r="B12" s="51">
-        <v>8</v>
-      </c>
-      <c r="C12" s="80" t="s">
+      <c r="A12" s="147" t="s">
+        <v>247</v>
+      </c>
+      <c r="B12" s="109">
+        <v>4</v>
+      </c>
+      <c r="C12" s="109" t="s">
         <v>8</v>
       </c>
       <c r="D12" s="109" t="s">
-        <v>183</v>
+        <v>227</v>
       </c>
       <c r="E12" s="52" t="s">
         <v>25</v>
@@ -9236,45 +9313,45 @@
       <c r="F12" s="51"/>
       <c r="G12" s="94"/>
       <c r="H12" s="39">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I12" s="39">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="J12" s="55">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="K12" s="56">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="L12" s="54">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="M12" s="55">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="N12" s="56">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="O12" s="54">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="P12" s="54">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="76" t="s">
-        <v>219</v>
-      </c>
-      <c r="B13" s="51">
-        <v>4</v>
-      </c>
-      <c r="C13" s="80" t="s">
+      <c r="A13" s="147" t="s">
+        <v>248</v>
+      </c>
+      <c r="B13" s="109">
+        <v>4</v>
+      </c>
+      <c r="C13" s="109" t="s">
         <v>8</v>
       </c>
       <c r="D13" s="109" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E13" s="52" t="s">
         <v>25</v>
@@ -9310,63 +9387,63 @@
       </c>
     </row>
     <row r="14" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="38" t="s">
-        <v>153</v>
+      <c r="A14" s="119" t="s">
+        <v>233</v>
       </c>
       <c r="B14" s="51">
-        <v>2</v>
-      </c>
-      <c r="C14" s="51" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="109" t="s">
-        <v>228</v>
-      </c>
-      <c r="E14" s="52" t="s">
-        <v>25</v>
+        <v>8</v>
+      </c>
+      <c r="C14" s="80" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="120" t="s">
+        <v>186</v>
+      </c>
+      <c r="E14" s="61" t="s">
+        <v>188</v>
       </c>
       <c r="F14" s="51"/>
       <c r="G14" s="94"/>
       <c r="H14" s="39">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="I14" s="39">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J14" s="55">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="K14" s="56">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="L14" s="54">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M14" s="55">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N14" s="56">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O14" s="54">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P14" s="54">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="38" t="s">
-        <v>156</v>
+      <c r="A15" s="76" t="s">
+        <v>215</v>
       </c>
       <c r="B15" s="51">
-        <v>1</v>
-      </c>
-      <c r="C15" s="51" t="s">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="C15" s="80" t="s">
+        <v>8</v>
       </c>
       <c r="D15" s="109" t="s">
-        <v>228</v>
+        <v>183</v>
       </c>
       <c r="E15" s="52" t="s">
         <v>25</v>
@@ -9374,91 +9451,91 @@
       <c r="F15" s="51"/>
       <c r="G15" s="94"/>
       <c r="H15" s="39">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="I15" s="39">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J15" s="55">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="K15" s="56">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="L15" s="54">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="M15" s="55">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="N15" s="56">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="O15" s="54">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="P15" s="54">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="38" t="s">
-        <v>146</v>
+      <c r="A16" s="76" t="s">
+        <v>218</v>
       </c>
       <c r="B16" s="51">
-        <v>2</v>
-      </c>
-      <c r="C16" s="51" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="121" t="s">
-        <v>186</v>
-      </c>
-      <c r="E16" s="129" t="s">
-        <v>188</v>
+        <v>4</v>
+      </c>
+      <c r="C16" s="80" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="109" t="s">
+        <v>227</v>
+      </c>
+      <c r="E16" s="52" t="s">
+        <v>25</v>
       </c>
       <c r="F16" s="51"/>
       <c r="G16" s="94"/>
       <c r="H16" s="39">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I16" s="39">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J16" s="55">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K16" s="56">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="L16" s="54">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="M16" s="55">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="N16" s="56">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O16" s="54">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="P16" s="54">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="38" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="B17" s="51">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C17" s="51" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" s="121" t="s">
-        <v>186</v>
+        <v>6</v>
+      </c>
+      <c r="D17" s="109" t="s">
+        <v>227</v>
       </c>
       <c r="E17" s="52" t="s">
         <v>25</v>
@@ -9466,603 +9543,601 @@
       <c r="F17" s="51"/>
       <c r="G17" s="94"/>
       <c r="H17" s="39">
+        <v>2</v>
+      </c>
+      <c r="I17" s="39">
+        <v>2</v>
+      </c>
+      <c r="J17" s="55">
+        <v>2</v>
+      </c>
+      <c r="K17" s="56">
+        <v>2</v>
+      </c>
+      <c r="L17" s="54">
+        <v>2</v>
+      </c>
+      <c r="M17" s="55">
+        <v>2</v>
+      </c>
+      <c r="N17" s="56">
+        <v>2</v>
+      </c>
+      <c r="O17" s="54">
+        <v>2</v>
+      </c>
+      <c r="P17" s="54">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="38" t="s">
+        <v>156</v>
+      </c>
+      <c r="B18" s="51">
         <v>1</v>
       </c>
-      <c r="I17" s="39">
+      <c r="C18" s="51" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="109" t="s">
+        <v>227</v>
+      </c>
+      <c r="E18" s="52" t="s">
+        <v>25</v>
+      </c>
+      <c r="F18" s="51"/>
+      <c r="G18" s="94"/>
+      <c r="H18" s="39">
         <v>1</v>
       </c>
-      <c r="J17" s="55">
+      <c r="I18" s="39">
         <v>1</v>
       </c>
-      <c r="K17" s="56">
+      <c r="J18" s="55">
         <v>1</v>
       </c>
-      <c r="L17" s="54">
+      <c r="K18" s="56">
         <v>1</v>
       </c>
-      <c r="M17" s="55">
+      <c r="L18" s="54">
         <v>1</v>
       </c>
-      <c r="N17" s="56">
+      <c r="M18" s="55">
         <v>1</v>
       </c>
-      <c r="O17" s="54">
+      <c r="N18" s="56">
         <v>1</v>
       </c>
-      <c r="P17" s="54">
+      <c r="O18" s="54">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="119" t="s">
+      <c r="P18" s="54">
+        <v>1</v>
+      </c>
+      <c r="R18">
+        <f>SUM(P22:P32)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="38" t="s">
+        <v>146</v>
+      </c>
+      <c r="B19" s="51">
+        <v>2</v>
+      </c>
+      <c r="C19" s="51" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="148" t="s">
+        <v>186</v>
+      </c>
+      <c r="E19" s="128" t="s">
+        <v>188</v>
+      </c>
+      <c r="F19" s="51"/>
+      <c r="G19" s="94"/>
+      <c r="H19" s="39">
+        <v>2</v>
+      </c>
+      <c r="I19" s="39">
+        <v>2</v>
+      </c>
+      <c r="J19" s="55">
+        <v>2</v>
+      </c>
+      <c r="K19" s="56">
+        <v>1</v>
+      </c>
+      <c r="L19" s="54">
+        <v>1</v>
+      </c>
+      <c r="M19" s="55">
+        <v>1</v>
+      </c>
+      <c r="N19" s="56">
+        <v>0</v>
+      </c>
+      <c r="O19" s="54">
+        <v>0</v>
+      </c>
+      <c r="P19" s="54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="38" t="s">
+        <v>250</v>
+      </c>
+      <c r="B20" s="51">
+        <v>2</v>
+      </c>
+      <c r="C20" s="51" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="51" t="s">
+        <v>251</v>
+      </c>
+      <c r="E20" s="52" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20" s="51"/>
+      <c r="G20" s="94"/>
+      <c r="H20" s="39">
+        <v>2</v>
+      </c>
+      <c r="I20" s="39">
+        <v>2</v>
+      </c>
+      <c r="J20" s="55">
+        <v>2</v>
+      </c>
+      <c r="K20" s="56">
+        <v>2</v>
+      </c>
+      <c r="L20" s="54">
+        <v>2</v>
+      </c>
+      <c r="M20" s="55">
+        <v>2</v>
+      </c>
+      <c r="N20" s="56">
+        <v>2</v>
+      </c>
+      <c r="O20" s="54">
+        <v>2</v>
+      </c>
+      <c r="P20" s="54">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="38" t="s">
+        <v>147</v>
+      </c>
+      <c r="B21" s="51">
+        <v>1</v>
+      </c>
+      <c r="C21" s="51" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="120" t="s">
+        <v>186</v>
+      </c>
+      <c r="E21" s="52" t="s">
+        <v>25</v>
+      </c>
+      <c r="F21" s="51"/>
+      <c r="G21" s="94"/>
+      <c r="H21" s="39">
+        <v>1</v>
+      </c>
+      <c r="I21" s="39">
+        <v>1</v>
+      </c>
+      <c r="J21" s="55">
+        <v>1</v>
+      </c>
+      <c r="K21" s="56">
+        <v>1</v>
+      </c>
+      <c r="L21" s="54">
+        <v>1</v>
+      </c>
+      <c r="M21" s="55">
+        <v>1</v>
+      </c>
+      <c r="N21" s="56">
+        <v>1</v>
+      </c>
+      <c r="O21" s="54">
+        <v>1</v>
+      </c>
+      <c r="P21" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="125" t="s">
         <v>234</v>
       </c>
-      <c r="B18" s="44">
-        <v>0</v>
-      </c>
-      <c r="C18" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" s="110" t="s">
-        <v>229</v>
-      </c>
-      <c r="E18" s="128" t="s">
+      <c r="B22" s="44">
+        <v>4</v>
+      </c>
+      <c r="C22" s="126" t="s">
+        <v>235</v>
+      </c>
+      <c r="D22" s="126" t="s">
+        <v>236</v>
+      </c>
+      <c r="E22" s="128" t="s">
+        <v>188</v>
+      </c>
+      <c r="F22" s="44"/>
+      <c r="G22" s="122"/>
+      <c r="H22" s="43">
+        <v>4</v>
+      </c>
+      <c r="I22" s="43">
+        <v>4</v>
+      </c>
+      <c r="J22" s="123">
+        <v>2</v>
+      </c>
+      <c r="K22" s="124">
+        <v>2</v>
+      </c>
+      <c r="L22" s="43">
+        <v>0</v>
+      </c>
+      <c r="M22" s="123">
+        <v>0</v>
+      </c>
+      <c r="N22" s="124">
+        <v>0</v>
+      </c>
+      <c r="O22" s="43">
+        <v>0</v>
+      </c>
+      <c r="P22" s="43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="125" t="s">
+        <v>237</v>
+      </c>
+      <c r="B23" s="44">
+        <v>1</v>
+      </c>
+      <c r="C23" s="126" t="s">
+        <v>235</v>
+      </c>
+      <c r="D23" s="126" t="s">
+        <v>187</v>
+      </c>
+      <c r="E23" s="128" t="s">
+        <v>188</v>
+      </c>
+      <c r="F23" s="44"/>
+      <c r="G23" s="122"/>
+      <c r="H23" s="43">
+        <v>1</v>
+      </c>
+      <c r="I23" s="43">
+        <v>1</v>
+      </c>
+      <c r="J23" s="123">
+        <v>1</v>
+      </c>
+      <c r="K23" s="124">
+        <v>1</v>
+      </c>
+      <c r="L23" s="43">
+        <v>1</v>
+      </c>
+      <c r="M23" s="123">
+        <v>1</v>
+      </c>
+      <c r="N23" s="124">
+        <v>0</v>
+      </c>
+      <c r="O23" s="43">
+        <v>0</v>
+      </c>
+      <c r="P23" s="43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="125" t="s">
+        <v>238</v>
+      </c>
+      <c r="B24" s="44">
+        <v>2</v>
+      </c>
+      <c r="C24" s="126" t="s">
+        <v>235</v>
+      </c>
+      <c r="D24" s="126" t="s">
+        <v>187</v>
+      </c>
+      <c r="E24" s="127" t="s">
         <v>25</v>
       </c>
-      <c r="F18" s="127" t="s">
+      <c r="F24" s="44"/>
+      <c r="G24" s="122"/>
+      <c r="H24" s="43">
+        <v>2</v>
+      </c>
+      <c r="I24" s="43">
+        <v>2</v>
+      </c>
+      <c r="J24" s="123">
+        <v>2</v>
+      </c>
+      <c r="K24" s="124">
+        <v>2</v>
+      </c>
+      <c r="L24" s="43">
+        <v>2</v>
+      </c>
+      <c r="M24" s="123">
+        <v>2</v>
+      </c>
+      <c r="N24" s="124">
+        <v>1</v>
+      </c>
+      <c r="O24" s="43">
+        <v>1</v>
+      </c>
+      <c r="P24" s="43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="125" t="s">
         <v>241</v>
       </c>
-      <c r="G18" s="97"/>
-      <c r="H18" s="43">
-        <v>0</v>
-      </c>
-      <c r="I18" s="43">
-        <v>0</v>
-      </c>
-      <c r="J18" s="45">
-        <v>0</v>
-      </c>
-      <c r="K18" s="46">
-        <v>0</v>
-      </c>
-      <c r="L18" s="43">
-        <v>0</v>
-      </c>
-      <c r="M18" s="45">
-        <v>0</v>
-      </c>
-      <c r="N18" s="46">
-        <v>0</v>
-      </c>
-      <c r="O18" s="43">
-        <v>0</v>
-      </c>
-      <c r="P18" s="43">
-        <v>0</v>
-      </c>
-      <c r="R18">
-        <f>SUM(P18:P29)</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="126" t="s">
+      <c r="B25" s="44">
+        <v>1</v>
+      </c>
+      <c r="C25" s="126" t="s">
+        <v>242</v>
+      </c>
+      <c r="D25" s="126" t="s">
+        <v>228</v>
+      </c>
+      <c r="E25" s="128" t="s">
+        <v>188</v>
+      </c>
+      <c r="F25" s="44"/>
+      <c r="G25" s="122"/>
+      <c r="H25" s="43">
+        <v>1</v>
+      </c>
+      <c r="I25" s="43">
+        <v>1</v>
+      </c>
+      <c r="J25" s="123">
+        <v>1</v>
+      </c>
+      <c r="K25" s="124">
+        <v>1</v>
+      </c>
+      <c r="L25" s="43">
+        <v>1</v>
+      </c>
+      <c r="M25" s="123">
+        <v>1</v>
+      </c>
+      <c r="N25" s="124">
+        <v>0</v>
+      </c>
+      <c r="O25" s="43">
+        <v>0</v>
+      </c>
+      <c r="P25" s="43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="125" t="s">
+        <v>239</v>
+      </c>
+      <c r="B26" s="44">
+        <v>4</v>
+      </c>
+      <c r="C26" s="126" t="s">
+        <v>235</v>
+      </c>
+      <c r="D26" s="126" t="s">
         <v>236</v>
       </c>
-      <c r="B19" s="44">
-        <v>4</v>
-      </c>
-      <c r="C19" s="127" t="s">
-        <v>237</v>
-      </c>
-      <c r="D19" s="127" t="s">
-        <v>238</v>
-      </c>
-      <c r="E19" s="129" t="s">
-        <v>188</v>
-      </c>
-      <c r="F19" s="44"/>
-      <c r="G19" s="123"/>
-      <c r="H19" s="43">
-        <v>4</v>
-      </c>
-      <c r="I19" s="43">
-        <v>4</v>
-      </c>
-      <c r="J19" s="124">
-        <v>2</v>
-      </c>
-      <c r="K19" s="125">
-        <v>2</v>
-      </c>
-      <c r="L19" s="43">
-        <v>0</v>
-      </c>
-      <c r="M19" s="124">
-        <v>0</v>
-      </c>
-      <c r="N19" s="125">
-        <v>0</v>
-      </c>
-      <c r="O19" s="43">
-        <v>0</v>
-      </c>
-      <c r="P19" s="43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="126" t="s">
-        <v>239</v>
-      </c>
-      <c r="B20" s="44">
-        <v>1</v>
-      </c>
-      <c r="C20" s="127" t="s">
-        <v>237</v>
-      </c>
-      <c r="D20" s="127" t="s">
-        <v>187</v>
-      </c>
-      <c r="E20" s="129" t="s">
-        <v>188</v>
-      </c>
-      <c r="F20" s="44"/>
-      <c r="G20" s="123"/>
-      <c r="H20" s="43">
-        <v>1</v>
-      </c>
-      <c r="I20" s="43">
-        <v>1</v>
-      </c>
-      <c r="J20" s="124">
-        <v>1</v>
-      </c>
-      <c r="K20" s="125">
-        <v>1</v>
-      </c>
-      <c r="L20" s="43">
-        <v>1</v>
-      </c>
-      <c r="M20" s="124">
-        <v>1</v>
-      </c>
-      <c r="N20" s="125">
-        <v>0</v>
-      </c>
-      <c r="O20" s="43">
-        <v>0</v>
-      </c>
-      <c r="P20" s="43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="126" t="s">
+      <c r="E26" s="127" t="s">
+        <v>25</v>
+      </c>
+      <c r="F26" s="44"/>
+      <c r="G26" s="122"/>
+      <c r="H26" s="43">
+        <v>4</v>
+      </c>
+      <c r="I26" s="43">
+        <v>4</v>
+      </c>
+      <c r="J26" s="123">
+        <v>4</v>
+      </c>
+      <c r="K26" s="124">
+        <v>4</v>
+      </c>
+      <c r="L26" s="43">
+        <v>4</v>
+      </c>
+      <c r="M26" s="123">
+        <v>4</v>
+      </c>
+      <c r="N26" s="124">
+        <v>2</v>
+      </c>
+      <c r="O26" s="43">
+        <v>2</v>
+      </c>
+      <c r="P26" s="43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="125" t="s">
         <v>240</v>
       </c>
-      <c r="B21" s="44">
-        <v>2</v>
-      </c>
-      <c r="C21" s="127" t="s">
-        <v>237</v>
-      </c>
-      <c r="D21" s="127" t="s">
-        <v>187</v>
-      </c>
-      <c r="E21" s="128" t="s">
+      <c r="B27" s="44">
+        <v>4</v>
+      </c>
+      <c r="C27" s="126" t="s">
+        <v>235</v>
+      </c>
+      <c r="D27" s="126" t="s">
+        <v>228</v>
+      </c>
+      <c r="E27" s="127" t="s">
         <v>25</v>
       </c>
-      <c r="F21" s="44"/>
-      <c r="G21" s="123"/>
-      <c r="H21" s="43">
-        <v>2</v>
-      </c>
-      <c r="I21" s="43">
-        <v>2</v>
-      </c>
-      <c r="J21" s="124">
-        <v>2</v>
-      </c>
-      <c r="K21" s="125">
-        <v>2</v>
-      </c>
-      <c r="L21" s="43">
-        <v>2</v>
-      </c>
-      <c r="M21" s="124">
-        <v>2</v>
-      </c>
-      <c r="N21" s="125">
-        <v>1</v>
-      </c>
-      <c r="O21" s="43">
-        <v>1</v>
-      </c>
-      <c r="P21" s="43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="126" t="s">
-        <v>244</v>
-      </c>
-      <c r="B22" s="44">
-        <v>1</v>
-      </c>
-      <c r="C22" s="127" t="s">
-        <v>245</v>
-      </c>
-      <c r="D22" s="127" t="s">
-        <v>229</v>
-      </c>
-      <c r="E22" s="129" t="s">
-        <v>188</v>
-      </c>
-      <c r="F22" s="44"/>
-      <c r="G22" s="123"/>
-      <c r="H22" s="43">
-        <v>1</v>
-      </c>
-      <c r="I22" s="43">
-        <v>1</v>
-      </c>
-      <c r="J22" s="124">
-        <v>1</v>
-      </c>
-      <c r="K22" s="125">
-        <v>1</v>
-      </c>
-      <c r="L22" s="43">
-        <v>1</v>
-      </c>
-      <c r="M22" s="124">
-        <v>1</v>
-      </c>
-      <c r="N22" s="125">
-        <v>0</v>
-      </c>
-      <c r="O22" s="43">
-        <v>0</v>
-      </c>
-      <c r="P22" s="43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="126" t="s">
-        <v>242</v>
-      </c>
-      <c r="B23" s="44">
-        <v>4</v>
-      </c>
-      <c r="C23" s="127" t="s">
-        <v>237</v>
-      </c>
-      <c r="D23" s="127" t="s">
-        <v>238</v>
-      </c>
-      <c r="E23" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="F23" s="44"/>
-      <c r="G23" s="123"/>
-      <c r="H23" s="43">
-        <v>4</v>
-      </c>
-      <c r="I23" s="43">
-        <v>4</v>
-      </c>
-      <c r="J23" s="124">
-        <v>4</v>
-      </c>
-      <c r="K23" s="125">
-        <v>4</v>
-      </c>
-      <c r="L23" s="43">
-        <v>4</v>
-      </c>
-      <c r="M23" s="124">
-        <v>4</v>
-      </c>
-      <c r="N23" s="125">
-        <v>2</v>
-      </c>
-      <c r="O23" s="43">
-        <v>2</v>
-      </c>
-      <c r="P23" s="43">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="126" t="s">
-        <v>243</v>
-      </c>
-      <c r="B24" s="44">
-        <v>4</v>
-      </c>
-      <c r="C24" s="127" t="s">
-        <v>237</v>
-      </c>
-      <c r="D24" s="127" t="s">
-        <v>229</v>
-      </c>
-      <c r="E24" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="F24" s="44"/>
-      <c r="G24" s="123"/>
-      <c r="H24" s="43">
-        <v>4</v>
-      </c>
-      <c r="I24" s="43">
-        <v>4</v>
-      </c>
-      <c r="J24" s="124">
-        <v>4</v>
-      </c>
-      <c r="K24" s="125">
-        <v>4</v>
-      </c>
-      <c r="L24" s="43">
-        <v>4</v>
-      </c>
-      <c r="M24" s="124">
-        <v>4</v>
-      </c>
-      <c r="N24" s="125">
-        <v>4</v>
-      </c>
-      <c r="O24" s="43">
-        <v>4</v>
-      </c>
-      <c r="P24" s="43">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="43" t="s">
-        <v>178</v>
-      </c>
-      <c r="B25" s="44">
-        <v>8</v>
-      </c>
-      <c r="C25" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="D25" s="110" t="s">
-        <v>185</v>
-      </c>
-      <c r="E25" s="53" t="s">
-        <v>25</v>
-      </c>
-      <c r="F25" s="44"/>
-      <c r="G25" s="97"/>
-      <c r="H25" s="43">
-        <v>8</v>
-      </c>
-      <c r="I25" s="43">
-        <v>8</v>
-      </c>
-      <c r="J25" s="45">
-        <v>8</v>
-      </c>
-      <c r="K25" s="46">
-        <v>8</v>
-      </c>
-      <c r="L25" s="43">
-        <v>8</v>
-      </c>
-      <c r="M25" s="45">
-        <v>8</v>
-      </c>
-      <c r="N25" s="46">
-        <v>7</v>
-      </c>
-      <c r="O25" s="43">
-        <v>7</v>
-      </c>
-      <c r="P25" s="43">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="43" t="s">
-        <v>222</v>
-      </c>
-      <c r="B26" s="44">
-        <v>2</v>
-      </c>
-      <c r="C26" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="D26" s="110" t="s">
-        <v>185</v>
-      </c>
-      <c r="E26" s="61" t="s">
-        <v>188</v>
-      </c>
-      <c r="F26" s="44"/>
-      <c r="G26" s="97"/>
-      <c r="H26" s="43">
-        <v>2</v>
-      </c>
-      <c r="I26" s="43">
-        <v>2</v>
-      </c>
-      <c r="J26" s="45">
-        <v>0</v>
-      </c>
-      <c r="K26" s="46">
-        <v>0</v>
-      </c>
-      <c r="L26" s="43">
-        <v>0</v>
-      </c>
-      <c r="M26" s="45">
-        <v>0</v>
-      </c>
-      <c r="N26" s="46">
-        <v>0</v>
-      </c>
-      <c r="O26" s="43">
-        <v>0</v>
-      </c>
-      <c r="P26" s="43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="43" t="s">
-        <v>223</v>
-      </c>
-      <c r="B27" s="44">
-        <v>2</v>
-      </c>
-      <c r="C27" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="D27" s="110" t="s">
-        <v>185</v>
-      </c>
-      <c r="E27" s="61" t="s">
-        <v>188</v>
-      </c>
       <c r="F27" s="44"/>
-      <c r="G27" s="97"/>
+      <c r="G27" s="122"/>
       <c r="H27" s="43">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I27" s="43">
-        <v>2</v>
-      </c>
-      <c r="J27" s="45">
-        <v>0</v>
-      </c>
-      <c r="K27" s="46">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="J27" s="123">
+        <v>4</v>
+      </c>
+      <c r="K27" s="124">
+        <v>4</v>
       </c>
       <c r="L27" s="43">
-        <v>0</v>
-      </c>
-      <c r="M27" s="45">
-        <v>0</v>
-      </c>
-      <c r="N27" s="46">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="M27" s="123">
+        <v>4</v>
+      </c>
+      <c r="N27" s="124">
+        <v>4</v>
       </c>
       <c r="O27" s="43">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="P27" s="43">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R27">
         <f>SUM(R3)</f>
         <v>10</v>
       </c>
       <c r="S27" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="28" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="43" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="B28" s="44">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C28" s="44" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D28" s="110" t="s">
         <v>185</v>
       </c>
-      <c r="E28" s="61" t="s">
-        <v>188</v>
+      <c r="E28" s="53" t="s">
+        <v>25</v>
       </c>
       <c r="F28" s="44"/>
       <c r="G28" s="97"/>
       <c r="H28" s="43">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="I28" s="43">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J28" s="45">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K28" s="46">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="L28" s="43">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="M28" s="45">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N28" s="46">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="O28" s="43">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="P28" s="43">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="R28">
         <f>SUM(R10)</f>
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="S28" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="29" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="77" t="s">
-        <v>176</v>
+      <c r="A29" s="43" t="s">
+        <v>221</v>
       </c>
       <c r="B29" s="44">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C29" s="44" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D29" s="110" t="s">
         <v>185</v>
       </c>
-      <c r="E29" s="53" t="s">
-        <v>25</v>
+      <c r="E29" s="61" t="s">
+        <v>188</v>
       </c>
       <c r="F29" s="44"/>
       <c r="G29" s="97"/>
       <c r="H29" s="43">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I29" s="43">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J29" s="45">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K29" s="46">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L29" s="43">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M29" s="45">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N29" s="46">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O29" s="43">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P29" s="43">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R29">
         <f>SUM(R18)</f>
@@ -10073,81 +10148,216 @@
       </c>
     </row>
     <row r="30" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="73" t="s">
+      <c r="A30" s="43" t="s">
+        <v>222</v>
+      </c>
+      <c r="B30" s="44">
+        <v>2</v>
+      </c>
+      <c r="C30" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" s="110" t="s">
+        <v>185</v>
+      </c>
+      <c r="E30" s="61" t="s">
+        <v>188</v>
+      </c>
+      <c r="F30" s="44"/>
+      <c r="G30" s="97"/>
+      <c r="H30" s="43">
+        <v>2</v>
+      </c>
+      <c r="I30" s="43">
+        <v>2</v>
+      </c>
+      <c r="J30" s="45">
+        <v>0</v>
+      </c>
+      <c r="K30" s="46">
+        <v>0</v>
+      </c>
+      <c r="L30" s="43">
+        <v>0</v>
+      </c>
+      <c r="M30" s="45">
+        <v>0</v>
+      </c>
+      <c r="N30" s="46">
+        <v>0</v>
+      </c>
+      <c r="O30" s="43">
+        <v>0</v>
+      </c>
+      <c r="P30" s="43">
+        <v>0</v>
+      </c>
+      <c r="R30">
+        <f>SUM(P33)</f>
+        <v>2</v>
+      </c>
+      <c r="S30" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="43" t="s">
+        <v>175</v>
+      </c>
+      <c r="B31" s="44">
+        <v>2</v>
+      </c>
+      <c r="C31" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" s="110" t="s">
+        <v>185</v>
+      </c>
+      <c r="E31" s="61" t="s">
+        <v>188</v>
+      </c>
+      <c r="F31" s="44"/>
+      <c r="G31" s="97"/>
+      <c r="H31" s="43">
+        <v>2</v>
+      </c>
+      <c r="I31" s="43">
+        <v>0</v>
+      </c>
+      <c r="J31" s="45">
+        <v>0</v>
+      </c>
+      <c r="K31" s="46">
+        <v>0</v>
+      </c>
+      <c r="L31" s="43">
+        <v>0</v>
+      </c>
+      <c r="M31" s="45">
+        <v>0</v>
+      </c>
+      <c r="N31" s="46">
+        <v>0</v>
+      </c>
+      <c r="O31" s="43">
+        <v>0</v>
+      </c>
+      <c r="P31" s="43">
+        <v>0</v>
+      </c>
+      <c r="R31">
+        <f>SUM(H34)</f>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="77" t="s">
+        <v>176</v>
+      </c>
+      <c r="B32" s="44">
+        <v>4</v>
+      </c>
+      <c r="C32" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="D32" s="110" t="s">
+        <v>185</v>
+      </c>
+      <c r="E32" s="53" t="s">
+        <v>25</v>
+      </c>
+      <c r="F32" s="44"/>
+      <c r="G32" s="97"/>
+      <c r="H32" s="43">
+        <v>4</v>
+      </c>
+      <c r="I32" s="43">
+        <v>4</v>
+      </c>
+      <c r="J32" s="45">
+        <v>4</v>
+      </c>
+      <c r="K32" s="46">
+        <v>4</v>
+      </c>
+      <c r="L32" s="43">
+        <v>2</v>
+      </c>
+      <c r="M32" s="45">
+        <v>2</v>
+      </c>
+      <c r="N32" s="46">
+        <v>2</v>
+      </c>
+      <c r="O32" s="43">
+        <v>2</v>
+      </c>
+      <c r="P32" s="43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="73" t="s">
         <v>211</v>
       </c>
-      <c r="B30" s="62">
-        <v>2</v>
-      </c>
-      <c r="C30" s="62" t="s">
-        <v>8</v>
-      </c>
-      <c r="D30" s="111" t="s">
+      <c r="B33" s="62">
+        <v>2</v>
+      </c>
+      <c r="C33" s="62" t="s">
+        <v>8</v>
+      </c>
+      <c r="D33" s="111" t="s">
         <v>186</v>
       </c>
-      <c r="E30" s="53" t="s">
+      <c r="E33" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="F30" s="62"/>
-      <c r="G30" s="102"/>
-      <c r="H30" s="57">
-        <v>2</v>
-      </c>
-      <c r="I30" s="57">
-        <v>2</v>
-      </c>
-      <c r="J30" s="58">
-        <v>2</v>
-      </c>
-      <c r="K30" s="59">
-        <v>2</v>
-      </c>
-      <c r="L30" s="57">
-        <v>2</v>
-      </c>
-      <c r="M30" s="58">
-        <v>2</v>
-      </c>
-      <c r="N30" s="59">
-        <v>2</v>
-      </c>
-      <c r="O30" s="57">
-        <v>2</v>
-      </c>
-      <c r="P30" s="57">
-        <v>2</v>
-      </c>
-      <c r="R30">
-        <f>SUM(P30)</f>
-        <v>2</v>
-      </c>
-      <c r="S30" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="31" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F31" s="104" t="s">
+      <c r="F33" s="62"/>
+      <c r="G33" s="102"/>
+      <c r="H33" s="57">
+        <v>2</v>
+      </c>
+      <c r="I33" s="57">
+        <v>2</v>
+      </c>
+      <c r="J33" s="58">
+        <v>2</v>
+      </c>
+      <c r="K33" s="59">
+        <v>2</v>
+      </c>
+      <c r="L33" s="57">
+        <v>2</v>
+      </c>
+      <c r="M33" s="58">
+        <v>2</v>
+      </c>
+      <c r="N33" s="59">
+        <v>2</v>
+      </c>
+      <c r="O33" s="57">
+        <v>2</v>
+      </c>
+      <c r="P33" s="57">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F34" s="104" t="s">
         <v>204</v>
       </c>
-      <c r="H31">
-        <f>SUM(H3:H30)</f>
-        <v>103</v>
-      </c>
-      <c r="R31">
-        <f>SUM(H31)</f>
-        <v>103</v>
-      </c>
-    </row>
-    <row r="32" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="33" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="34" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="35" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="36" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="37" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="38" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="39" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="40" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="41" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="H34">
+        <f>SUM(H3:H33)</f>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="38" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="39" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="41" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="H1:J1"/>
@@ -10291,9 +10501,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O9" sqref="O9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -10302,30 +10512,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="147" t="s">
-        <v>227</v>
-      </c>
-      <c r="B1" s="139"/>
-      <c r="C1" s="139"/>
-      <c r="D1" s="139"/>
-      <c r="E1" s="140"/>
-      <c r="F1" s="140"/>
-      <c r="G1" s="140"/>
-      <c r="H1" s="140"/>
-      <c r="I1" s="140"/>
-      <c r="J1" s="140"/>
+      <c r="A1" s="146" t="s">
+        <v>226</v>
+      </c>
+      <c r="B1" s="138"/>
+      <c r="C1" s="138"/>
+      <c r="D1" s="138"/>
+      <c r="E1" s="139"/>
+      <c r="F1" s="139"/>
+      <c r="G1" s="139"/>
+      <c r="H1" s="139"/>
+      <c r="I1" s="139"/>
+      <c r="J1" s="139"/>
     </row>
     <row r="2" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="8"/>
-      <c r="B2" s="141"/>
-      <c r="C2" s="142"/>
-      <c r="D2" s="143"/>
-      <c r="E2" s="144"/>
-      <c r="F2" s="145"/>
-      <c r="G2" s="146"/>
-      <c r="H2" s="144"/>
-      <c r="I2" s="145"/>
-      <c r="J2" s="146"/>
+      <c r="B2" s="140"/>
+      <c r="C2" s="141"/>
+      <c r="D2" s="142"/>
+      <c r="E2" s="143"/>
+      <c r="F2" s="144"/>
+      <c r="G2" s="145"/>
+      <c r="H2" s="143"/>
+      <c r="I2" s="144"/>
+      <c r="J2" s="145"/>
     </row>
     <row r="3" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
@@ -10432,40 +10642,40 @@
         <v>27</v>
       </c>
       <c r="B6" s="10">
-        <f>SUM('Sprint 2'!H3:H30)</f>
-        <v>103</v>
+        <f>SUM('Sprint 2'!H3:H33)</f>
+        <v>115</v>
       </c>
       <c r="C6" s="15">
         <f>SUM('Sprint 2'!I3:I37)</f>
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="D6" s="28">
         <f>SUM('Sprint 2'!J3:J37)</f>
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="E6" s="10">
         <f>SUM('Sprint 2'!K3:K37)</f>
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="F6" s="15">
         <f>SUM('Sprint 2'!L3:L37)</f>
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="G6" s="28">
         <f>SUM('Sprint 2'!M3:M37)</f>
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="H6" s="10">
         <f>SUM('Sprint 2'!N3:N37)</f>
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="I6" s="15">
         <f>SUM('Sprint 2'!O3:O37)</f>
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="J6" s="28">
         <f>SUM('Sprint 2'!P3:P37)</f>
-        <v>50</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -10474,35 +10684,35 @@
       </c>
       <c r="B7" s="5">
         <f>SUM('Sprint 2'!$B$3:$B$37)-(((B5-1)*SUM('Sprint 2'!$B$3:$B$37))/($J$5-1))</f>
-        <v>103</v>
+        <v>115</v>
       </c>
       <c r="C7" s="16">
         <f>SUM('Sprint 2'!$B$3:$B$37)-(((C5-1)*SUM('Sprint 2'!$B$3:$B$37))/($J$5-1))</f>
-        <v>90.125</v>
+        <v>100.625</v>
       </c>
       <c r="D7" s="11">
         <f>SUM('Sprint 2'!$B$3:$B$37)-(((D5-1)*SUM('Sprint 2'!$B$3:$B$37))/($J$5-1))</f>
-        <v>77.25</v>
+        <v>86.25</v>
       </c>
       <c r="E7" s="5">
         <f>SUM('Sprint 2'!$B$3:$B$37)-(((E5-1)*SUM('Sprint 2'!$B$3:$B$37))/($J$5-1))</f>
-        <v>64.375</v>
+        <v>71.875</v>
       </c>
       <c r="F7" s="16">
         <f>SUM('Sprint 2'!$B$3:$B$37)-(((F5-1)*SUM('Sprint 2'!$B$3:$B$37))/($J$5-1))</f>
-        <v>51.5</v>
+        <v>57.5</v>
       </c>
       <c r="G7" s="11">
         <f>SUM('Sprint 2'!$B$3:$B$37)-(((G5-1)*SUM('Sprint 2'!$B$3:$B$37))/($J$5-1))</f>
-        <v>38.625</v>
+        <v>43.125</v>
       </c>
       <c r="H7" s="5">
         <f>SUM('Sprint 2'!$B$3:$B$37)-(((H5-1)*SUM('Sprint 2'!$B$3:$B$37))/($J$5-1))</f>
-        <v>25.75</v>
+        <v>28.75</v>
       </c>
       <c r="I7" s="16">
         <f>SUM('Sprint 2'!$B$3:$B$37)-(((I5-1)*SUM('Sprint 2'!$B$3:$B$37))/($J$5-1))</f>
-        <v>12.875</v>
+        <v>14.375</v>
       </c>
       <c r="J7" s="11">
         <f>SUM('Sprint 2'!$B$3:$B$37)-(((J5-1)*SUM('Sprint 2'!$B$3:$B$37))/($J$5-1))</f>

</xml_diff>

<commit_message>
did some work, reported time
</commit_message>
<xml_diff>
--- a/PayBack - CEN3031 Scrum.xlsx
+++ b/PayBack - CEN3031 Scrum.xlsx
@@ -2558,21 +2558,7 @@
     <cellStyle name="40% - Accent5 2" xfId="10"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="130">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="128">
     <dxf>
       <fill>
         <patternFill>
@@ -3742,11 +3728,11 @@
             </a:ln>
           </c:spPr>
         </c:dropLines>
-        <c:axId val="58148736"/>
-        <c:axId val="58191872"/>
+        <c:axId val="117994240"/>
+        <c:axId val="117996160"/>
       </c:areaChart>
       <c:dateAx>
-        <c:axId val="58148736"/>
+        <c:axId val="117994240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3786,14 +3772,14 @@
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="low"/>
-        <c:crossAx val="58191872"/>
+        <c:crossAx val="117996160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="58191872"/>
+        <c:axId val="117996160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3837,7 +3823,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="58148736"/>
+        <c:crossAx val="117994240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3971,25 +3957,25 @@
                   <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>85</c:v>
+                  <c:v>83</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>85</c:v>
+                  <c:v>83</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>85</c:v>
+                  <c:v>83</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>85</c:v>
+                  <c:v>83</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>85</c:v>
+                  <c:v>83</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>85</c:v>
+                  <c:v>83</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>85</c:v>
+                  <c:v>83</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4113,11 +4099,11 @@
             </a:ln>
           </c:spPr>
         </c:dropLines>
-        <c:axId val="118627712"/>
-        <c:axId val="118763904"/>
+        <c:axId val="160887168"/>
+        <c:axId val="160889088"/>
       </c:areaChart>
       <c:dateAx>
-        <c:axId val="118627712"/>
+        <c:axId val="160887168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4157,14 +4143,14 @@
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="low"/>
-        <c:crossAx val="118763904"/>
+        <c:crossAx val="160889088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="118763904"/>
+        <c:axId val="160889088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4208,7 +4194,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="118627712"/>
+        <c:crossAx val="160887168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4985,11 +4971,11 @@
         </c:hiLowLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="59749888"/>
-        <c:axId val="59751808"/>
+        <c:axId val="155915008"/>
+        <c:axId val="155916928"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="59749888"/>
+        <c:axId val="155915008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5067,14 +5053,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="59751808"/>
+        <c:crossAx val="155916928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="59751808"/>
+        <c:axId val="155916928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5164,7 +5150,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="59749888"/>
+        <c:crossAx val="155915008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6247,8 +6233,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="82024704"/>
-        <c:axId val="82046976"/>
+        <c:axId val="155993600"/>
+        <c:axId val="155995136"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -6676,7 +6662,7 @@
         </c:extLst>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="82024704"/>
+        <c:axId val="155993600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6719,14 +6705,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82046976"/>
+        <c:crossAx val="155995136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="82046976"/>
+        <c:axId val="155995136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6777,7 +6763,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82024704"/>
+        <c:crossAx val="155993600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7122,11 +7108,11 @@
             </a:ln>
           </c:spPr>
         </c:dropLines>
-        <c:axId val="82350080"/>
-        <c:axId val="82358272"/>
+        <c:axId val="160479488"/>
+        <c:axId val="160481664"/>
       </c:areaChart>
       <c:dateAx>
-        <c:axId val="82350080"/>
+        <c:axId val="160479488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7166,14 +7152,14 @@
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="low"/>
-        <c:crossAx val="82358272"/>
+        <c:crossAx val="160481664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="82358272"/>
+        <c:axId val="160481664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7217,7 +7203,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82350080"/>
+        <c:crossAx val="160479488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7454,7 +7440,7 @@
                   <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>2</c:v>
@@ -7841,25 +7827,25 @@
                   <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>24</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>24</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>24</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>24</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>24</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>24</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7977,11 +7963,11 @@
         <c:dropLines/>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="86267392"/>
-        <c:axId val="86942848"/>
+        <c:axId val="160662656"/>
+        <c:axId val="160664576"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="86267392"/>
+        <c:axId val="160662656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8060,14 +8046,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="86942848"/>
+        <c:crossAx val="160664576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="86942848"/>
+        <c:axId val="160664576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8155,7 +8141,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="86267392"/>
+        <c:crossAx val="160662656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8970,25 +8956,25 @@
                   <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9203,11 +9189,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="87591552"/>
-        <c:axId val="88507136"/>
+        <c:axId val="160807168"/>
+        <c:axId val="160813056"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="87591552"/>
+        <c:axId val="160807168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9251,14 +9237,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="88507136"/>
+        <c:crossAx val="160813056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="88507136"/>
+        <c:axId val="160813056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9309,7 +9295,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="87591552"/>
+        <c:crossAx val="160807168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14721,332 +14707,332 @@
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <conditionalFormatting sqref="E19">
-    <cfRule type="cellIs" dxfId="129" priority="87" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="87" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23">
-    <cfRule type="cellIs" dxfId="128" priority="86" operator="equal">
+    <cfRule type="cellIs" dxfId="126" priority="86" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24">
-    <cfRule type="cellIs" dxfId="127" priority="85" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="85" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E25">
-    <cfRule type="cellIs" dxfId="126" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="124" priority="84" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E26">
-    <cfRule type="cellIs" dxfId="125" priority="83" operator="equal">
+    <cfRule type="cellIs" dxfId="123" priority="83" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E27">
-    <cfRule type="cellIs" dxfId="124" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="82" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E28">
-    <cfRule type="cellIs" dxfId="123" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="121" priority="81" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E50">
-    <cfRule type="cellIs" dxfId="122" priority="76" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="76" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E52">
-    <cfRule type="cellIs" dxfId="121" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="75" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E55">
-    <cfRule type="cellIs" dxfId="120" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="118" priority="74" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E63">
-    <cfRule type="cellIs" dxfId="119" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="71" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E81">
-    <cfRule type="cellIs" dxfId="118" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="69" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E82">
-    <cfRule type="cellIs" dxfId="117" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="68" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E32">
-    <cfRule type="cellIs" dxfId="116" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="65" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E37">
-    <cfRule type="cellIs" dxfId="115" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="63" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E46">
-    <cfRule type="cellIs" dxfId="114" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="61" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E51">
-    <cfRule type="cellIs" dxfId="113" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="111" priority="60" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E53">
-    <cfRule type="cellIs" dxfId="112" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="59" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E56">
-    <cfRule type="cellIs" dxfId="111" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="58" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E63">
-    <cfRule type="cellIs" dxfId="110" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="56" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E67">
-    <cfRule type="cellIs" dxfId="109" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="55" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E82">
-    <cfRule type="cellIs" dxfId="108" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="53" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E83">
-    <cfRule type="cellIs" dxfId="107" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="52" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E33">
-    <cfRule type="cellIs" dxfId="106" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="49" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E37">
-    <cfRule type="cellIs" dxfId="105" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="47" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E46">
-    <cfRule type="cellIs" dxfId="104" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="45" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E51">
-    <cfRule type="cellIs" dxfId="103" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="44" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E53">
-    <cfRule type="cellIs" dxfId="102" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="43" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E56">
-    <cfRule type="cellIs" dxfId="101" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="42" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E63">
-    <cfRule type="cellIs" dxfId="100" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="40" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E67">
-    <cfRule type="cellIs" dxfId="99" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="39" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E82">
-    <cfRule type="cellIs" dxfId="98" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="37" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E83">
-    <cfRule type="cellIs" dxfId="97" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="36" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E37">
-    <cfRule type="cellIs" dxfId="96" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="33" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E38">
-    <cfRule type="cellIs" dxfId="95" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="32" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E46">
-    <cfRule type="cellIs" dxfId="94" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="31" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E47">
-    <cfRule type="cellIs" dxfId="93" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="30" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E52">
-    <cfRule type="cellIs" dxfId="92" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="29" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E54">
-    <cfRule type="cellIs" dxfId="91" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="28" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E57">
-    <cfRule type="cellIs" dxfId="90" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="27" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E63">
-    <cfRule type="cellIs" dxfId="89" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="26" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E67">
-    <cfRule type="cellIs" dxfId="88" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="25" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E68">
-    <cfRule type="cellIs" dxfId="87" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="24" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E80">
-    <cfRule type="cellIs" dxfId="86" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="23" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E83">
-    <cfRule type="cellIs" dxfId="85" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="22" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E84">
-    <cfRule type="cellIs" dxfId="84" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="21" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E91">
-    <cfRule type="cellIs" dxfId="83" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="20" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E96">
-    <cfRule type="cellIs" dxfId="82" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="19" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E35">
-    <cfRule type="cellIs" dxfId="81" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="18" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E34">
-    <cfRule type="cellIs" dxfId="80" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="17" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E64">
-    <cfRule type="cellIs" dxfId="79" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="16" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E64">
-    <cfRule type="cellIs" dxfId="78" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="15" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E64">
-    <cfRule type="cellIs" dxfId="77" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="14" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E64">
-    <cfRule type="cellIs" dxfId="76" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="13" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E65">
-    <cfRule type="cellIs" dxfId="75" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="12" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E65">
-    <cfRule type="cellIs" dxfId="74" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="11" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E65">
-    <cfRule type="cellIs" dxfId="73" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="10" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E65">
-    <cfRule type="cellIs" dxfId="72" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="9" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E66">
-    <cfRule type="cellIs" dxfId="71" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="8" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E66">
-    <cfRule type="cellIs" dxfId="70" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="7" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E66">
-    <cfRule type="cellIs" dxfId="69" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="6" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E66">
-    <cfRule type="cellIs" dxfId="68" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="5" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E59">
-    <cfRule type="cellIs" dxfId="67" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="4" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E59">
-    <cfRule type="cellIs" dxfId="66" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="3" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E59">
-    <cfRule type="cellIs" dxfId="65" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="2" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E59">
-    <cfRule type="cellIs" dxfId="64" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="1" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19754,8 +19740,8 @@
   <dimension ref="A1:P63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q17" sqref="Q17"/>
+      <pane ySplit="2" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q42" sqref="Q42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -21539,25 +21525,25 @@
         <v>2</v>
       </c>
       <c r="J39" s="100">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K39" s="101">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L39" s="34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M39" s="100">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N39" s="101">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O39" s="34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P39" s="133">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -21677,25 +21663,25 @@
         <v>2</v>
       </c>
       <c r="J42" s="100">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K42" s="101">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L42" s="34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M42" s="100">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N42" s="101">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O42" s="34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P42" s="133">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -21951,31 +21937,31 @@
       </c>
       <c r="J50">
         <f t="shared" si="2"/>
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="K50">
         <f t="shared" si="2"/>
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="L50">
         <f t="shared" si="2"/>
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="M50">
         <f t="shared" si="2"/>
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="N50">
         <f t="shared" si="2"/>
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="O50">
         <f t="shared" si="2"/>
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="P50">
         <f t="shared" si="2"/>
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="51" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -22331,31 +22317,31 @@
       </c>
       <c r="J60">
         <f t="shared" si="10"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K60">
         <f t="shared" si="10"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="L60">
         <f t="shared" si="10"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="M60">
         <f t="shared" si="10"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="N60">
         <f t="shared" si="10"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="O60">
         <f t="shared" si="10"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="P60">
         <f t="shared" si="10"/>
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="61" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -22454,31 +22440,31 @@
       </c>
       <c r="J63">
         <f t="shared" si="13"/>
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="K63">
         <f t="shared" si="13"/>
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="L63">
         <f t="shared" si="13"/>
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M63">
         <f t="shared" si="13"/>
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="N63">
         <f t="shared" si="13"/>
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="O63">
         <f t="shared" si="13"/>
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="P63">
         <f t="shared" si="13"/>
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -22497,62 +22483,62 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E19">
-    <cfRule type="cellIs" dxfId="63" priority="115" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="115" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18">
-    <cfRule type="cellIs" dxfId="62" priority="114" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="114" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="cellIs" dxfId="61" priority="91" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="91" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="cellIs" dxfId="60" priority="112" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="112" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16">
-    <cfRule type="cellIs" dxfId="59" priority="111" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="111" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E38">
-    <cfRule type="cellIs" dxfId="58" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="60" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E44">
-    <cfRule type="cellIs" dxfId="57" priority="100" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="100" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21">
-    <cfRule type="cellIs" dxfId="56" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="57" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="cellIs" dxfId="55" priority="95" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="95" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="cellIs" dxfId="54" priority="96" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="96" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="cellIs" dxfId="53" priority="94" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="94" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="cellIs" dxfId="52" priority="93" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="93" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22638,77 +22624,77 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E33">
-    <cfRule type="cellIs" dxfId="51" priority="76" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="76" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E34">
-    <cfRule type="cellIs" dxfId="50" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="75" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E35">
-    <cfRule type="cellIs" dxfId="49" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="74" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E36">
-    <cfRule type="cellIs" dxfId="48" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="73" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E37">
-    <cfRule type="cellIs" dxfId="47" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="72" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E38">
-    <cfRule type="cellIs" dxfId="46" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="71" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E39">
-    <cfRule type="cellIs" dxfId="45" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="70" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E33">
-    <cfRule type="cellIs" dxfId="44" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="65" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E34">
-    <cfRule type="cellIs" dxfId="43" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="64" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E36">
-    <cfRule type="cellIs" dxfId="42" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="62" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E37">
-    <cfRule type="cellIs" dxfId="41" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="61" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E35">
-    <cfRule type="cellIs" dxfId="40" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="63" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E39">
-    <cfRule type="cellIs" dxfId="39" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="59" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E40">
-    <cfRule type="cellIs" dxfId="38" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="58" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="cellIs" dxfId="37" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="56" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22731,7 +22717,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule type="cellIs" dxfId="36" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="53" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22754,22 +22740,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="cellIs" dxfId="35" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="50" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24">
-    <cfRule type="cellIs" dxfId="34" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="49" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E41">
-    <cfRule type="cellIs" dxfId="33" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="48" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E42">
-    <cfRule type="cellIs" dxfId="32" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="47" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22792,7 +22778,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="cellIs" dxfId="31" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="43" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22815,7 +22801,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23">
-    <cfRule type="cellIs" dxfId="30" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="40" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23145,31 +23131,31 @@
       </c>
       <c r="D5" s="108">
         <f>SUM('Sprint 3'!J3:J45)</f>
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E5" s="139">
         <f>SUM('Sprint 3'!K3:K45)</f>
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F5" s="108">
         <f>SUM('Sprint 3'!L3:L45)</f>
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G5" s="108">
         <f>SUM('Sprint 3'!M3:M45)</f>
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H5" s="139">
         <f>SUM('Sprint 3'!N3:N45)</f>
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I5" s="108">
         <f>SUM('Sprint 3'!O3:O45)</f>
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J5" s="108">
         <f>SUM('Sprint 3'!P3:P45)</f>
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="K5" s="153"/>
     </row>

</xml_diff>